<commit_message>
logic interface art wish list
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -67,14 +67,40 @@
   </si>
   <si>
     <t>Tom</t>
+  </si>
+  <si>
+    <t>Level select to show picture of map as well as descriptions of map</t>
+  </si>
+  <si>
+    <t>Date Completed</t>
+  </si>
+  <si>
+    <t>online support for high scores</t>
+  </si>
+  <si>
+    <t>best time</t>
+  </si>
+  <si>
+    <t>shortest algorithm</t>
+  </si>
+  <si>
+    <t>best combination</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -91,13 +117,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -129,11 +155,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,104 +456,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" s="5" customFormat="1">
+      <c r="B1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" s="3" customFormat="1">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4">
+        <v>39881</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="3" customFormat="1">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:3" s="2" customFormat="1">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="3" customFormat="1">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" s="2" customFormat="1">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="3" customFormat="1">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" s="2" customFormat="1">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" s="2" customFormat="1">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="3" customFormat="1">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" s="2" customFormat="1">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="3" customFormat="1"/>
-    <row r="11" spans="1:2">
-      <c r="B11" s="1" t="s">
+    <row r="8" spans="1:3" s="2" customFormat="1"/>
+    <row r="11" spans="1:3" s="5" customFormat="1">
+      <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="3" customFormat="1">
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="1:3" s="2" customFormat="1">
+      <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="3" customFormat="1">
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="1:3" s="2" customFormat="1">
+      <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="3" customFormat="1">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:3" s="2" customFormat="1">
+      <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="3" customFormat="1">
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="1:3" s="2" customFormat="1">
+      <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="3" customFormat="1">
-      <c r="B16" s="3" t="s">
+    <row r="16" spans="1:3" s="2" customFormat="1">
+      <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="3" customFormat="1">
-      <c r="B17" s="3" t="s">
+    <row r="17" spans="3:4" s="2" customFormat="1">
+      <c r="C17" s="2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" s="2" customFormat="1">
+      <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" s="2" customFormat="1">
+      <c r="C19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" s="2" customFormat="1">
+      <c r="D20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" s="2" customFormat="1">
+      <c r="D21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" s="2" customFormat="1">
+      <c r="D22" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -538,7 +599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="A1:I12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
tutorial maps are balanced now wish list updated commands now have proper values for byte counts
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -85,6 +85,45 @@
   </si>
   <si>
     <t>best combination</t>
+  </si>
+  <si>
+    <t>bytes used by command in tooltip</t>
+  </si>
+  <si>
+    <t>slash switched/changed in bytes used line</t>
+  </si>
+  <si>
+    <t>if piece in hand cannot be dropped, place command here greys out</t>
+  </si>
+  <si>
+    <t>if piece in hand cannot be dropped due to byte limits, piece greys out</t>
+  </si>
+  <si>
+    <t>move forward until unable should only count as 1 command processed and not 1 for each square processed</t>
+  </si>
+  <si>
+    <t>view score state should show the level and level title/description of what you just beat</t>
+  </si>
+  <si>
+    <t>BUGS</t>
+  </si>
+  <si>
+    <t>on certain maps, keyboard control for panning does not work until after the mouse pans that direction first</t>
+  </si>
+  <si>
+    <t>command insertion</t>
+  </si>
+  <si>
+    <t>rotate map left/right</t>
+  </si>
+  <si>
+    <t>ice squares should only count as 1 command</t>
+  </si>
+  <si>
+    <t>you died state has some funkiness with abort/execute</t>
+  </si>
+  <si>
+    <t>maps need balancing</t>
   </si>
 </sst>
 </file>
@@ -108,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +163,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,13 +200,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -525,68 +572,142 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="2" customFormat="1"/>
-    <row r="11" spans="1:3" s="5" customFormat="1">
-      <c r="C11" s="5" t="s">
-        <v>1</v>
+    <row r="8" spans="1:3" s="2" customFormat="1">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="2" customFormat="1">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="2" customFormat="1">
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="2" customFormat="1">
+      <c r="C11" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="2" customFormat="1">
       <c r="C12" s="2" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="2" customFormat="1">
       <c r="C13" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="2" customFormat="1">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>6</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="7" customFormat="1">
+      <c r="C14" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="2" customFormat="1">
       <c r="C15" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="2" customFormat="1"/>
+    <row r="18" spans="1:4" s="5" customFormat="1">
+      <c r="C18" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="2" customFormat="1">
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="2" customFormat="1">
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="2" customFormat="1">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="2" customFormat="1">
+      <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1">
-      <c r="C16" s="2" t="s">
+    <row r="23" spans="1:4" s="2" customFormat="1">
+      <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:4" s="2" customFormat="1">
-      <c r="C17" s="2" t="s">
+    <row r="24" spans="1:4" s="2" customFormat="1">
+      <c r="C24" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="3:4" s="2" customFormat="1">
-      <c r="C18" s="2" t="s">
+    <row r="25" spans="1:4" s="2" customFormat="1">
+      <c r="C25" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="3:4" s="2" customFormat="1">
-      <c r="C19" s="2" t="s">
+    <row r="26" spans="1:4" s="2" customFormat="1">
+      <c r="C26" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="3:4" s="2" customFormat="1">
-      <c r="D20" s="2" t="s">
+    <row r="27" spans="1:4" s="2" customFormat="1">
+      <c r="D27" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="3:4" s="2" customFormat="1">
-      <c r="D21" s="2" t="s">
+    <row r="28" spans="1:4" s="2" customFormat="1">
+      <c r="D28" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="3:4" s="2" customFormat="1">
-      <c r="D22" s="2" t="s">
+    <row r="29" spans="1:4" s="2" customFormat="1">
+      <c r="D29" s="2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="2" customFormat="1">
+      <c r="C30" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="C31" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="C32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated start and end tiles with new art from cameron needs more cowbell, by cowbell i mean the green needs more green and red needs more red, in fact, the yellow needs more red updated wish  list
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -129,9 +129,6 @@
     <t>fix ice in subroutines</t>
   </si>
   <si>
-    <t>[</t>
-  </si>
-  <si>
     <t>tab artwork was added as well as implemented</t>
   </si>
   <si>
@@ -145,6 +142,24 @@
   </si>
   <si>
     <t>start new game does not check for an existing file properly</t>
+  </si>
+  <si>
+    <t>in-game pause menu with load/save/quit/return to main menu/save and quit/return to game</t>
+  </si>
+  <si>
+    <t>make it so you cannot resize the screen</t>
+  </si>
+  <si>
+    <t>level ideas</t>
+  </si>
+  <si>
+    <t>ability to disable/enable end square</t>
+  </si>
+  <si>
+    <t>bonus stages - short out levels where commands get randomized and other fun stuff</t>
+  </si>
+  <si>
+    <t>everything you know is wrong</t>
   </si>
 </sst>
 </file>
@@ -227,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -237,7 +252,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -650,11 +664,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:3" s="3" customFormat="1">
+      <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -670,18 +684,18 @@
     </row>
     <row r="16" spans="1:3" s="3" customFormat="1">
       <c r="A16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="4">
         <v>39881</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="2" customFormat="1">
       <c r="C17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="3" customFormat="1">
@@ -692,118 +706,152 @@
         <v>39881</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" ht="16.5" customHeight="1"/>
-    <row r="21" spans="1:4" s="5" customFormat="1">
-      <c r="C21" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="2" customFormat="1" ht="16.5" customHeight="1">
+      <c r="C19" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="2" customFormat="1">
+      <c r="C20" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="2" customFormat="1"/>
+    <row r="22" spans="1:4" s="2" customFormat="1"/>
+    <row r="23" spans="1:4" s="5" customFormat="1">
+      <c r="C23" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="2" customFormat="1">
-      <c r="C22" s="2" t="s">
+    <row r="24" spans="1:4" s="2" customFormat="1">
+      <c r="C24" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="2" customFormat="1">
-      <c r="C23" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="2" customFormat="1">
-      <c r="A24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="2" customFormat="1">
       <c r="C25" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="2" customFormat="1">
+      <c r="A26" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C26" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="2" customFormat="1">
       <c r="C27" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="2" customFormat="1">
       <c r="C28" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="2" customFormat="1">
       <c r="C29" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="2" customFormat="1">
+      <c r="C30" s="2" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="2" customFormat="1">
-      <c r="D30" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="2" customFormat="1">
       <c r="D31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="2" customFormat="1">
       <c r="D32" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="2" customFormat="1">
+      <c r="D33" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1">
-      <c r="C33" s="2" t="s">
+    <row r="34" spans="1:4" s="2" customFormat="1">
+      <c r="C34" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1">
-      <c r="C34" s="2" t="s">
+    <row r="35" spans="1:4" s="2" customFormat="1">
+      <c r="C35" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1">
-      <c r="C35" s="2" t="s">
+    <row r="36" spans="1:4" s="2" customFormat="1">
+      <c r="C36" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="C36" s="6"/>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="B37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="5" t="s">
+    <row r="37" spans="1:4">
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="C38" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1">
-      <c r="C38" s="2" t="s">
+    <row r="39" spans="1:4" s="2" customFormat="1">
+      <c r="C39" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:4" s="3" customFormat="1">
+      <c r="A40" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B40" s="4">
         <v>39881</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C40" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="C40" s="1" t="s">
-        <v>42</v>
+    <row r="41" spans="1:4" s="3" customFormat="1">
+      <c r="A41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="4">
+        <v>39882</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="2" customFormat="1">
+      <c r="C42" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="C45" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="C46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="C47" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="C48" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added PRELIMINARY sound support for the oal framework, the shit still doesn't work right even letting it pause the damn game, but whatever updated robot art to include cameron's new robot graphic, since two directions were missing, i just mirrored it for now added oal framework files and whatnot to project under folder OpenALSound added a bunch of wav files that we can mess around with if we do decide to somehow get sound working, someone should work on sound at some point the samples for playstatic and playstream from the open al sdk are now converted to 2008, those are what we will need to use if we do ever want to add sound.. playstatic would be like we had badly implemented before where it pauses the game while playing, playstream is a little more complex but allows streaming audio to play while the game is being processed i think
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>everything you know is wrong</t>
+  </si>
+  <si>
+    <t>Menus need to at the very least use better temp art</t>
+  </si>
+  <si>
+    <t>Level Designers</t>
   </si>
 </sst>
 </file>
@@ -546,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -678,6 +684,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" s="2" customFormat="1">
+      <c r="A15" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="C15" s="2" t="s">
         <v>35</v>
       </c>
@@ -719,138 +728,143 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="2" customFormat="1"/>
+    <row r="21" spans="1:4" s="2" customFormat="1">
+      <c r="C21" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="22" spans="1:4" s="2" customFormat="1"/>
-    <row r="23" spans="1:4" s="5" customFormat="1">
-      <c r="C23" s="5" t="s">
+    <row r="23" spans="1:4" s="2" customFormat="1"/>
+    <row r="24" spans="1:4" s="5" customFormat="1">
+      <c r="C24" s="5" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="2" customFormat="1">
-      <c r="C24" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="2" customFormat="1">
       <c r="C25" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="2" customFormat="1">
+      <c r="C26" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="2" customFormat="1">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:4" s="2" customFormat="1">
+      <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="2" customFormat="1">
-      <c r="C27" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="2" customFormat="1">
       <c r="C28" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="2" customFormat="1">
       <c r="C29" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="2" customFormat="1">
       <c r="C30" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="2" customFormat="1">
+      <c r="C31" s="2" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="2" customFormat="1">
-      <c r="D31" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="2" customFormat="1">
       <c r="D32" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="2" customFormat="1">
       <c r="D33" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="2" customFormat="1">
+      <c r="D34" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="2" customFormat="1">
-      <c r="C34" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="2" customFormat="1">
       <c r="C35" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="2" customFormat="1">
       <c r="C36" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="2" customFormat="1">
+      <c r="C37" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="C37" s="6"/>
-    </row>
     <row r="38" spans="1:4">
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="C39" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="2" customFormat="1">
-      <c r="C39" s="2" t="s">
+    <row r="40" spans="1:4" s="2" customFormat="1">
+      <c r="C40" s="2" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="3" customFormat="1">
-      <c r="A40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="3" customFormat="1">
       <c r="A41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="4">
+        <v>39881</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="3" customFormat="1">
+      <c r="A42" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B42" s="4">
         <v>39882</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="2" customFormat="1">
-      <c r="C42" s="2" t="s">
+    <row r="43" spans="1:4" s="2" customFormat="1">
+      <c r="C43" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="C45" s="5" t="s">
+    <row r="46" spans="1:4">
+      <c r="C46" s="5" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="C46" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="C47" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="C48" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
total commands processed clears properly between levels now added tile tutorial 1 revisit, with subroutines required now to complete the level
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Level Designers</t>
+  </si>
+  <si>
+    <t>subs calling subs may not be working right still, not 100% sure</t>
+  </si>
+  <si>
+    <t>game saves the level you're on and not the highest level you can select</t>
   </si>
 </sst>
 </file>
@@ -552,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -848,23 +854,36 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="C46" s="5" t="s">
+    <row r="44" spans="1:4" s="2" customFormat="1">
+      <c r="C44" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="2" customFormat="1">
+      <c r="A45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="C47" s="5" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="C47" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="C48" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="3:3">
       <c r="C49" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
menu system graphic overhaul in the theme of cameron's art "It's about damn time"
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -172,6 +172,15 @@
   </si>
   <si>
     <t>game saves the level you're on and not the highest level you can select</t>
+  </si>
+  <si>
+    <t>Credits needs to be implemented</t>
+  </si>
+  <si>
+    <t>activate needs more descriptive tooltips</t>
+  </si>
+  <si>
+    <t>bytes used during game needs a black semi-transparent backdrop</t>
   </si>
 </sst>
 </file>
@@ -558,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -595,11 +604,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:3" s="3" customFormat="1">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="4">
+        <v>39883</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -628,41 +640,35 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="2" customFormat="1">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="3" customFormat="1">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:3" s="3" customFormat="1">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="4">
         <v>39881</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="7" customFormat="1">
-      <c r="A10" s="7" t="s">
+    <row r="11" spans="1:3" s="7" customFormat="1">
+      <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="3" customFormat="1">
-      <c r="A11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="3" customFormat="1">
@@ -673,217 +679,237 @@
         <v>39881</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B13" s="4">
+        <v>39881</v>
+      </c>
       <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="3" customFormat="1">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="8" customFormat="1">
-      <c r="C14" s="8" t="s">
+    <row r="15" spans="1:3" s="8" customFormat="1">
+      <c r="C15" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:3" s="2" customFormat="1">
+      <c r="A16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="3" customFormat="1">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:3" s="3" customFormat="1">
+      <c r="A17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B17" s="4">
         <v>39881</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="2" customFormat="1">
-      <c r="C17" s="2" t="s">
+    <row r="18" spans="1:3" s="2" customFormat="1">
+      <c r="C18" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="3" customFormat="1">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:3" s="3" customFormat="1">
+      <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B19" s="4">
         <v>39881</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" ht="16.5" customHeight="1">
-      <c r="C19" s="2" t="s">
+    <row r="20" spans="1:3" s="2" customFormat="1" ht="16.5" customHeight="1">
+      <c r="C20" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="2" customFormat="1">
-      <c r="C20" s="2" t="s">
+    <row r="21" spans="1:3" s="2" customFormat="1">
+      <c r="C21" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="2" customFormat="1">
-      <c r="C21" s="2" t="s">
+    <row r="22" spans="1:3" s="2" customFormat="1">
+      <c r="C22" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="2" customFormat="1"/>
-    <row r="23" spans="1:4" s="2" customFormat="1"/>
-    <row r="24" spans="1:4" s="5" customFormat="1">
-      <c r="C24" s="5" t="s">
+    <row r="23" spans="1:3" s="2" customFormat="1">
+      <c r="C23" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="2" customFormat="1">
+      <c r="C24" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="2" customFormat="1"/>
+    <row r="26" spans="1:3" s="5" customFormat="1">
+      <c r="C26" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="2" customFormat="1">
-      <c r="C25" s="2" t="s">
+    <row r="27" spans="1:3" s="2" customFormat="1">
+      <c r="C27" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="2" customFormat="1">
-      <c r="C26" s="2" t="s">
+    <row r="28" spans="1:3" s="2" customFormat="1">
+      <c r="C28" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="2" customFormat="1">
-      <c r="A27" s="2" t="s">
+    <row r="29" spans="1:3" s="2" customFormat="1">
+      <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="2" customFormat="1">
-      <c r="C28" s="2" t="s">
+    <row r="30" spans="1:3" s="2" customFormat="1">
+      <c r="C30" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="2" customFormat="1">
-      <c r="C29" s="2" t="s">
+    <row r="31" spans="1:3" s="2" customFormat="1">
+      <c r="C31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="2" customFormat="1">
-      <c r="C30" s="2" t="s">
+    <row r="32" spans="1:3" s="2" customFormat="1">
+      <c r="C32" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="2" customFormat="1">
-      <c r="C31" s="2" t="s">
+    <row r="33" spans="1:4" s="2" customFormat="1">
+      <c r="C33" s="2" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="2" customFormat="1">
-      <c r="D32" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="2" customFormat="1">
-      <c r="D33" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="2" customFormat="1">
       <c r="D34" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="2" customFormat="1">
+      <c r="D35" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="2" customFormat="1">
+      <c r="D36" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="2" customFormat="1">
-      <c r="C35" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="2" customFormat="1">
-      <c r="C36" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="2" customFormat="1">
       <c r="C37" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="2" customFormat="1">
+      <c r="C38" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="2" customFormat="1">
+      <c r="C39" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="C38" s="6"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="C39" s="5" t="s">
+    <row r="40" spans="1:4">
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="C41" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="2" customFormat="1">
-      <c r="C40" s="2" t="s">
+    <row r="42" spans="1:4" s="2" customFormat="1">
+      <c r="C42" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="3" customFormat="1">
-      <c r="A41" s="3" t="s">
+    <row r="43" spans="1:4" s="3" customFormat="1">
+      <c r="A43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B43" s="4">
         <v>39881</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="3" customFormat="1">
-      <c r="A42" s="3" t="s">
+    <row r="44" spans="1:4" s="3" customFormat="1">
+      <c r="A44" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B44" s="4">
         <v>39882</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="2" customFormat="1">
-      <c r="C43" s="2" t="s">
+    <row r="45" spans="1:4" s="2" customFormat="1">
+      <c r="C45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:4" s="2" customFormat="1">
-      <c r="C44" s="2" t="s">
+    <row r="46" spans="1:4" s="2" customFormat="1">
+      <c r="C46" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="2" customFormat="1">
-      <c r="A45" s="2" t="s">
+    <row r="47" spans="1:4" s="2" customFormat="1">
+      <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="C47" s="5" t="s">
+    <row r="49" spans="3:3">
+      <c r="C49" s="5" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="C48" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3">
-      <c r="C49" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="50" spans="3:3">
       <c r="C50" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3">
+      <c r="C52" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Insertion and Deletion to LogicInterface COMPLETE (finally, sorry guys).
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="16215" windowHeight="10200" tabRatio="499"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -741,8 +741,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" ht="16.5" customHeight="1">
-      <c r="C20" s="2" t="s">
+    <row r="20" spans="1:3" s="3" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4">
+        <v>39883</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
map screenshots added fixed all states i think that have menus and text to look a lot better breakable tiles are now semi-transparent so we can see what's behind them level select is far more detailed now for information gamevars now has a vector that matches the levelist called levelart for screenshots
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="16215" windowHeight="10200" tabRatio="499"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>bytes used during game needs a black semi-transparent backdrop</t>
+  </si>
+  <si>
+    <t>Menu art should all be cleaned up now</t>
   </si>
 </sst>
 </file>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -615,71 +618,86 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:3" s="3" customFormat="1">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="2" customFormat="1">
-      <c r="A6" s="2" t="s">
+      <c r="B5" s="4">
+        <v>39881</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="7" customFormat="1">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="2" customFormat="1">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="2" customFormat="1">
-      <c r="C8" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="2" customFormat="1">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
+      <c r="C6" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="3" customFormat="1">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>39881</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="3" customFormat="1">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4">
+        <v>39881</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="3" customFormat="1">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4">
         <v>39881</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="7" customFormat="1">
-      <c r="A11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="3" customFormat="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="3" customFormat="1">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>39881</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="3" customFormat="1" ht="16.5" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B12" s="4">
-        <v>39881</v>
+        <v>39883</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="3" customFormat="1">
@@ -687,18 +705,21 @@
         <v>10</v>
       </c>
       <c r="B13" s="4">
-        <v>39881</v>
+        <v>39883</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="3" customFormat="1">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B14" s="4">
+        <v>39883</v>
+      </c>
       <c r="C14" s="3" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="8" customFormat="1">
@@ -714,208 +735,207 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="3" customFormat="1">
-      <c r="A17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>37</v>
+    <row r="17" spans="1:3" s="2" customFormat="1">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="2" customFormat="1">
+      <c r="A18" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C18" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="3" customFormat="1">
-      <c r="A19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="3" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A20" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="2" customFormat="1">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="4">
-        <v>39883</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>42</v>
+      <c r="C19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="2" customFormat="1">
+      <c r="C20" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="2" customFormat="1">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C21" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="2" customFormat="1">
       <c r="C22" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="2" customFormat="1">
       <c r="C23" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="2" customFormat="1">
       <c r="C24" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="2" customFormat="1">
+      <c r="C25" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="2" customFormat="1"/>
-    <row r="26" spans="1:3" s="5" customFormat="1">
-      <c r="C26" s="5" t="s">
+    <row r="26" spans="1:3" s="2" customFormat="1"/>
+    <row r="27" spans="1:3" s="5" customFormat="1">
+      <c r="C27" s="5" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="2" customFormat="1">
-      <c r="C27" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="2" customFormat="1">
       <c r="C28" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="2" customFormat="1">
+      <c r="C29" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="2" customFormat="1">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:3" s="2" customFormat="1">
+      <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="2" customFormat="1">
-      <c r="C30" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="2" customFormat="1">
       <c r="C31" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="2" customFormat="1">
       <c r="C32" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="2" customFormat="1">
       <c r="C33" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="2" customFormat="1">
+      <c r="C34" s="2" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="2" customFormat="1">
-      <c r="D34" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="2" customFormat="1">
       <c r="D35" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="2" customFormat="1">
       <c r="D36" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="2" customFormat="1">
+      <c r="D37" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="2" customFormat="1">
-      <c r="C37" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="2" customFormat="1">
       <c r="C38" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="2" customFormat="1">
       <c r="C39" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="2" customFormat="1">
+      <c r="C40" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="C40" s="6"/>
-    </row>
     <row r="41" spans="1:4">
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="C42" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="2" customFormat="1">
-      <c r="C42" s="2" t="s">
+    <row r="43" spans="1:4" s="2" customFormat="1">
+      <c r="C43" s="2" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="3" customFormat="1">
-      <c r="A43" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="3" customFormat="1">
       <c r="A44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="4">
+        <v>39881</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="3" customFormat="1">
+      <c r="A45" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B45" s="4">
         <v>39882</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="2" customFormat="1">
-      <c r="C45" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="2" customFormat="1">
       <c r="C46" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="2" customFormat="1">
+      <c r="C47" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="2" customFormat="1">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:4" s="2" customFormat="1">
+      <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="3:3">
-      <c r="C49" s="5" t="s">
+    <row r="50" spans="3:3">
+      <c r="C50" s="5" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3">
-      <c r="C50" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="51" spans="3:3">
       <c r="C51" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="3:3">
       <c r="C52" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3">
+      <c r="C53" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
our game is now known as stupid robot updated logo artwork youdied uses a png instead of text clearcolor has been moved to gamestate so that we can set all clearcolors to whatever we want whenever we want wishlish updated start/end tiles are more green and red respectively so yeah
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>"did you know" info for pregame screen</t>
+  </si>
+  <si>
+    <t>devlogofades broke again, fixed now</t>
+  </si>
+  <si>
+    <t>pause menu esc should fire a return to game</t>
   </si>
 </sst>
 </file>
@@ -607,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P70"/>
+  <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -853,105 +859,90 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="2" customFormat="1"/>
-    <row r="27" spans="1:3" s="5" customFormat="1">
-      <c r="C27" s="5" t="s">
+    <row r="26" spans="1:3" s="2" customFormat="1">
+      <c r="C26" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="2" customFormat="1"/>
+    <row r="28" spans="1:3" s="5" customFormat="1">
+      <c r="C28" s="5" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="2" customFormat="1">
-      <c r="C28" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="2" customFormat="1">
       <c r="C29" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="2" customFormat="1">
+      <c r="C30" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="2" customFormat="1">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:3" s="2" customFormat="1">
+      <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="2" customFormat="1">
-      <c r="C31" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="2" customFormat="1">
       <c r="C32" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="2" customFormat="1">
       <c r="C33" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="2" customFormat="1">
       <c r="C34" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" s="2" customFormat="1">
+      <c r="C35" s="2" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" s="2" customFormat="1">
-      <c r="D35" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:16" s="2" customFormat="1">
       <c r="D36" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:16" s="2" customFormat="1">
       <c r="D37" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" s="2" customFormat="1">
+      <c r="D38" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" s="2" customFormat="1">
-      <c r="C38" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:16" s="2" customFormat="1">
       <c r="C39" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:16" s="2" customFormat="1">
       <c r="C40" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" s="2" customFormat="1">
+      <c r="C41" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:16">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -968,182 +959,192 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16">
-      <c r="C43" s="5" t="s">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="C44" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="2" customFormat="1">
-      <c r="C44" s="2" t="s">
+    <row r="45" spans="1:16" s="2" customFormat="1">
+      <c r="C45" s="2" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" s="3" customFormat="1">
-      <c r="A45" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:16" s="3" customFormat="1">
       <c r="A46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="4">
+        <v>39881</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" s="3" customFormat="1">
+      <c r="A47" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B47" s="4">
         <v>39882</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="2" customFormat="1">
-      <c r="C47" s="2" t="s">
+    <row r="48" spans="1:16" s="3" customFormat="1">
+      <c r="A48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="2" customFormat="1">
-      <c r="C48" s="2" t="s">
+    <row r="49" spans="1:3" s="2" customFormat="1">
+      <c r="C49" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="2" customFormat="1">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:3" s="2" customFormat="1">
+      <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="2" customFormat="1">
-      <c r="C50" s="2" t="s">
+    <row r="51" spans="1:3" s="2" customFormat="1">
+      <c r="C51" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2" t="s">
+    <row r="52" spans="1:3" s="3" customFormat="1">
+      <c r="A52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
-      <c r="P51" s="2"/>
-    </row>
-    <row r="52" spans="1:16">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2" t="s">
+    </row>
+    <row r="53" spans="1:3" s="3" customFormat="1">
+      <c r="A53" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
-    </row>
-    <row r="53" spans="1:16">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2" t="s">
+    </row>
+    <row r="54" spans="1:3" s="3" customFormat="1">
+      <c r="A54" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
-    </row>
-    <row r="56" spans="1:16">
-      <c r="C56" s="5" t="s">
+    </row>
+    <row r="55" spans="1:3" s="3" customFormat="1">
+      <c r="A55" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="C58" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
-      <c r="C57" s="1" t="s">
+    <row r="59" spans="1:3">
+      <c r="C59" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
-      <c r="C58" s="1" t="s">
+    <row r="60" spans="1:3">
+      <c r="C60" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
-      <c r="C59" s="1" t="s">
+    <row r="61" spans="1:3">
+      <c r="C61" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
-      <c r="C62" s="5" t="s">
+    <row r="64" spans="1:3">
+      <c r="C64" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
-      <c r="C63" s="1" t="s">
+    <row r="65" spans="3:4">
+      <c r="C65" s="1" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16">
-      <c r="C64" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="65" spans="3:4">
-      <c r="D65" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="3:4">
-      <c r="C67" s="1" t="s">
-        <v>60</v>
+      <c r="D67" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4">
+      <c r="C71" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4">
+      <c r="C72" s="1" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
preliminary to get reid of keyboard input for navigation and replacing with onscreen "compass" for some damned reason the click handlers aren't working and I have no idea why, but its there visually for the time being even though it doesn't function at all
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -237,7 +237,7 @@
     <t>pause menu esc should fire a return to game</t>
   </si>
   <si>
-    <t>a</t>
+    <t>compass click handlers aren't working and I have no idea why - dave</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
   <dimension ref="A1:P72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added verification of map positions so that the compass, keyboard and mouse won't scroll "too far" causing scrolling to really scroll too far added a default white image to gamestates to use as a background added a background image for bytes left and changes the text to black added clearer tooltips for all logic blocks when you die, it now resets the logic interface to the aborted States/LevelSelectState.cpp switched the execute/abort/clear/reset buttons to use their proper hover artwork level select state now has a white background for when it is used mid-GameObjectManager pause game state now accepts esc to exit the state updated excel sheet
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="75">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -219,9 +219,6 @@
     <t>add mouse controlled interface for panning/zooming to elmininate keyboard input</t>
   </si>
   <si>
-    <t>subs calling subs may not be working right still, not 100% sure - last command of 2nd sub called processes an extra time</t>
-  </si>
-  <si>
     <t>add more descriptive tooltips</t>
   </si>
   <si>
@@ -237,7 +234,13 @@
     <t>pause menu esc should fire a return to game</t>
   </si>
   <si>
-    <t>compass click handlers aren't working and I have no idea why - dave</t>
+    <t>because level select can pop up during ingame, it needs a white background</t>
+  </si>
+  <si>
+    <t>compass click handlers aren't working and I have no idea why - fixed</t>
+  </si>
+  <si>
+    <t>subs calling subs may not be working right still, not 100% sure - last command of 2nd sub called may process an extra time</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,12 +280,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,14 +311,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -818,8 +816,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="6" customFormat="1">
-      <c r="C19" s="6" t="s">
+    <row r="19" spans="1:3" s="3" customFormat="1">
+      <c r="A19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="4">
+        <v>39888</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -854,207 +858,208 @@
     </row>
     <row r="24" spans="1:3" s="2" customFormat="1">
       <c r="C24" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="2" customFormat="1">
       <c r="C25" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="2" customFormat="1">
-      <c r="C26" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="3" customFormat="1">
+      <c r="A26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="4">
+        <v>39888</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="3" customFormat="1">
+      <c r="A27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="4">
+        <v>39888</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="3" customFormat="1">
+      <c r="A28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="4">
+        <v>39888</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="2" customFormat="1">
-      <c r="C27" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="5" customFormat="1">
-      <c r="C28" s="5" t="s">
+    <row r="29" spans="1:3" s="6" customFormat="1">
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:3" s="6" customFormat="1">
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" s="6" customFormat="1">
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" s="6" customFormat="1">
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:16" s="5" customFormat="1">
+      <c r="C33" s="5" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" s="2" customFormat="1">
-      <c r="C29" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="2" customFormat="1">
-      <c r="C30" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="2" customFormat="1">
-      <c r="A31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="2" customFormat="1">
-      <c r="C32" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" s="2" customFormat="1">
-      <c r="C33" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="2" customFormat="1">
       <c r="C34" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="2" customFormat="1">
       <c r="C35" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:16" s="2" customFormat="1">
-      <c r="D36" s="2" t="s">
-        <v>19</v>
+      <c r="A36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:16" s="2" customFormat="1">
-      <c r="D37" s="2" t="s">
-        <v>20</v>
+      <c r="C37" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:16" s="2" customFormat="1">
-      <c r="D38" s="2" t="s">
-        <v>21</v>
+      <c r="C38" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:16" s="2" customFormat="1">
       <c r="C39" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:16" s="2" customFormat="1">
       <c r="C40" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:16" s="2" customFormat="1">
-      <c r="C41" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-    </row>
-    <row r="43" spans="1:16">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-    </row>
-    <row r="44" spans="1:16">
-      <c r="C44" s="5" t="s">
-        <v>28</v>
+      <c r="D41" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" s="2" customFormat="1">
+      <c r="D42" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" s="2" customFormat="1">
+      <c r="D43" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" s="2" customFormat="1">
+      <c r="C44" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:16" s="2" customFormat="1">
       <c r="C45" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" s="2" customFormat="1">
+      <c r="C46" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="C49" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="3" customFormat="1">
+      <c r="A50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="4">
+        <v>39888</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="3" customFormat="1">
-      <c r="A46" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" s="4">
+    <row r="51" spans="1:3" s="3" customFormat="1">
+      <c r="A51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="4">
         <v>39881</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" s="3" customFormat="1">
-      <c r="A47" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" s="4">
-        <v>39882</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" s="3" customFormat="1">
-      <c r="A48" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B48" s="4">
-        <v>39887</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="2" customFormat="1">
-      <c r="C49" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" s="2" customFormat="1">
-      <c r="A50" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" s="2" customFormat="1">
-      <c r="C51" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="3" customFormat="1">
       <c r="A52" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B52" s="4">
-        <v>39887</v>
+        <v>39882</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="3" customFormat="1">
@@ -1065,93 +1070,133 @@
         <v>39887</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="2" customFormat="1">
+      <c r="C54" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" s="2" customFormat="1">
+      <c r="A55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="2" customFormat="1">
+      <c r="C56" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="3" customFormat="1">
+      <c r="A57" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="3" customFormat="1">
+      <c r="A58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="3" customFormat="1">
-      <c r="A54" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="4">
+    <row r="59" spans="1:3" s="3" customFormat="1">
+      <c r="A59" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" s="4">
         <v>39887</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="3" customFormat="1">
-      <c r="A55" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B55" s="4">
+    <row r="60" spans="1:3" s="3" customFormat="1">
+      <c r="A60" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="4">
         <v>39887</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="C58" s="5" t="s">
+      <c r="C60" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="C63" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="C59" s="1" t="s">
+    <row r="64" spans="1:3">
+      <c r="C64" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="C60" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="C61" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="C64" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="67" spans="3:4">
-      <c r="D67" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="68" spans="3:4">
-      <c r="C68" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="3:4">
-      <c r="C69" s="1" t="s">
-        <v>60</v>
+      <c r="C69" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4">
+      <c r="D72" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4">
+      <c r="C73" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4">
+      <c r="C74" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4">
+      <c r="C75" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4">
+      <c r="C76" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="3:4">
-      <c r="C72" s="1" t="s">
+    <row r="77" spans="3:4">
+      <c r="C77" s="1" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
wish list updated 350 biatch
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>Condense the filesize of the content folder</t>
+  </si>
+  <si>
+    <t>load game needs to go to the select profile state</t>
   </si>
 </sst>
 </file>
@@ -317,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -326,6 +329,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -652,11 +656,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" s="3" customFormat="1">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="4">
+        <v>39892</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -838,53 +845,51 @@
     </row>
     <row r="20" spans="1:3" s="2" customFormat="1">
       <c r="A20" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B20" s="8"/>
       <c r="C20" s="2" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="2" customFormat="1">
       <c r="A21" s="2" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="2" customFormat="1">
       <c r="A22" s="2" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="2" customFormat="1">
       <c r="A23" s="2" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="2" customFormat="1">
       <c r="A24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="2" customFormat="1">
+      <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" s="3" customFormat="1">
-      <c r="A25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="4">
-        <v>39888</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="3" customFormat="1">
@@ -895,7 +900,7 @@
         <v>39888</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="3" customFormat="1">
@@ -906,7 +911,7 @@
         <v>39888</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="3" customFormat="1">
@@ -914,14 +919,22 @@
         <v>10</v>
       </c>
       <c r="B28" s="4">
+        <v>39888</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="3" customFormat="1">
+      <c r="A29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="4">
         <v>39889</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" s="6" customFormat="1">
-      <c r="B29" s="7"/>
     </row>
     <row r="30" spans="1:3" s="6" customFormat="1">
       <c r="B30" s="7"/>
@@ -929,116 +942,101 @@
     <row r="31" spans="1:3" s="6" customFormat="1">
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="1:3" s="5" customFormat="1">
-      <c r="C32" s="5" t="s">
+    <row r="32" spans="1:3" s="6" customFormat="1">
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" s="5" customFormat="1">
+      <c r="C33" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="2" customFormat="1">
-      <c r="C33" s="2" t="s">
+    <row r="34" spans="1:4" s="2" customFormat="1">
+      <c r="C34" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="2" customFormat="1">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:4" s="2" customFormat="1">
+      <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="2" customFormat="1">
-      <c r="C35" s="2" t="s">
+    <row r="36" spans="1:4" s="2" customFormat="1">
+      <c r="C36" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="2" customFormat="1">
-      <c r="C36" s="2" t="s">
+    <row r="37" spans="1:4" s="2" customFormat="1">
+      <c r="C37" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="2" customFormat="1">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:4" s="2" customFormat="1">
+      <c r="A38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="2" customFormat="1">
-      <c r="C38" s="2" t="s">
+    <row r="39" spans="1:4" s="2" customFormat="1">
+      <c r="C39" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="2" customFormat="1">
-      <c r="C39" s="2" t="s">
+    <row r="40" spans="1:4" s="2" customFormat="1">
+      <c r="C40" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="2" customFormat="1">
-      <c r="C40" s="2" t="s">
+    <row r="41" spans="1:4" s="2" customFormat="1">
+      <c r="C41" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="2" customFormat="1">
-      <c r="C41" s="2" t="s">
+    <row r="42" spans="1:4" s="2" customFormat="1">
+      <c r="C42" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="2" customFormat="1">
-      <c r="D42" s="2" t="s">
+    <row r="43" spans="1:4" s="2" customFormat="1">
+      <c r="D43" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="2" customFormat="1">
-      <c r="D43" s="2" t="s">
+    <row r="44" spans="1:4" s="2" customFormat="1">
+      <c r="D44" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="2" customFormat="1">
-      <c r="D44" s="2" t="s">
+    <row r="45" spans="1:4" s="2" customFormat="1">
+      <c r="D45" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="2" customFormat="1">
-      <c r="C45" s="2" t="s">
+    <row r="46" spans="1:4" s="2" customFormat="1">
+      <c r="C46" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="2" customFormat="1">
-      <c r="C46" s="2" t="s">
+    <row r="47" spans="1:4" s="2" customFormat="1">
+      <c r="C47" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="2" customFormat="1">
-      <c r="C47" s="2" t="s">
+    <row r="48" spans="1:4" s="2" customFormat="1">
+      <c r="C48" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="48" spans="1:16">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
     </row>
     <row r="49" spans="1:16">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="C49" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -1053,20 +1051,27 @@
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
     </row>
-    <row r="51" spans="1:16">
-      <c r="C51" s="5" t="s">
+    <row r="50" spans="1:16">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="C52" s="5" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" s="3" customFormat="1">
-      <c r="A52" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B52" s="4">
-        <v>39888</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:16" s="3" customFormat="1">
@@ -1074,61 +1079,61 @@
         <v>10</v>
       </c>
       <c r="B53" s="4">
-        <v>39881</v>
+        <v>39888</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:16" s="3" customFormat="1">
       <c r="A54" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B54" s="4">
-        <v>39882</v>
+        <v>39881</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:16" s="3" customFormat="1">
       <c r="A55" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B55" s="4">
+        <v>39882</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" s="3" customFormat="1">
+      <c r="A56" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="4">
         <v>39887</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="2" customFormat="1">
-      <c r="C56" s="2" t="s">
+    <row r="57" spans="1:16" s="2" customFormat="1">
+      <c r="C57" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="2" customFormat="1">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:16" s="2" customFormat="1">
+      <c r="A58" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="2" customFormat="1">
-      <c r="C58" s="2" t="s">
+    <row r="59" spans="1:16" s="2" customFormat="1">
+      <c r="C59" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" s="3" customFormat="1">
-      <c r="A59" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B59" s="4">
-        <v>39887</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:16" s="3" customFormat="1">
@@ -1139,7 +1144,7 @@
         <v>39887</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:16" s="3" customFormat="1">
@@ -1150,7 +1155,7 @@
         <v>39887</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:16" s="3" customFormat="1">
@@ -1161,71 +1166,82 @@
         <v>39887</v>
       </c>
       <c r="C62" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" s="3" customFormat="1">
+      <c r="A63" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="3:4">
-      <c r="C65" s="5" t="s">
+    <row r="66" spans="3:4">
+      <c r="C66" s="5" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="66" spans="3:4">
-      <c r="C66" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4">
+      <c r="C69" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="3:4">
-      <c r="C71" s="5" t="s">
+    <row r="72" spans="3:4">
+      <c r="C72" s="5" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="72" spans="3:4">
-      <c r="C72" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4">
+      <c r="C74" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="3:4">
-      <c r="D74" s="1" t="s">
+    <row r="75" spans="3:4">
+      <c r="D75" s="1" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="75" spans="3:4">
-      <c r="C75" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="80" spans="3:4">
+      <c r="C80" s="1" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor map updates wish list update
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="16215" windowHeight="10200" tabRatio="499"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="11040" windowHeight="6930" tabRatio="499"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="89">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -171,9 +171,6 @@
     <t>bytes used during game needs a black semi-transparent backdrop</t>
   </si>
   <si>
-    <t>map centering issues occasionally</t>
-  </si>
-  <si>
     <t>Color of start and end squares need to stand out more</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t xml:space="preserve">The hole tile isn't clear that it’s a hole in the floor. </t>
   </si>
   <si>
-    <t>Raised tiles need to be shorter to improve visibility of the map</t>
-  </si>
-  <si>
     <t>Jump needs a new icon</t>
   </si>
   <si>
@@ -234,9 +228,6 @@
     <t>subs calling subs may not be working right still, not 100% sure - last command of 2nd sub called may process an extra time</t>
   </si>
   <si>
-    <t>saving games needs to save board state if a reprogram switch was hit - dump game state when reprogram switch is hit</t>
-  </si>
-  <si>
     <t>dave</t>
   </si>
   <si>
@@ -253,6 +244,45 @@
   </si>
   <si>
     <t>ability to disable/enable/move end square</t>
+  </si>
+  <si>
+    <t>ability to totally disable a tile so it doesn't show up at all</t>
+  </si>
+  <si>
+    <t>subs shouldn't be able to call themselves</t>
+  </si>
+  <si>
+    <t>if sub1/2 isn't available it shouldn't allow clicking or even draw the tabs</t>
+  </si>
+  <si>
+    <t>level select/profile should have exit</t>
+  </si>
+  <si>
+    <t>Brief pause upon level completion, do a victory dance or whatever</t>
+  </si>
+  <si>
+    <t>at end of level, buttons should be, in order, advance, return to main menu</t>
+  </si>
+  <si>
+    <t>add a button to replay level when you finish a level</t>
+  </si>
+  <si>
+    <t>click to add for instructions if the block hasn't been moved</t>
+  </si>
+  <si>
+    <t>in the hover tooltips for instructions it should say what the instruction is</t>
+  </si>
+  <si>
+    <t>for any fucked up shit we have that can work on a level, have it as a tickbox to enable it for the entire level</t>
+  </si>
+  <si>
+    <t>punch should not automatically move you into the square</t>
+  </si>
+  <si>
+    <t>Raised tiles need to be shorter to improve visibility of the map - different color tile tops, as well as better designed levels</t>
+  </si>
+  <si>
+    <t>map centering issues verifymappositions() is where the errors are, this needs some work</t>
   </si>
 </sst>
 </file>
@@ -323,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -332,6 +362,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,15 +657,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P81"/>
+  <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -849,9 +880,11 @@
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="4">
+        <v>39901</v>
+      </c>
       <c r="C20" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -868,312 +901,329 @@
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="1:16" s="2" customFormat="1">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="4">
+        <v>39901</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+    </row>
+    <row r="22" spans="1:16" s="3" customFormat="1">
+      <c r="A22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="4">
+        <v>39888</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" s="3" customFormat="1">
+      <c r="A23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="4">
+        <v>39888</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" s="3" customFormat="1">
+      <c r="A24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="4">
+        <v>39888</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" s="3" customFormat="1">
+      <c r="A25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="4">
+        <v>39889</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" s="2" customFormat="1">
+      <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="2" customFormat="1">
-      <c r="A22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" s="2" customFormat="1">
-      <c r="A23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-    </row>
-    <row r="24" spans="1:16" s="2" customFormat="1">
-      <c r="A24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" s="2" customFormat="1">
-      <c r="A25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" s="3" customFormat="1">
-      <c r="A26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="4">
-        <v>39888</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" s="3" customFormat="1">
-      <c r="A27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="4">
-        <v>39888</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>70</v>
+    <row r="27" spans="1:16" s="2" customFormat="1">
+      <c r="A27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="3" customFormat="1">
       <c r="A28" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B28" s="4">
+        <v>39901</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" s="2" customFormat="1">
+      <c r="A29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="8">
+        <v>39902</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" s="3" customFormat="1">
+      <c r="A30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="4">
+        <v>39901</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" s="2" customFormat="1">
+      <c r="A31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" s="2" customFormat="1">
+      <c r="A32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="2" customFormat="1">
+      <c r="C33" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="3" customFormat="1">
+      <c r="A34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="4">
+        <v>39901</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="3" customFormat="1">
+      <c r="A35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="4">
+        <v>39901</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="6" customFormat="1">
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="1:3" s="6" customFormat="1">
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:3" s="6" customFormat="1">
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="1:3" s="5" customFormat="1">
+      <c r="C39" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="3" customFormat="1">
+      <c r="A40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="4">
+        <v>39901</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="2" customFormat="1">
+      <c r="C41" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="2" customFormat="1">
+      <c r="A42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="2" customFormat="1">
+      <c r="C43" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="2" customFormat="1">
+      <c r="C44" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="2" customFormat="1">
+      <c r="A45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="2" customFormat="1">
+      <c r="C46" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="2" customFormat="1">
+      <c r="C47" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="2" customFormat="1">
+      <c r="C48" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" s="2" customFormat="1">
+      <c r="D49" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" s="2" customFormat="1">
+      <c r="D50" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" s="2" customFormat="1">
+      <c r="D51" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" s="2" customFormat="1">
+      <c r="A52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" s="2" customFormat="1">
+      <c r="A53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" s="2" customFormat="1">
+      <c r="A54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="C58" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" s="3" customFormat="1">
+      <c r="A59" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" s="4">
         <v>39888</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" s="3" customFormat="1">
-      <c r="A29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="4">
-        <v>39889</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" s="6" customFormat="1">
-      <c r="B30" s="7"/>
-    </row>
-    <row r="31" spans="1:16" s="6" customFormat="1">
-      <c r="B31" s="7"/>
-    </row>
-    <row r="32" spans="1:16" s="6" customFormat="1">
-      <c r="B32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" s="5" customFormat="1">
-      <c r="C33" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="2" customFormat="1">
-      <c r="C34" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="2" customFormat="1">
-      <c r="A35" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="2" customFormat="1">
-      <c r="C36" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="2" customFormat="1">
-      <c r="C37" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="2" customFormat="1">
-      <c r="A38" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="3" customFormat="1">
-      <c r="A39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="2" customFormat="1">
-      <c r="C40" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="2" customFormat="1">
-      <c r="C41" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="2" customFormat="1">
-      <c r="C42" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="2" customFormat="1">
-      <c r="D43" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="2" customFormat="1">
-      <c r="D44" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="2" customFormat="1">
-      <c r="D45" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="2" customFormat="1">
-      <c r="A46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="2" customFormat="1">
-      <c r="A47" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="2" customFormat="1">
-      <c r="C48" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16">
-      <c r="A49" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-    </row>
-    <row r="50" spans="1:16">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-    </row>
-    <row r="52" spans="1:16">
-      <c r="C52" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" s="3" customFormat="1">
-      <c r="A53" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B53" s="4">
-        <v>39888</v>
-      </c>
-      <c r="C53" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" s="3" customFormat="1">
-      <c r="A54" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" s="3" customFormat="1">
-      <c r="A55" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" s="4">
-        <v>39882</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" s="3" customFormat="1">
-      <c r="A56" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" s="4">
-        <v>39887</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" s="2" customFormat="1">
-      <c r="C57" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" s="3" customFormat="1">
-      <c r="A58" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" s="2" customFormat="1">
-      <c r="C59" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:16" s="3" customFormat="1">
@@ -1181,21 +1231,21 @@
         <v>10</v>
       </c>
       <c r="B60" s="4">
-        <v>39887</v>
+        <v>39881</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:16" s="3" customFormat="1">
       <c r="A61" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B61" s="4">
-        <v>39887</v>
+        <v>39882</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:16" s="3" customFormat="1">
@@ -1206,88 +1256,182 @@
         <v>39887</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:16" s="3" customFormat="1">
       <c r="A63" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B63" s="4">
+        <v>39901</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" s="3" customFormat="1">
+      <c r="A64" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" s="4">
         <v>39887</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="3:4">
-      <c r="C66" s="5" t="s">
+      <c r="C64" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" s="3" customFormat="1">
+      <c r="A65" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" s="3" customFormat="1">
+      <c r="A66" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" s="3" customFormat="1">
+      <c r="A67" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B67" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" s="2" customFormat="1">
+      <c r="C68" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" s="3" customFormat="1">
+      <c r="A69" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" s="2" customFormat="1">
+      <c r="C70" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" s="2" customFormat="1">
+      <c r="C71" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" s="2" customFormat="1"/>
+    <row r="73" spans="1:3" s="2" customFormat="1"/>
+    <row r="76" spans="1:3">
+      <c r="C76" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="3:4">
-      <c r="C67" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="68" spans="3:4">
-      <c r="C68" s="1" t="s">
+    <row r="77" spans="1:3">
+      <c r="C77" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="C78" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="3:4">
-      <c r="C69" s="1" t="s">
+    <row r="79" spans="1:3">
+      <c r="C79" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="3:4">
-      <c r="C72" s="5" t="s">
+    <row r="80" spans="1:3">
+      <c r="C80" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="C81" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="C83" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="C84" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="3:4">
-      <c r="C73" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="74" spans="3:4">
-      <c r="C74" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="75" spans="3:4">
-      <c r="D75" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="76" spans="3:4">
-      <c r="C76" s="1" t="s">
+    <row r="85" spans="1:4">
+      <c r="C85" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="D86" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="C87" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="C88" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="C89" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="3:4">
-      <c r="C77" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="78" spans="3:4">
-      <c r="C78" s="1" t="s">
+    <row r="90" spans="1:4" s="3" customFormat="1">
+      <c r="A90" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="3:4">
-      <c r="C79" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="80" spans="3:4">
-      <c r="C80" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="81" spans="3:3">
-      <c r="C81" s="1" t="s">
-        <v>77</v>
+    <row r="91" spans="1:4" s="3" customFormat="1">
+      <c r="A91" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="C92" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated move forward until unable image to be CLEARLY different
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -353,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -362,7 +362,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -968,42 +967,48 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="2" customFormat="1">
-      <c r="A26" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" s="2" customFormat="1">
-      <c r="A27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>63</v>
+    <row r="26" spans="1:16" s="3" customFormat="1">
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="4">
+        <v>39901</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" s="3" customFormat="1">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="3" customFormat="1">
       <c r="A28" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B28" s="4">
         <v>39901</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" s="2" customFormat="1">
-      <c r="A29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="8">
-        <v>39902</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" s="3" customFormat="1">
+      <c r="A29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="4">
+        <v>39901</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="3" customFormat="1">
@@ -1014,50 +1019,41 @@
         <v>39901</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="2" customFormat="1">
       <c r="A31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" s="2" customFormat="1">
+      <c r="C32" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="2" customFormat="1">
+      <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="2" customFormat="1">
-      <c r="A32" s="2" t="s">
+    <row r="34" spans="1:3" s="2" customFormat="1">
+      <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1">
-      <c r="C33" s="2" t="s">
+    <row r="35" spans="1:3" s="2" customFormat="1">
+      <c r="C35" s="2" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="3" customFormat="1">
-      <c r="A34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="4">
-        <v>39901</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="3" customFormat="1">
-      <c r="A35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="4">
-        <v>39901</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="6" customFormat="1">
@@ -1085,73 +1081,76 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1">
-      <c r="C41" s="2" t="s">
+    <row r="41" spans="1:3" s="3" customFormat="1">
+      <c r="A41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="2" customFormat="1">
+      <c r="C42" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:3" s="2" customFormat="1">
+      <c r="A43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="2" customFormat="1">
-      <c r="C43" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="2" customFormat="1">
       <c r="C44" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="2" customFormat="1">
+      <c r="C45" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:3" s="2" customFormat="1">
+      <c r="A46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" s="2" customFormat="1">
-      <c r="C46" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="2" customFormat="1">
       <c r="C47" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="2" customFormat="1">
       <c r="C48" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" s="2" customFormat="1">
+      <c r="C49" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" s="2" customFormat="1">
-      <c r="D49" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:16" s="2" customFormat="1">
       <c r="D50" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:16" s="2" customFormat="1">
       <c r="D51" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" s="2" customFormat="1">
+      <c r="D52" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" s="2" customFormat="1">
-      <c r="A52" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:16" s="2" customFormat="1">
@@ -1159,15 +1158,15 @@
         <v>7</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:16" s="2" customFormat="1">
       <c r="A54" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -1314,20 +1313,20 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="2" customFormat="1">
-      <c r="C68" s="2" t="s">
+    <row r="68" spans="1:3" s="3" customFormat="1">
+      <c r="A68" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" s="2" customFormat="1">
+      <c r="C69" s="2" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" s="3" customFormat="1">
-      <c r="A69" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B69" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="2" customFormat="1">
@@ -1377,56 +1376,56 @@
         <v>52</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
-      <c r="C84" s="1" t="s">
+    <row r="84" spans="1:4" s="3" customFormat="1">
+      <c r="A84" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B84" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="3" customFormat="1">
+      <c r="A85" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B85" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="C86" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="C85" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="D86" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="C87" s="1" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="C88" s="1" t="s">
-        <v>87</v>
+      <c r="D88" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="C89" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="C90" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="C91" s="1" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" s="3" customFormat="1">
-      <c r="A90" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B90" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" s="3" customFormat="1">
-      <c r="A91" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B91" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:4">

</xml_diff>

<commit_message>
removed all climb over blocks from the map files changed the description of climb to no longer say "and climb over stuff" adjusted the gap tile so that it is easier to see what it is
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -875,7 +875,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="2" customFormat="1">
+    <row r="20" spans="1:16" s="3" customFormat="1">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -885,19 +885,6 @@
       <c r="C20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
     </row>
     <row r="21" spans="1:16" s="2" customFormat="1">
       <c r="A21" s="3" t="s">

</xml_diff>

<commit_message>
more fixes to tutorial maps updated Wish List added support for disabling of the end square something else was fixed
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="90">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>map centering issues verifymappositions() is where the errors are, this needs some work</t>
+  </si>
+  <si>
+    <t>move forward until unable does not end its trigger when facing a door</t>
   </si>
 </sst>
 </file>
@@ -658,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -842,7 +845,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="3" customFormat="1">
+    <row r="17" spans="1:3" s="3" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -853,7 +856,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="3" customFormat="1">
+    <row r="18" spans="1:3" s="3" customFormat="1">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -864,7 +867,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="3" customFormat="1">
+    <row r="19" spans="1:3" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
@@ -875,7 +878,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="3" customFormat="1">
+    <row r="20" spans="1:3" s="3" customFormat="1">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -886,7 +889,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="2" customFormat="1">
+    <row r="21" spans="1:3" s="3" customFormat="1">
       <c r="A21" s="3" t="s">
         <v>70</v>
       </c>
@@ -896,21 +899,8 @@
       <c r="C21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-    </row>
-    <row r="22" spans="1:16" s="3" customFormat="1">
+    </row>
+    <row r="22" spans="1:3" s="3" customFormat="1">
       <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
@@ -921,7 +911,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="3" customFormat="1">
+    <row r="23" spans="1:3" s="3" customFormat="1">
       <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
@@ -932,7 +922,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="3" customFormat="1">
+    <row r="24" spans="1:3" s="3" customFormat="1">
       <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
@@ -943,7 +933,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="3" customFormat="1">
+    <row r="25" spans="1:3" s="3" customFormat="1">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
@@ -954,7 +944,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="3" customFormat="1">
+    <row r="26" spans="1:3" s="3" customFormat="1">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -965,7 +955,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="3" customFormat="1">
+    <row r="27" spans="1:3" s="3" customFormat="1">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -976,7 +966,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="3" customFormat="1">
+    <row r="28" spans="1:3" s="3" customFormat="1">
       <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
@@ -987,7 +977,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="3" customFormat="1">
+    <row r="29" spans="1:3" s="3" customFormat="1">
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
@@ -998,7 +988,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="3" customFormat="1">
+    <row r="30" spans="1:3" s="3" customFormat="1">
       <c r="A30" s="3" t="s">
         <v>10</v>
       </c>
@@ -1009,7 +999,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="2" customFormat="1">
+    <row r="31" spans="1:3" s="2" customFormat="1">
       <c r="A31" s="2" t="s">
         <v>46</v>
       </c>
@@ -1017,7 +1007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="2" customFormat="1">
+    <row r="32" spans="1:3" s="2" customFormat="1">
       <c r="C32" s="2" t="s">
         <v>63</v>
       </c>
@@ -1079,81 +1069,81 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1">
-      <c r="C42" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="2" customFormat="1">
-      <c r="A43" s="2" t="s">
+    <row r="42" spans="1:3" s="3" customFormat="1">
+      <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>12</v>
+      <c r="C42" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="3" customFormat="1">
+      <c r="A43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="2" customFormat="1">
       <c r="C44" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="2" customFormat="1">
+      <c r="A45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="2" customFormat="1">
+      <c r="C46" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" s="2" customFormat="1">
-      <c r="C45" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" s="2" customFormat="1">
-      <c r="A46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="2" customFormat="1">
       <c r="C47" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="2" customFormat="1">
+      <c r="A48" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C48" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:16" s="2" customFormat="1">
       <c r="C49" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" s="2" customFormat="1">
+      <c r="C50" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" s="2" customFormat="1">
+      <c r="C51" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" s="2" customFormat="1">
-      <c r="D50" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" s="2" customFormat="1">
-      <c r="D51" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:16" s="2" customFormat="1">
       <c r="D52" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" s="2" customFormat="1">
+      <c r="D53" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" s="2" customFormat="1">
+      <c r="D54" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" s="2" customFormat="1">
-      <c r="A53" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" s="2" customFormat="1">
-      <c r="A54" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -1326,7 +1316,17 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:3" s="2" customFormat="1"/>
+    <row r="72" spans="1:3" s="3" customFormat="1">
+      <c r="A72" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="73" spans="1:3" s="2" customFormat="1"/>
     <row r="76" spans="1:3">
       <c r="C76" s="5" t="s">
@@ -1396,19 +1396,25 @@
         <v>53</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="C87" s="1" t="s">
+    <row r="87" spans="1:4" s="3" customFormat="1">
+      <c r="A87" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B87" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="C88" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
-      <c r="D88" s="1" t="s">
+    <row r="89" spans="1:4">
+      <c r="D89" s="1" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="C89" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:4">

</xml_diff>

<commit_message>
Now able to exit to main menu from level select and profile select states
as well as choosing a profile that you tried to create, but already exists (once i can get the button to display anyways)

there is also now a button that will allow you to replay the level you just finished, although i need to find the code that will clear out the command list
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="11040" windowHeight="6930" tabRatio="499"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="90">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -356,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -365,6 +365,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1016,20 +1017,29 @@
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B33" s="8">
+        <v>39902</v>
+      </c>
       <c r="C33" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:3" s="3" customFormat="1">
+      <c r="A34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1">
-      <c r="C35" s="2" t="s">
+    <row r="35" spans="1:3" s="3" customFormat="1">
+      <c r="A35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed some artwork, a few other things need to be fixed
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>move forward until unable does not end its trigger when facing a door</t>
+  </si>
+  <si>
+    <t>When in mid game, if you leave to main menu and create a new profile, it wipes out the save file</t>
   </si>
 </sst>
 </file>
@@ -356,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -365,7 +368,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1013,14 +1015,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:3" s="3" customFormat="1">
+      <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="4">
         <v>39902</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1028,6 +1030,9 @@
       <c r="A34" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="B34" s="4">
+        <v>39902</v>
+      </c>
       <c r="C34" s="3" t="s">
         <v>81</v>
       </c>
@@ -1043,8 +1048,13 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="6" customFormat="1">
-      <c r="B36" s="7"/>
+    <row r="36" spans="1:3" s="2" customFormat="1">
+      <c r="A36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="37" spans="1:3" s="6" customFormat="1">
       <c r="B37" s="7"/>

</xml_diff>

<commit_message>
LevelSelectState now deletes itself, and the button now works to select a profile entered by user that already exists. Still need to fix the saving problems, and wishlist is updated
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="92">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -288,7 +288,10 @@
     <t>move forward until unable does not end its trigger when facing a door</t>
   </si>
   <si>
-    <t>When in mid game, if you leave to main menu and create a new profile, it wipes out the save file</t>
+    <t>Level select from create profile doesn’t erase its state</t>
+  </si>
+  <si>
+    <t>When in mid game, if you leave to main menu and create a new profile, it wipes out the save file / all saving files aren't working properly</t>
   </si>
 </sst>
 </file>
@@ -664,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1053,11 +1056,19 @@
         <v>14</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="3" customFormat="1">
+      <c r="A37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="4">
+        <v>39904</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" s="6" customFormat="1">
-      <c r="B37" s="7"/>
     </row>
     <row r="38" spans="1:3" s="6" customFormat="1">
       <c r="B38" s="7"/>

</xml_diff>

<commit_message>
Subs now can't call eachother... kind of a redesign / workaround but it works.
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="11040" windowHeight="6930" tabRatio="499"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>When in mid game, if you leave to main menu and create a new profile, it wipes out the save file / all saving files aren't working properly</t>
+  </si>
+  <si>
+    <t>Note: Subs redesigned to not call any other subs</t>
   </si>
 </sst>
 </file>
@@ -315,7 +318,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +334,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -371,6 +380,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1288,7 +1298,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="3" customFormat="1">
+    <row r="65" spans="1:7" s="3" customFormat="1">
       <c r="A65" s="3" t="s">
         <v>10</v>
       </c>
@@ -1299,7 +1309,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="1:3" s="3" customFormat="1">
+    <row r="66" spans="1:7" s="3" customFormat="1">
       <c r="A66" s="3" t="s">
         <v>10</v>
       </c>
@@ -1310,7 +1320,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:3" s="3" customFormat="1">
+    <row r="67" spans="1:7" s="3" customFormat="1">
       <c r="A67" s="3" t="s">
         <v>10</v>
       </c>
@@ -1321,7 +1331,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="3" customFormat="1">
+    <row r="68" spans="1:7" s="3" customFormat="1">
       <c r="A68" s="3" t="s">
         <v>10</v>
       </c>
@@ -1332,22 +1342,37 @@
         <v>88</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="2" customFormat="1">
+    <row r="69" spans="1:7" s="2" customFormat="1">
       <c r="C69" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="2" customFormat="1">
-      <c r="C70" s="2" t="s">
+    <row r="70" spans="1:7" s="3" customFormat="1">
+      <c r="A70" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="4">
+        <v>39905</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" s="2" customFormat="1">
-      <c r="C71" s="2" t="s">
+      <c r="G70" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" s="3" customFormat="1">
+      <c r="A71" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:3" s="3" customFormat="1">
+    <row r="72" spans="1:7" s="3" customFormat="1">
       <c r="A72" s="3" t="s">
         <v>10</v>
       </c>
@@ -1358,28 +1383,28 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="2" customFormat="1"/>
-    <row r="76" spans="1:3">
+    <row r="73" spans="1:7" s="8" customFormat="1"/>
+    <row r="76" spans="1:7">
       <c r="C76" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:7">
       <c r="C77" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:7">
       <c r="C78" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:7">
       <c r="C79" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:7">
       <c r="C80" s="1" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
map updates - map 2 is now functioning, maps 3-10 need testing but have enough bytes to complete select profile state has a back button create new game, if profile exists, has a back button now select level now shows what your highest level available is level select now shows the best score for the current level if you single-click to add a new command, it autoscrolls down when it goes too far you can now drag commands in to a line beyond the first 3 lines switches and teleports now rotate with the map in memory as well as graphically
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="108">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -225,9 +225,6 @@
     <t>compass click handlers aren't working and I have no idea why - fixed</t>
   </si>
   <si>
-    <t>subs calling subs may not be working right still, not 100% sure - last command of 2nd sub called may process an extra time</t>
-  </si>
-  <si>
     <t>dave</t>
   </si>
   <si>
@@ -295,6 +292,54 @@
   </si>
   <si>
     <t>Note: Subs redesigned to not call any other subs</t>
+  </si>
+  <si>
+    <t>Select profile state needs a "back" button</t>
+  </si>
+  <si>
+    <t>Under create new game, if profile already exists, there needs to be a back button</t>
+  </si>
+  <si>
+    <t>select level should show what your highest level available is</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>if you put in a lot of commands, while processing it should auto-scroll to the next row</t>
+  </si>
+  <si>
+    <t>if you drag an instruction into the instruction list, it drops it as if it was on the first page and not on the current scroll page</t>
+  </si>
+  <si>
+    <t>156 used</t>
+  </si>
+  <si>
+    <t>62 with reprogram</t>
+  </si>
+  <si>
+    <t>replay level needs a total restart of map, it is picking up from the repgoram square</t>
+  </si>
+  <si>
+    <t>if you put in a lot of commands, while processing you should be able to scroll the instruction list</t>
+  </si>
+  <si>
+    <t>110 used</t>
+  </si>
+  <si>
+    <t>switches and teleporters aren't rotating with the map (they are visually, not in the object list)</t>
+  </si>
+  <si>
+    <t>if you put in a lot of commands with auto click and it adds another row, it should auto-scroll to next row</t>
+  </si>
+  <si>
+    <t>IRRELEVANT - subs can't call subs anymoresubs calling subs may not be working right still, not 100% sure - last command of 2nd sub called may process an extra time</t>
+  </si>
+  <si>
+    <t>this looks as if it should be functioning… not sure why it isn't</t>
+  </si>
+  <si>
+    <t>level select should show the score for the current level</t>
   </si>
 </sst>
 </file>
@@ -318,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,6 +385,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -381,6 +432,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P92"/>
+  <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -902,18 +955,18 @@
         <v>39901</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="3" customFormat="1">
       <c r="A21" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="4">
         <v>39901</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="3" customFormat="1">
@@ -979,7 +1032,7 @@
         <v>39902</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="3" customFormat="1">
@@ -990,7 +1043,7 @@
         <v>39901</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="3" customFormat="1">
@@ -1001,7 +1054,7 @@
         <v>39901</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="3" customFormat="1">
@@ -1012,19 +1065,25 @@
         <v>39901</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="2" customFormat="1">
-      <c r="A31" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="3" customFormat="1">
+      <c r="A31" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="B31" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="2" customFormat="1">
-      <c r="C32" s="2" t="s">
+    <row r="32" spans="1:3" s="3" customFormat="1">
+      <c r="A32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1036,7 +1095,7 @@
         <v>39902</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="3" customFormat="1">
@@ -1047,7 +1106,7 @@
         <v>39902</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="3" customFormat="1">
@@ -1058,15 +1117,15 @@
         <v>39902</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="2" customFormat="1">
-      <c r="A36" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="3" customFormat="1">
+      <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>91</v>
+      <c r="C36" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="3" customFormat="1">
@@ -1077,15 +1136,29 @@
         <v>39904</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="6" customFormat="1">
-      <c r="B38" s="7"/>
-    </row>
-    <row r="39" spans="1:3" s="5" customFormat="1">
-      <c r="C39" s="5" t="s">
-        <v>1</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="3" customFormat="1">
+      <c r="A38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="3" customFormat="1">
+      <c r="A39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="3" customFormat="1">
@@ -1093,209 +1166,163 @@
         <v>10</v>
       </c>
       <c r="B40" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="3" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="2" customFormat="1">
+      <c r="B42" s="9"/>
+    </row>
+    <row r="43" spans="1:3" s="2" customFormat="1">
+      <c r="B43" s="9"/>
+    </row>
+    <row r="44" spans="1:3" s="6" customFormat="1">
+      <c r="B44" s="7"/>
+    </row>
+    <row r="45" spans="1:3" s="5" customFormat="1">
+      <c r="C45" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="3" customFormat="1">
+      <c r="A46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="4">
         <v>39901</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="3" customFormat="1">
-      <c r="A41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="4">
+    <row r="47" spans="1:3" s="3" customFormat="1">
+      <c r="A47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="4">
         <v>39902</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="3" customFormat="1">
-      <c r="A42" s="3" t="s">
+    <row r="48" spans="1:3" s="3" customFormat="1">
+      <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="3" customFormat="1">
-      <c r="A43" s="3" t="s">
+    <row r="49" spans="1:16" s="3" customFormat="1">
+      <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="2" customFormat="1">
-      <c r="C44" s="2" t="s">
+    <row r="50" spans="1:16" s="3" customFormat="1">
+      <c r="C50" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1">
-      <c r="A45" s="2" t="s">
+    <row r="51" spans="1:16" s="10" customFormat="1">
+      <c r="A51" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C51" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="2" customFormat="1">
-      <c r="C46" s="2" t="s">
+    <row r="52" spans="1:16" s="10" customFormat="1">
+      <c r="C52" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="2" customFormat="1">
-      <c r="C47" s="2" t="s">
+    <row r="53" spans="1:16" s="10" customFormat="1">
+      <c r="C53" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="2" customFormat="1">
-      <c r="A48" s="2" t="s">
+    <row r="54" spans="1:16" s="10" customFormat="1">
+      <c r="A54" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C54" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="2" customFormat="1">
-      <c r="C49" s="2" t="s">
+    <row r="55" spans="1:16" s="10" customFormat="1">
+      <c r="C55" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="2" customFormat="1">
-      <c r="C50" s="2" t="s">
+    <row r="56" spans="1:16" s="10" customFormat="1">
+      <c r="C56" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="2" customFormat="1">
-      <c r="C51" s="2" t="s">
+    <row r="57" spans="1:16" s="10" customFormat="1">
+      <c r="C57" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="2" customFormat="1">
-      <c r="D52" s="2" t="s">
+    <row r="58" spans="1:16" s="10" customFormat="1">
+      <c r="D58" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="2" customFormat="1">
-      <c r="D53" s="2" t="s">
+    <row r="59" spans="1:16" s="10" customFormat="1">
+      <c r="D59" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="2" customFormat="1">
-      <c r="D54" s="2" t="s">
+    <row r="60" spans="1:16" s="10" customFormat="1">
+      <c r="D60" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
-      <c r="A55" s="2" t="s">
+    <row r="61" spans="1:16" s="10" customFormat="1">
+      <c r="A61" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2" t="s">
+      <c r="C61" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
-      <c r="O55" s="2"/>
-      <c r="P55" s="2"/>
-    </row>
-    <row r="56" spans="1:16">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
-      <c r="O56" s="2"/>
-      <c r="P56" s="2"/>
-    </row>
-    <row r="58" spans="1:16">
-      <c r="C58" s="5" t="s">
+    </row>
+    <row r="62" spans="1:16">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="P62" s="2"/>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="C64" s="5" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" s="3" customFormat="1">
-      <c r="A59" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B59" s="4">
-        <v>39888</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" s="3" customFormat="1">
-      <c r="A60" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B60" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" s="3" customFormat="1">
-      <c r="A61" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B61" s="4">
-        <v>39882</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" s="3" customFormat="1">
-      <c r="A62" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B62" s="4">
-        <v>39887</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" s="3" customFormat="1">
-      <c r="A63" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B63" s="4">
-        <v>39901</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" s="3" customFormat="1">
-      <c r="A64" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B64" s="4">
-        <v>39887</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:7" s="3" customFormat="1">
@@ -1303,10 +1330,10 @@
         <v>10</v>
       </c>
       <c r="B65" s="4">
-        <v>39887</v>
+        <v>39888</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:7" s="3" customFormat="1">
@@ -1314,21 +1341,21 @@
         <v>10</v>
       </c>
       <c r="B66" s="4">
-        <v>39887</v>
+        <v>39881</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:7" s="3" customFormat="1">
       <c r="A67" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B67" s="4">
-        <v>39887</v>
+        <v>39882</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
     </row>
     <row r="68" spans="1:7" s="3" customFormat="1">
@@ -1336,40 +1363,43 @@
         <v>10</v>
       </c>
       <c r="B68" s="4">
-        <v>39902</v>
+        <v>39887</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" s="2" customFormat="1">
-      <c r="C69" s="2" t="s">
-        <v>69</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="3" customFormat="1">
+      <c r="A69" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" s="4">
+        <v>39901</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:7" s="3" customFormat="1">
       <c r="A70" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B70" s="4">
-        <v>39905</v>
+        <v>39887</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:7" s="3" customFormat="1">
       <c r="A71" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B71" s="4">
-        <v>39902</v>
+        <v>39887</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="3" customFormat="1">
@@ -1377,57 +1407,119 @@
         <v>10</v>
       </c>
       <c r="B72" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" s="3" customFormat="1">
+      <c r="A73" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="3" customFormat="1">
+      <c r="A74" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" s="4">
         <v>39902</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" s="8" customFormat="1"/>
-    <row r="76" spans="1:7">
-      <c r="C76" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="C77" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="C78" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="C79" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="C80" s="1" t="s">
+      <c r="C74" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="10" customFormat="1">
+      <c r="C75" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" s="3" customFormat="1">
+      <c r="A76" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" s="4">
+        <v>39905</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="C81" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="C83" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" s="3" customFormat="1">
-      <c r="A84" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B84" s="4">
+      <c r="G76" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" s="3" customFormat="1">
+      <c r="A77" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" s="4">
         <v>39902</v>
       </c>
-      <c r="C84" s="3" t="s">
-        <v>58</v>
+      <c r="C77" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" s="3" customFormat="1">
+      <c r="A78" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" s="3" customFormat="1">
+      <c r="A79" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" s="2" customFormat="1">
+      <c r="B80" s="9"/>
+      <c r="C80" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" s="3" customFormat="1">
+      <c r="A81" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B81" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" s="2" customFormat="1">
+      <c r="B82" s="9"/>
+      <c r="C82" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" s="2" customFormat="1">
+      <c r="B83" s="9"/>
+      <c r="C83" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" s="2" customFormat="1">
+      <c r="B84" s="9"/>
+      <c r="D84" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="85" spans="1:4" s="3" customFormat="1">
@@ -1435,57 +1527,217 @@
         <v>10</v>
       </c>
       <c r="B85" s="4">
-        <v>39902</v>
+        <v>39907</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" s="3" customFormat="1">
-      <c r="A86" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B86" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" s="3" customFormat="1">
-      <c r="A87" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B87" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="C88" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" s="8" customFormat="1"/>
     <row r="89" spans="1:4">
-      <c r="D89" s="1" t="s">
-        <v>62</v>
+      <c r="C89" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="C90" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="C91" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="C92" s="1" t="s">
-        <v>74</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="C93" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="C94" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="C96" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" s="3" customFormat="1">
+      <c r="A97" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="3" customFormat="1">
+      <c r="A98" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B98" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" s="3" customFormat="1">
+      <c r="A99" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B99" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" s="3" customFormat="1">
+      <c r="A100" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B100" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="C101" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="D102" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="C103" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="C104" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="C105" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="1">
+        <v>1</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="1">
+        <v>2</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="1">
+        <v>3</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="1">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
go figure, i fogot a few files
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1176,7 +1176,9 @@
       <c r="A41" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="4"/>
+      <c r="B41" s="4">
+        <v>39907</v>
+      </c>
       <c r="C41" s="3" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
renamed all maps to be mapcX for chris's maps, mapgX for geo's maps and mapoX for oscar's map, prepping for totally rearranging the order in which the maps appear.
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="123">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -312,9 +312,6 @@
     <t>if you drag an instruction into the instruction list, it drops it as if it was on the first page and not on the current scroll page</t>
   </si>
   <si>
-    <t>156 used</t>
-  </si>
-  <si>
     <t>62 with reprogram</t>
   </si>
   <si>
@@ -324,9 +321,6 @@
     <t>if you put in a lot of commands, while processing you should be able to scroll the instruction list</t>
   </si>
   <si>
-    <t>110 used</t>
-  </si>
-  <si>
     <t>switches and teleporters aren't rotating with the map (they are visually, not in the object list)</t>
   </si>
   <si>
@@ -340,6 +334,57 @@
   </si>
   <si>
     <t>level select should show the score for the current level</t>
+  </si>
+  <si>
+    <t>used left switch</t>
+  </si>
+  <si>
+    <t>fixed bad switch</t>
+  </si>
+  <si>
+    <t>very easy, should be an earlier level</t>
+  </si>
+  <si>
+    <t>fairly easy - fun water map</t>
+  </si>
+  <si>
+    <t>jump-move forward and jump-move forward 3 are EASILY mass repeated on this map, will test with subs</t>
+  </si>
+  <si>
+    <t>fun - lots of jumping</t>
+  </si>
+  <si>
+    <t>sub1 = jump/move forward, sub2 = jump</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>subs</t>
+  </si>
+  <si>
+    <t>reprogram</t>
+  </si>
+  <si>
+    <t>annoying as hell</t>
+  </si>
+  <si>
+    <t>easy - very straightforward</t>
+  </si>
+  <si>
+    <t>not very complex, fairly easy as well - lots of random extra stuff not related to finishing the map</t>
+  </si>
+  <si>
+    <t>could probably lose the reprogram square, additionally, not sure if intended, but the last two switches can be skipped entirely, may want to disable jump on this map, or make some reason for the switches</t>
+  </si>
+  <si>
+    <t>very linear, interesting figuring out what does what</t>
+  </si>
+  <si>
+    <t>needs edge squares removed maybe</t>
+  </si>
+  <si>
+    <t>can't be beaten</t>
   </si>
 </sst>
 </file>
@@ -728,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P139"/>
+  <dimension ref="A1:P136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1180,7 +1225,7 @@
         <v>39907</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="2" customFormat="1">
@@ -1439,7 +1484,7 @@
     </row>
     <row r="75" spans="1:7" s="10" customFormat="1">
       <c r="C75" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="3" customFormat="1">
@@ -1486,7 +1531,7 @@
         <v>39907</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:7" s="2" customFormat="1">
@@ -1509,19 +1554,19 @@
     <row r="82" spans="1:4" s="2" customFormat="1">
       <c r="B82" s="9"/>
       <c r="C82" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:4" s="2" customFormat="1">
       <c r="B83" s="9"/>
       <c r="C83" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:4" s="2" customFormat="1">
       <c r="B84" s="9"/>
       <c r="D84" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="1:4" s="3" customFormat="1">
@@ -1532,7 +1577,7 @@
         <v>39907</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:4" s="8" customFormat="1"/>
@@ -1640,7 +1685,18 @@
         <v>73</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="121" spans="1:11">
+      <c r="B121" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
       <c r="A122" s="1">
         <v>1</v>
       </c>
@@ -1648,98 +1704,170 @@
         <v>95</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:11">
       <c r="A123" s="1">
         <v>2</v>
       </c>
-      <c r="B123" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
+      <c r="B123" s="1">
+        <v>156</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
       <c r="A124" s="1">
         <v>3</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
+      <c r="B124" s="1">
+        <v>110</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
       <c r="A125" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="126" spans="1:3">
+      <c r="B125" s="1">
+        <v>88</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
       <c r="A126" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="127" spans="1:3">
+      <c r="B126" s="1">
+        <v>92</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
       <c r="A127" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="128" spans="1:3">
+      <c r="B127" s="1">
+        <v>78</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
       <c r="A128" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="129" spans="1:1">
+      <c r="B128" s="1">
+        <v>64</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
       <c r="A129" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="B129" s="1">
+        <v>156</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
       <c r="A130" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="131" spans="1:1">
+      <c r="B130" s="1">
+        <v>306</v>
+      </c>
+      <c r="C130" s="1">
+        <v>164</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
       <c r="A131" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
+      <c r="B131" s="1">
+        <v>154</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
       <c r="A132" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="133" spans="1:1">
+      <c r="B132" s="1">
+        <v>128</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
       <c r="A133" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:12">
       <c r="A134" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="135" spans="1:1">
+      <c r="B134" s="1">
+        <v>182</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
       <c r="A135" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="136" spans="1:1">
+      <c r="B135" s="1">
+        <v>318</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L135" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
       <c r="A136" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="137" spans="1:1">
-      <c r="A137" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1">
-      <c r="A138" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1">
-      <c r="A139" s="1">
-        <v>18</v>
+      <c r="F136" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
map updates changed the order of almost all the maps in the game updated memory requirements of maps
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="123">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -303,9 +303,6 @@
     <t>select level should show what your highest level available is</t>
   </si>
   <si>
-    <t>ok</t>
-  </si>
-  <si>
     <t>if you put in a lot of commands, while processing it should auto-scroll to the next row</t>
   </si>
   <si>
@@ -385,6 +382,9 @@
   </si>
   <si>
     <t>can't be beaten</t>
+  </si>
+  <si>
+    <t>short and sweet</t>
   </si>
 </sst>
 </file>
@@ -773,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P136"/>
+  <dimension ref="A1:P140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+      <selection activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1225,7 +1225,7 @@
         <v>39907</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="2" customFormat="1">
@@ -1484,7 +1484,7 @@
     </row>
     <row r="75" spans="1:7" s="10" customFormat="1">
       <c r="C75" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="3" customFormat="1">
@@ -1531,13 +1531,13 @@
         <v>39907</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" spans="1:7" s="2" customFormat="1">
       <c r="B80" s="9"/>
       <c r="C80" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:4" s="3" customFormat="1">
@@ -1548,25 +1548,25 @@
         <v>39907</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:4" s="2" customFormat="1">
       <c r="B82" s="9"/>
       <c r="C82" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="83" spans="1:4" s="2" customFormat="1">
       <c r="B83" s="9"/>
       <c r="C83" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:4" s="2" customFormat="1">
       <c r="B84" s="9"/>
       <c r="D84" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="85" spans="1:4" s="3" customFormat="1">
@@ -1577,7 +1577,7 @@
         <v>39907</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:4" s="8" customFormat="1"/>
@@ -1685,79 +1685,29 @@
         <v>73</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:6">
       <c r="B121" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D121" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11">
-      <c r="A122" s="1">
-        <v>1</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11">
-      <c r="A123" s="1">
-        <v>2</v>
-      </c>
-      <c r="B123" s="1">
-        <v>156</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11">
-      <c r="A124" s="1">
-        <v>3</v>
-      </c>
-      <c r="B124" s="1">
-        <v>110</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11">
-      <c r="A125" s="1">
-        <v>4</v>
-      </c>
-      <c r="B125" s="1">
-        <v>88</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K125" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11">
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B126" s="1">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K126" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="127" spans="1:11">
+    <row r="127" spans="1:6">
       <c r="A127" s="1">
         <v>6</v>
       </c>
@@ -1765,18 +1715,18 @@
         <v>78</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
       <c r="A128" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B128" s="1">
-        <v>64</v>
+        <v>154</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="129" spans="1:12">
@@ -1787,7 +1737,13 @@
         <v>156</v>
       </c>
       <c r="F129" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H129" s="1" t="s">
         <v>109</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="130" spans="1:12">
@@ -1801,24 +1757,18 @@
         <v>164</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H130" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="I130" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="131" spans="1:12">
       <c r="A131" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B131" s="1">
-        <v>154</v>
+        <v>56</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="132" spans="1:12">
@@ -1829,13 +1779,16 @@
         <v>128</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="133" spans="1:12">
       <c r="A133" s="1">
         <v>12</v>
       </c>
+      <c r="F133" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="1">
@@ -1845,7 +1798,7 @@
         <v>182</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="135" spans="1:12">
@@ -1856,10 +1809,10 @@
         <v>318</v>
       </c>
       <c r="F135" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L135" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="L135" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="136" spans="1:12">
@@ -1867,10 +1820,66 @@
         <v>15</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
+      <c r="A137" s="1">
+        <v>2</v>
+      </c>
+      <c r="B137" s="1">
+        <v>156</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
+      <c r="A138" s="1">
+        <v>3</v>
+      </c>
+      <c r="B138" s="1">
+        <v>110</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
+      <c r="A139" s="1">
+        <v>4</v>
+      </c>
+      <c r="B139" s="1">
+        <v>88</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K139" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
+      <c r="A140" s="1">
+        <v>5</v>
+      </c>
+      <c r="B140" s="1">
+        <v>92</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K140" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A126:G130">
+    <sortCondition ref="B126:B130"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added updating scoring mechanism fixed mapo1 to be completable added activate back in to mapc3 added history document
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="142">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -378,13 +378,70 @@
     <t>very linear, interesting figuring out what does what</t>
   </si>
   <si>
-    <t>needs edge squares removed maybe</t>
-  </si>
-  <si>
     <t>can't be beaten</t>
   </si>
   <si>
     <t>short and sweet</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>c4</t>
+  </si>
+  <si>
+    <t>c5</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>g2</t>
+  </si>
+  <si>
+    <t>g3</t>
+  </si>
+  <si>
+    <t>g4</t>
+  </si>
+  <si>
+    <t>g5</t>
+  </si>
+  <si>
+    <t>o1</t>
+  </si>
+  <si>
+    <t>o2</t>
+  </si>
+  <si>
+    <t>o3</t>
+  </si>
+  <si>
+    <t>o4</t>
+  </si>
+  <si>
+    <t>o5</t>
+  </si>
+  <si>
+    <t>not too bad</t>
+  </si>
+  <si>
+    <t>in game should show the level number</t>
+  </si>
+  <si>
+    <t>when sub1/sub2 are selected and they are propmtly greyed out, it kindly informs you that there is not enough memory to use this</t>
+  </si>
+  <si>
+    <t>Scoring changes - almost no bonus on tutorials, tons more on regular levels</t>
+  </si>
+  <si>
+    <t>when activating a reprogram square, the "abort" button needs to trigger into an execute button…</t>
   </si>
 </sst>
 </file>
@@ -773,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P140"/>
+  <dimension ref="A1:P128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F132" sqref="F132"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1128,6 +1185,9 @@
       <c r="A32" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B32" s="4">
+        <v>39904</v>
+      </c>
       <c r="C32" s="3" t="s">
         <v>63</v>
       </c>
@@ -1169,6 +1229,9 @@
       <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="B36" s="4">
+        <v>39905</v>
+      </c>
       <c r="C36" s="3" t="s">
         <v>90</v>
       </c>
@@ -1230,27 +1293,25 @@
     </row>
     <row r="42" spans="1:3" s="2" customFormat="1">
       <c r="B42" s="9"/>
+      <c r="C42" s="2" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="43" spans="1:3" s="2" customFormat="1">
       <c r="B43" s="9"/>
-    </row>
-    <row r="44" spans="1:3" s="6" customFormat="1">
-      <c r="B44" s="7"/>
-    </row>
-    <row r="45" spans="1:3" s="5" customFormat="1">
-      <c r="C45" s="5" t="s">
+      <c r="C43" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="2" customFormat="1">
+      <c r="B44" s="9"/>
+    </row>
+    <row r="45" spans="1:3" s="6" customFormat="1">
+      <c r="B45" s="7"/>
+    </row>
+    <row r="46" spans="1:3" s="5" customFormat="1">
+      <c r="C46" s="5" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" s="3" customFormat="1">
-      <c r="A46" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" s="4">
-        <v>39901</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="3" customFormat="1">
@@ -1258,151 +1319,163 @@
         <v>10</v>
       </c>
       <c r="B47" s="4">
-        <v>39902</v>
+        <v>39901</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="3" customFormat="1">
       <c r="A48" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B48" s="4">
+        <v>39902</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:16" s="3" customFormat="1">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="B49" s="4">
+        <v>39904</v>
+      </c>
       <c r="C49" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" s="3" customFormat="1">
+      <c r="A50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="4">
+        <v>39904</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="3" customFormat="1">
-      <c r="C50" s="3" t="s">
+    <row r="51" spans="1:16" s="3" customFormat="1">
+      <c r="A51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="4">
+        <v>39906</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="10" customFormat="1">
-      <c r="A51" s="10" t="s">
+    <row r="52" spans="1:16" s="3" customFormat="1">
+      <c r="A52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" s="10" customFormat="1">
+      <c r="A53" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C53" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="10" customFormat="1">
-      <c r="C52" s="10" t="s">
+    <row r="54" spans="1:16" s="10" customFormat="1">
+      <c r="C54" s="10" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" s="10" customFormat="1">
-      <c r="C53" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" s="10" customFormat="1">
-      <c r="A54" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:16" s="10" customFormat="1">
       <c r="C55" s="10" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:16" s="10" customFormat="1">
+      <c r="A56" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="C56" s="10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:16" s="10" customFormat="1">
       <c r="C57" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" s="10" customFormat="1">
+      <c r="C58" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" s="10" customFormat="1">
+      <c r="C59" s="10" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" s="10" customFormat="1">
-      <c r="D58" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" s="10" customFormat="1">
-      <c r="D59" s="10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:16" s="10" customFormat="1">
       <c r="D60" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" s="10" customFormat="1">
+      <c r="D61" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" s="10" customFormat="1">
+      <c r="D62" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="10" customFormat="1">
-      <c r="A61" s="10" t="s">
+    <row r="63" spans="1:16" s="10" customFormat="1">
+      <c r="A63" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C63" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-      <c r="O62" s="2"/>
-      <c r="P62" s="2"/>
-    </row>
     <row r="64" spans="1:16">
-      <c r="C64" s="5" t="s">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
+      <c r="P64" s="2"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="C66" s="5" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" s="3" customFormat="1">
-      <c r="A65" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B65" s="4">
-        <v>39888</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" s="3" customFormat="1">
-      <c r="A66" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B66" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:7" s="3" customFormat="1">
       <c r="A67" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B67" s="4">
-        <v>39882</v>
+        <v>39888</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:7" s="3" customFormat="1">
@@ -1410,10 +1483,10 @@
         <v>10</v>
       </c>
       <c r="B68" s="4">
-        <v>39887</v>
+        <v>39881</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="3" customFormat="1">
@@ -1421,10 +1494,10 @@
         <v>14</v>
       </c>
       <c r="B69" s="4">
-        <v>39901</v>
+        <v>39882</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="70" spans="1:7" s="3" customFormat="1">
@@ -1435,18 +1508,18 @@
         <v>39887</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" spans="1:7" s="3" customFormat="1">
       <c r="A71" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B71" s="4">
-        <v>39887</v>
+        <v>39901</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="3" customFormat="1">
@@ -1457,7 +1530,7 @@
         <v>39887</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="3" customFormat="1">
@@ -1468,7 +1541,7 @@
         <v>39887</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="74" spans="1:7" s="3" customFormat="1">
@@ -1476,68 +1549,73 @@
         <v>10</v>
       </c>
       <c r="B74" s="4">
-        <v>39902</v>
+        <v>39887</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" s="10" customFormat="1">
-      <c r="C75" s="10" t="s">
-        <v>102</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="3" customFormat="1">
+      <c r="A75" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="3" customFormat="1">
       <c r="A76" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B76" s="4">
-        <v>39905</v>
+        <v>39902</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" s="3" customFormat="1">
-      <c r="A77" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B77" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>77</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" s="10" customFormat="1">
+      <c r="C77" s="10" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:7" s="3" customFormat="1">
       <c r="A78" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B78" s="4">
-        <v>39902</v>
+        <v>39905</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:7" s="3" customFormat="1">
       <c r="A79" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B79" s="4">
-        <v>39907</v>
+        <v>39902</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" s="2" customFormat="1">
-      <c r="B80" s="9"/>
-      <c r="C80" s="2" t="s">
-        <v>95</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" s="3" customFormat="1">
+      <c r="A80" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="81" spans="1:4" s="3" customFormat="1">
@@ -1548,108 +1626,98 @@
         <v>39907</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:4" s="2" customFormat="1">
       <c r="B82" s="9"/>
       <c r="C82" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" s="2" customFormat="1">
-      <c r="B83" s="9"/>
-      <c r="C83" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" s="3" customFormat="1">
+      <c r="A83" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:4" s="2" customFormat="1">
       <c r="B84" s="9"/>
-      <c r="D84" s="2" t="s">
+      <c r="C84" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="2" customFormat="1">
+      <c r="B85" s="9"/>
+      <c r="C85" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" s="2" customFormat="1">
+      <c r="B86" s="9"/>
+      <c r="D86" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="1:4" s="3" customFormat="1">
-      <c r="A85" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B85" s="4">
+    <row r="87" spans="1:4" s="3" customFormat="1">
+      <c r="A87" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B87" s="4">
         <v>39907</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:4" s="8" customFormat="1"/>
-    <row r="89" spans="1:4">
-      <c r="C89" s="5" t="s">
+    <row r="88" spans="1:4" s="2" customFormat="1">
+      <c r="B88" s="9"/>
+      <c r="C88" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" s="8" customFormat="1"/>
+    <row r="92" spans="1:4">
+      <c r="C92" s="5" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="C90" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="C91" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="C92" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="C93" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="C94" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="C95" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="C96" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="C97" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
-      <c r="C96" s="5" t="s">
+    <row r="99" spans="1:5">
+      <c r="C99" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="97" spans="1:4" s="3" customFormat="1">
-      <c r="A97" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B97" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" s="3" customFormat="1">
-      <c r="A98" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B98" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" s="3" customFormat="1">
-      <c r="A99" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B99" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" s="3" customFormat="1">
+    <row r="100" spans="1:5" s="3" customFormat="1">
       <c r="A100" s="3" t="s">
         <v>10</v>
       </c>
@@ -1657,228 +1725,303 @@
         <v>39902</v>
       </c>
       <c r="C100" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" s="3" customFormat="1">
+      <c r="A101" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B101" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" s="3" customFormat="1">
+      <c r="A102" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B102" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" s="3" customFormat="1">
+      <c r="A103" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B103" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C103" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
-      <c r="C101" s="1" t="s">
+    <row r="104" spans="1:5">
+      <c r="C104" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="D102" s="1" t="s">
+    <row r="105" spans="1:5">
+      <c r="D105" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="C103" s="1" t="s">
+    <row r="106" spans="1:5">
+      <c r="C106" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
-      <c r="C104" s="1" t="s">
+    <row r="107" spans="1:5">
+      <c r="C107" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
-      <c r="C105" s="1" t="s">
+    <row r="108" spans="1:5">
+      <c r="C108" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
-      <c r="B121" s="1" t="s">
+    <row r="112" spans="1:5">
+      <c r="C112" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="E112" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
-      <c r="A126" s="1">
+    <row r="114" spans="1:12">
+      <c r="A114" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B114" s="1">
+        <v>1</v>
+      </c>
+      <c r="C114" s="1">
+        <v>56</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
+      <c r="A115" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B115" s="1">
         <v>7</v>
       </c>
+      <c r="C115" s="1">
+        <v>64</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
+      <c r="A116" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B116" s="1">
+        <v>6</v>
+      </c>
+      <c r="C116" s="1">
+        <v>78</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
+      <c r="A117" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B117" s="1">
+        <v>3</v>
+      </c>
+      <c r="C117" s="1">
+        <v>110</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="A118" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B118" s="1">
+        <v>11</v>
+      </c>
+      <c r="C118" s="1">
+        <v>128</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="A119" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B119" s="1">
+        <v>10</v>
+      </c>
+      <c r="C119" s="1">
+        <v>154</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="A120" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B120" s="1">
+        <v>8</v>
+      </c>
+      <c r="C120" s="1">
+        <v>156</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J120" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="A121" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B121" s="1">
+        <v>13</v>
+      </c>
+      <c r="C121" s="1">
+        <v>182</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B122" s="1">
+        <v>9</v>
+      </c>
+      <c r="C122" s="1">
+        <v>306</v>
+      </c>
+      <c r="D122" s="1">
+        <v>164</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
+      <c r="A123" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B123" s="1">
+        <v>14</v>
+      </c>
+      <c r="C123" s="1">
+        <v>318</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
+      <c r="A124" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B124" s="1">
+        <v>12</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
+      <c r="A125" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B125" s="1">
+        <v>15</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
+      <c r="A126" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="B126" s="1">
-        <v>64</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127" s="1">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C126" s="1">
+        <v>92</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L126" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
+      <c r="A127" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="B127" s="1">
-        <v>78</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
-      <c r="A128" s="1">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="C127" s="1">
+        <v>88</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L127" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
+      <c r="A128" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="B128" s="1">
-        <v>154</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="129" spans="1:12">
-      <c r="A129" s="1">
-        <v>8</v>
-      </c>
-      <c r="B129" s="1">
+        <v>2</v>
+      </c>
+      <c r="C128" s="1">
         <v>156</v>
       </c>
-      <c r="F129" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H129" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I129" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="130" spans="1:12">
-      <c r="A130" s="1">
-        <v>9</v>
-      </c>
-      <c r="B130" s="1">
-        <v>306</v>
-      </c>
-      <c r="C130" s="1">
-        <v>164</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12">
-      <c r="A131" s="1">
-        <v>1</v>
-      </c>
-      <c r="B131" s="1">
-        <v>56</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12">
-      <c r="A132" s="1">
-        <v>11</v>
-      </c>
-      <c r="B132" s="1">
-        <v>128</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12">
-      <c r="A133" s="1">
-        <v>12</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="134" spans="1:12">
-      <c r="A134" s="1">
-        <v>13</v>
-      </c>
-      <c r="B134" s="1">
-        <v>182</v>
-      </c>
-      <c r="F134" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12">
-      <c r="A135" s="1">
-        <v>14</v>
-      </c>
-      <c r="B135" s="1">
-        <v>318</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L135" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="136" spans="1:12">
-      <c r="A136" s="1">
-        <v>15</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="137" spans="1:12">
-      <c r="A137" s="1">
-        <v>2</v>
-      </c>
-      <c r="B137" s="1">
-        <v>156</v>
-      </c>
-      <c r="F137" s="1" t="s">
+      <c r="G128" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="138" spans="1:12">
-      <c r="A138" s="1">
-        <v>3</v>
-      </c>
-      <c r="B138" s="1">
-        <v>110</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="139" spans="1:12">
-      <c r="A139" s="1">
-        <v>4</v>
-      </c>
-      <c r="B139" s="1">
-        <v>88</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K139" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="140" spans="1:12">
-      <c r="A140" s="1">
-        <v>5</v>
-      </c>
-      <c r="B140" s="1">
-        <v>92</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K140" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A126:G130">
-    <sortCondition ref="B126:B130"/>
+  <sortState ref="A126:L140">
+    <sortCondition ref="C126:C140"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
level info is now shown in game
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="144">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -442,6 +442,12 @@
   </si>
   <si>
     <t>when activating a reprogram square, the "abort" button needs to trigger into an execute button…</t>
+  </si>
+  <si>
+    <t>current processed command is not showing the sub as being processed, but instead the previous command being processed</t>
+  </si>
+  <si>
+    <t>if inside a sub, it should highlight that sub in the main command list</t>
   </si>
 </sst>
 </file>
@@ -830,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P128"/>
+  <dimension ref="A1:P131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1291,9 +1297,14 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1">
-      <c r="B42" s="9"/>
-      <c r="C42" s="2" t="s">
+    <row r="42" spans="1:3" s="3" customFormat="1">
+      <c r="A42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1306,23 +1317,15 @@
     <row r="44" spans="1:3" s="2" customFormat="1">
       <c r="B44" s="9"/>
     </row>
-    <row r="45" spans="1:3" s="6" customFormat="1">
-      <c r="B45" s="7"/>
-    </row>
-    <row r="46" spans="1:3" s="5" customFormat="1">
-      <c r="C46" s="5" t="s">
+    <row r="45" spans="1:3" s="2" customFormat="1">
+      <c r="B45" s="9"/>
+    </row>
+    <row r="46" spans="1:3" s="6" customFormat="1">
+      <c r="B46" s="7"/>
+    </row>
+    <row r="47" spans="1:3" s="5" customFormat="1">
+      <c r="C47" s="5" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" s="3" customFormat="1">
-      <c r="A47" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47" s="4">
-        <v>39901</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="3" customFormat="1">
@@ -1330,24 +1333,24 @@
         <v>10</v>
       </c>
       <c r="B48" s="4">
+        <v>39901</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="3" customFormat="1">
+      <c r="A49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="4">
         <v>39902</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="3" customFormat="1">
-      <c r="A49" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" s="4">
-        <v>39904</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" s="3" customFormat="1">
+    <row r="50" spans="1:4" s="3" customFormat="1">
       <c r="A50" s="3" t="s">
         <v>7</v>
       </c>
@@ -1355,185 +1358,185 @@
         <v>39904</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="3" customFormat="1">
+      <c r="A51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="4">
+        <v>39904</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="3" customFormat="1">
-      <c r="A51" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B51" s="4">
+    <row r="52" spans="1:4" s="3" customFormat="1">
+      <c r="A52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="4">
         <v>39906</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="3" customFormat="1">
-      <c r="A52" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B52" s="4">
+    <row r="53" spans="1:4" s="3" customFormat="1">
+      <c r="A53" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="4">
         <v>39908</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="10" customFormat="1">
-      <c r="A53" s="10" t="s">
+    <row r="54" spans="1:4" s="10" customFormat="1">
+      <c r="A54" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C54" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="10" customFormat="1">
-      <c r="C54" s="10" t="s">
+    <row r="55" spans="1:4" s="10" customFormat="1">
+      <c r="C55" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="10" customFormat="1">
-      <c r="C55" s="10" t="s">
+    <row r="56" spans="1:4" s="10" customFormat="1">
+      <c r="C56" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="10" customFormat="1">
-      <c r="A56" s="10" t="s">
+    <row r="57" spans="1:4" s="10" customFormat="1">
+      <c r="A57" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C57" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="10" customFormat="1">
-      <c r="C57" s="10" t="s">
+    <row r="58" spans="1:4" s="10" customFormat="1">
+      <c r="C58" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="10" customFormat="1">
-      <c r="C58" s="10" t="s">
+    <row r="59" spans="1:4" s="10" customFormat="1">
+      <c r="C59" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:16" s="10" customFormat="1">
-      <c r="C59" s="10" t="s">
+    <row r="60" spans="1:4" s="10" customFormat="1">
+      <c r="C60" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="10" customFormat="1">
-      <c r="D60" s="10" t="s">
+    <row r="61" spans="1:4" s="10" customFormat="1">
+      <c r="D61" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="10" customFormat="1">
-      <c r="D61" s="10" t="s">
+    <row r="62" spans="1:4" s="10" customFormat="1">
+      <c r="D62" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:16" s="10" customFormat="1">
-      <c r="D62" s="10" t="s">
+    <row r="63" spans="1:4" s="10" customFormat="1">
+      <c r="D63" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:16" s="10" customFormat="1">
-      <c r="A63" s="10" t="s">
+    <row r="64" spans="1:4" s="10" customFormat="1">
+      <c r="A64" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C64" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
-      <c r="M64" s="2"/>
-      <c r="N64" s="2"/>
-      <c r="O64" s="2"/>
-      <c r="P64" s="2"/>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="C66" s="5" t="s">
+    <row r="65" spans="1:16">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2"/>
+    </row>
+    <row r="67" spans="1:16">
+      <c r="C67" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="3" customFormat="1">
-      <c r="A67" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67" s="4">
+    <row r="68" spans="1:16" s="3" customFormat="1">
+      <c r="A68" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="4">
         <v>39888</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="3" customFormat="1">
-      <c r="A68" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" s="4">
+    <row r="69" spans="1:16" s="3" customFormat="1">
+      <c r="A69" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" s="4">
         <v>39881</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="3" customFormat="1">
-      <c r="A69" s="3" t="s">
+    <row r="70" spans="1:16" s="3" customFormat="1">
+      <c r="A70" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B70" s="4">
         <v>39882</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="3" customFormat="1">
-      <c r="A70" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B70" s="4">
+    <row r="71" spans="1:16" s="3" customFormat="1">
+      <c r="A71" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" s="4">
         <v>39887</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="3" customFormat="1">
-      <c r="A71" s="3" t="s">
+    <row r="72" spans="1:16" s="3" customFormat="1">
+      <c r="A72" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B71" s="4">
+      <c r="B72" s="4">
         <v>39901</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="3" customFormat="1">
-      <c r="A72" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B72" s="4">
-        <v>39887</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" s="3" customFormat="1">
+    <row r="73" spans="1:16" s="3" customFormat="1">
       <c r="A73" s="3" t="s">
         <v>10</v>
       </c>
@@ -1541,10 +1544,10 @@
         <v>39887</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" s="3" customFormat="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" s="3" customFormat="1">
       <c r="A74" s="3" t="s">
         <v>10</v>
       </c>
@@ -1552,10 +1555,10 @@
         <v>39887</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" s="3" customFormat="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" s="3" customFormat="1">
       <c r="A75" s="3" t="s">
         <v>10</v>
       </c>
@@ -1563,59 +1566,59 @@
         <v>39887</v>
       </c>
       <c r="C75" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" s="3" customFormat="1">
+      <c r="A76" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B76" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="3" customFormat="1">
-      <c r="A76" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B76" s="4">
+    <row r="77" spans="1:16" s="3" customFormat="1">
+      <c r="A77" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" s="4">
         <v>39902</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="10" customFormat="1">
-      <c r="C77" s="10" t="s">
+    <row r="78" spans="1:16" s="10" customFormat="1">
+      <c r="C78" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="3" customFormat="1">
-      <c r="A78" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B78" s="4">
-        <v>39905</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" s="3" customFormat="1">
+    <row r="79" spans="1:16" s="3" customFormat="1">
       <c r="A79" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B79" s="4">
-        <v>39902</v>
+        <v>39905</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" s="3" customFormat="1">
+        <v>76</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" s="3" customFormat="1">
       <c r="A80" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B80" s="4">
         <v>39902</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:4" s="3" customFormat="1">
@@ -1623,134 +1626,124 @@
         <v>10</v>
       </c>
       <c r="B81" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" s="3" customFormat="1">
+      <c r="A82" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82" s="4">
         <v>39907</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C82" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="82" spans="1:4" s="2" customFormat="1">
-      <c r="B82" s="9"/>
-      <c r="C82" s="2" t="s">
+    <row r="83" spans="1:4" s="2" customFormat="1">
+      <c r="B83" s="9"/>
+      <c r="C83" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:4" s="3" customFormat="1">
-      <c r="A83" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B83" s="4">
+    <row r="84" spans="1:4" s="3" customFormat="1">
+      <c r="A84" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B84" s="4">
         <v>39907</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" s="2" customFormat="1">
-      <c r="B84" s="9"/>
-      <c r="C84" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="85" spans="1:4" s="2" customFormat="1">
       <c r="B85" s="9"/>
       <c r="C85" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:4" s="2" customFormat="1">
       <c r="B86" s="9"/>
-      <c r="D86" s="2" t="s">
+      <c r="C86" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" s="2" customFormat="1">
+      <c r="B87" s="9"/>
+      <c r="D87" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="87" spans="1:4" s="3" customFormat="1">
-      <c r="A87" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B87" s="4">
+    <row r="88" spans="1:4" s="3" customFormat="1">
+      <c r="A88" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88" s="4">
         <v>39907</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:4" s="2" customFormat="1">
-      <c r="B88" s="9"/>
-      <c r="C88" s="2" t="s">
+    <row r="89" spans="1:4" s="2" customFormat="1">
+      <c r="B89" s="9"/>
+      <c r="C89" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="1:4" s="8" customFormat="1"/>
-    <row r="92" spans="1:4">
-      <c r="C92" s="5" t="s">
+    <row r="90" spans="1:4" s="2" customFormat="1">
+      <c r="B90" s="9"/>
+      <c r="C90" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" s="2" customFormat="1">
+      <c r="B91" s="9"/>
+      <c r="D91" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" s="8" customFormat="1"/>
+    <row r="95" spans="1:4">
+      <c r="C95" s="5" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="C93" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="C94" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="C95" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="C96" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="C97" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="C98" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="C99" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
-      <c r="C97" s="1" t="s">
+    <row r="100" spans="1:4">
+      <c r="C100" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
-      <c r="C99" s="5" t="s">
+    <row r="102" spans="1:4">
+      <c r="C102" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="3" customFormat="1">
-      <c r="A100" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B100" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" s="3" customFormat="1">
-      <c r="A101" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B101" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" s="3" customFormat="1">
-      <c r="A102" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B102" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" s="3" customFormat="1">
+    <row r="103" spans="1:4" s="3" customFormat="1">
       <c r="A103" s="3" t="s">
         <v>10</v>
       </c>
@@ -1758,264 +1751,297 @@
         <v>39902</v>
       </c>
       <c r="C103" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" s="3" customFormat="1">
+      <c r="A104" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" s="3" customFormat="1">
+      <c r="A105" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B105" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" s="3" customFormat="1">
+      <c r="A106" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B106" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
-      <c r="C104" s="1" t="s">
+    <row r="107" spans="1:4">
+      <c r="C107" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
-      <c r="D105" s="1" t="s">
+    <row r="108" spans="1:4">
+      <c r="D108" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
-      <c r="C106" s="1" t="s">
+    <row r="109" spans="1:4">
+      <c r="C109" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
-      <c r="C107" s="1" t="s">
+    <row r="110" spans="1:4">
+      <c r="C110" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
-      <c r="C108" s="1" t="s">
+    <row r="111" spans="1:4">
+      <c r="C111" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
-      <c r="C112" s="1" t="s">
+    <row r="115" spans="1:10">
+      <c r="C115" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E112" s="1" t="s">
+      <c r="E115" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="114" spans="1:12">
-      <c r="A114" s="1" t="s">
+    <row r="117" spans="1:10">
+      <c r="A117" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B117" s="1">
         <v>1</v>
       </c>
-      <c r="C114" s="1">
+      <c r="C117" s="1">
         <v>56</v>
       </c>
-      <c r="G114" s="1" t="s">
+      <c r="G117" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="115" spans="1:12">
-      <c r="A115" s="1" t="s">
+    <row r="118" spans="1:10">
+      <c r="A118" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B118" s="1">
         <v>7</v>
       </c>
-      <c r="C115" s="1">
+      <c r="C118" s="1">
         <v>64</v>
       </c>
-      <c r="G115" s="1" t="s">
+      <c r="G118" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="116" spans="1:12">
-      <c r="A116" s="1" t="s">
+    <row r="119" spans="1:10">
+      <c r="A119" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B119" s="1">
         <v>6</v>
       </c>
-      <c r="C116" s="1">
+      <c r="C119" s="1">
         <v>78</v>
       </c>
-      <c r="G116" s="1" t="s">
+      <c r="G119" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
-      <c r="A117" s="1" t="s">
+    <row r="120" spans="1:10">
+      <c r="A120" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B117" s="1">
+      <c r="B120" s="1">
         <v>3</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C120" s="1">
         <v>110</v>
       </c>
-      <c r="E117" s="1" t="s">
+      <c r="E120" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G117" s="1" t="s">
+      <c r="G120" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="118" spans="1:12">
-      <c r="A118" s="1" t="s">
+    <row r="121" spans="1:10">
+      <c r="A121" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B118" s="1">
+      <c r="B121" s="1">
         <v>11</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C121" s="1">
         <v>128</v>
       </c>
-      <c r="G118" s="1" t="s">
+      <c r="G121" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
-      <c r="A119" s="1" t="s">
+    <row r="122" spans="1:10">
+      <c r="A122" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B119" s="1">
-        <v>10</v>
-      </c>
-      <c r="C119" s="1">
+      <c r="B122" s="1">
+        <v>10</v>
+      </c>
+      <c r="C122" s="1">
         <v>154</v>
       </c>
-      <c r="G119" s="1" t="s">
+      <c r="G122" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="120" spans="1:12">
-      <c r="A120" s="1" t="s">
+    <row r="123" spans="1:10">
+      <c r="A123" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B120" s="1">
+      <c r="B123" s="1">
         <v>8</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C123" s="1">
         <v>156</v>
       </c>
-      <c r="G120" s="1" t="s">
+      <c r="G123" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I120" s="1" t="s">
+      <c r="I123" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="J120" s="1" t="s">
+      <c r="J123" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
-      <c r="A121" s="1" t="s">
+    <row r="124" spans="1:10">
+      <c r="A124" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B121" s="1">
+      <c r="B124" s="1">
         <v>13</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C124" s="1">
         <v>182</v>
       </c>
-      <c r="G121" s="1" t="s">
+      <c r="G124" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="122" spans="1:12">
-      <c r="A122" s="1" t="s">
+    <row r="125" spans="1:10">
+      <c r="A125" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B125" s="1">
         <v>9</v>
       </c>
-      <c r="C122" s="1">
+      <c r="C125" s="1">
         <v>306</v>
       </c>
-      <c r="D122" s="1">
+      <c r="D125" s="1">
         <v>164</v>
       </c>
-      <c r="G122" s="1" t="s">
+      <c r="G125" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="123" spans="1:12">
-      <c r="A123" s="1" t="s">
+    <row r="126" spans="1:10">
+      <c r="A126" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B126" s="1">
         <v>14</v>
       </c>
-      <c r="C123" s="1">
+      <c r="C126" s="1">
         <v>318</v>
       </c>
-      <c r="G123" s="1" t="s">
+      <c r="G126" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
-      <c r="A124" s="1" t="s">
+    <row r="127" spans="1:10">
+      <c r="A127" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B127" s="1">
         <v>12</v>
       </c>
-      <c r="G124" s="1" t="s">
+      <c r="G127" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
-      <c r="A125" s="1" t="s">
+    <row r="128" spans="1:10">
+      <c r="A128" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B125" s="1">
+      <c r="B128" s="1">
         <v>15</v>
       </c>
-      <c r="G125" s="1" t="s">
+      <c r="G128" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="126" spans="1:12">
-      <c r="A126" s="1" t="s">
+    <row r="129" spans="1:12">
+      <c r="A129" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B126" s="1">
+      <c r="B129" s="1">
         <v>5</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C129" s="1">
         <v>92</v>
       </c>
-      <c r="G126" s="1" t="s">
+      <c r="G129" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="L126" s="1" t="s">
+      <c r="L129" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="127" spans="1:12">
-      <c r="A127" s="1" t="s">
+    <row r="130" spans="1:12">
+      <c r="A130" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B127" s="1">
+      <c r="B130" s="1">
         <v>4</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C130" s="1">
         <v>88</v>
       </c>
-      <c r="G127" s="1" t="s">
+      <c r="G130" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="L127" s="1" t="s">
+      <c r="L130" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="128" spans="1:12">
-      <c r="A128" s="1" t="s">
+    <row r="131" spans="1:12">
+      <c r="A131" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B128" s="1">
+      <c r="B131" s="1">
         <v>2</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C131" s="1">
         <v>156</v>
       </c>
-      <c r="G128" s="1" t="s">
+      <c r="G131" s="1" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
't' in game now insta-toggles all targets of the switch square you are standing in, it doesn't care which way you are facing anymore either, yay for debug code
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="150">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -454,6 +454,18 @@
   </si>
   <si>
     <t>teleporters should not hijack the graphics engine</t>
+  </si>
+  <si>
+    <t>when you hit save game in pause menu, it needs to fire a click ok state</t>
+  </si>
+  <si>
+    <t>nuke save game button from options menu</t>
+  </si>
+  <si>
+    <t>update all map mini images to match the current maps, AFTER all the maps have been cleaned up/tweaked</t>
+  </si>
+  <si>
+    <t>tutorial map 7 - remove the two solid blocks</t>
   </si>
 </sst>
 </file>
@@ -836,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P131"/>
+  <dimension ref="A1:P137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1319,216 +1331,201 @@
     </row>
     <row r="45" spans="1:3" s="2" customFormat="1">
       <c r="B45" s="8"/>
-    </row>
-    <row r="46" spans="1:3" s="6" customFormat="1">
-      <c r="B46" s="7"/>
-    </row>
-    <row r="47" spans="1:3" s="5" customFormat="1">
-      <c r="C47" s="5" t="s">
+      <c r="C45" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="2" customFormat="1">
+      <c r="B46" s="8"/>
+      <c r="C46" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="2" customFormat="1">
+      <c r="B47" s="8"/>
+    </row>
+    <row r="48" spans="1:3" s="2" customFormat="1">
+      <c r="B48" s="8"/>
+      <c r="C48" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="6" customFormat="1">
+      <c r="B49" s="7"/>
+    </row>
+    <row r="50" spans="1:3" s="5" customFormat="1">
+      <c r="C50" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="3" customFormat="1">
-      <c r="A48" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B48" s="4">
+    <row r="51" spans="1:3" s="3" customFormat="1">
+      <c r="A51" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="4">
         <v>39901</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="3" customFormat="1">
-      <c r="A49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B49" s="4">
+    <row r="52" spans="1:3" s="3" customFormat="1">
+      <c r="A52" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="4">
         <v>39902</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:4" s="3" customFormat="1">
-      <c r="A50" s="3" t="s">
+    <row r="53" spans="1:3" s="3" customFormat="1">
+      <c r="A53" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B53" s="4">
         <v>39904</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1">
-      <c r="A51" s="3" t="s">
+    <row r="54" spans="1:3" s="3" customFormat="1">
+      <c r="A54" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B54" s="4">
         <v>39904</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:4" s="3" customFormat="1">
-      <c r="A52" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B52" s="4">
+    <row r="55" spans="1:3" s="3" customFormat="1">
+      <c r="A55" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="4">
         <v>39906</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="3" customFormat="1">
-      <c r="A53" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B53" s="4">
+    <row r="56" spans="1:3" s="3" customFormat="1">
+      <c r="A56" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" s="4">
         <v>39908</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:4" s="9" customFormat="1">
-      <c r="A54" s="9" t="s">
+    <row r="57" spans="1:3" s="9" customFormat="1">
+      <c r="A57" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C57" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:4" s="3" customFormat="1">
-      <c r="A55" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B55" s="4">
+    <row r="58" spans="1:3" s="3" customFormat="1">
+      <c r="A58" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" s="4">
         <v>39908</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="9" customFormat="1">
-      <c r="C56" s="9" t="s">
+    <row r="59" spans="1:3" s="9" customFormat="1">
+      <c r="C59" s="9" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="57" spans="1:4" s="9" customFormat="1">
-      <c r="C57" s="9" t="s">
+    <row r="60" spans="1:3" s="9" customFormat="1">
+      <c r="C60" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" s="9" customFormat="1">
-      <c r="A58" s="9" t="s">
+    <row r="61" spans="1:3" s="9" customFormat="1">
+      <c r="A61" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C61" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="9" customFormat="1">
-      <c r="C59" s="9" t="s">
+    <row r="62" spans="1:3" s="9" customFormat="1">
+      <c r="C62" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="9" customFormat="1">
-      <c r="C60" s="9" t="s">
+    <row r="63" spans="1:3" s="9" customFormat="1">
+      <c r="C63" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="9" customFormat="1">
-      <c r="C61" s="9" t="s">
+    <row r="64" spans="1:3" s="9" customFormat="1">
+      <c r="C64" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:4" s="9" customFormat="1">
-      <c r="D62" s="9" t="s">
+    <row r="65" spans="1:16" s="9" customFormat="1">
+      <c r="D65" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:4" s="9" customFormat="1">
-      <c r="D63" s="9" t="s">
+    <row r="66" spans="1:16" s="9" customFormat="1">
+      <c r="D66" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:4" s="9" customFormat="1">
-      <c r="D64" s="9" t="s">
+    <row r="67" spans="1:16" s="9" customFormat="1">
+      <c r="D67" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="9" customFormat="1">
-      <c r="A65" s="9" t="s">
+    <row r="68" spans="1:16" s="9" customFormat="1">
+      <c r="A68" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C68" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="9" customFormat="1">
-      <c r="B66" s="10"/>
-      <c r="C66" s="9" t="s">
+    <row r="69" spans="1:16" s="9" customFormat="1">
+      <c r="B69" s="10"/>
+      <c r="C69" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
-      <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
-      <c r="O67" s="2"/>
-      <c r="P67" s="2"/>
-    </row>
-    <row r="69" spans="1:16">
-      <c r="C69" s="5" t="s">
+    <row r="70" spans="1:16">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2"/>
+      <c r="P70" s="2"/>
+    </row>
+    <row r="72" spans="1:16">
+      <c r="C72" s="5" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" s="3" customFormat="1">
-      <c r="A70" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B70" s="4">
-        <v>39888</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" s="3" customFormat="1">
-      <c r="A71" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B71" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" s="3" customFormat="1">
-      <c r="A72" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B72" s="4">
-        <v>39882</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="73" spans="1:16" s="3" customFormat="1">
@@ -1536,32 +1533,32 @@
         <v>9</v>
       </c>
       <c r="B73" s="4">
-        <v>39887</v>
+        <v>39888</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="74" spans="1:16" s="3" customFormat="1">
       <c r="A74" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B74" s="4">
-        <v>39901</v>
+        <v>39881</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:16" s="3" customFormat="1">
       <c r="A75" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B75" s="4">
-        <v>39887</v>
+        <v>39882</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="76" spans="1:16" s="3" customFormat="1">
@@ -1572,18 +1569,18 @@
         <v>39887</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:16" s="3" customFormat="1">
       <c r="A77" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B77" s="4">
-        <v>39887</v>
+        <v>39901</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="1:16" s="3" customFormat="1">
@@ -1594,7 +1591,7 @@
         <v>39887</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="79" spans="1:16" s="3" customFormat="1">
@@ -1602,68 +1599,73 @@
         <v>9</v>
       </c>
       <c r="B79" s="4">
-        <v>39902</v>
+        <v>39887</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" s="9" customFormat="1">
-      <c r="C80" s="9" t="s">
-        <v>101</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" s="3" customFormat="1">
+      <c r="A80" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B80" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="81" spans="1:7" s="3" customFormat="1">
       <c r="A81" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B81" s="4">
-        <v>39905</v>
+        <v>39887</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="1:7" s="3" customFormat="1">
       <c r="A82" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B82" s="4">
         <v>39902</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" s="3" customFormat="1">
-      <c r="A83" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B83" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" s="9" customFormat="1">
+      <c r="C83" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="3" customFormat="1">
       <c r="A84" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B84" s="4">
-        <v>39907</v>
+        <v>39905</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="2" customFormat="1">
-      <c r="B85" s="8"/>
-      <c r="C85" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="3" customFormat="1">
+      <c r="A85" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="86" spans="1:7" s="3" customFormat="1">
@@ -1671,125 +1673,120 @@
         <v>9</v>
       </c>
       <c r="B86" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="3" customFormat="1">
+      <c r="A87" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" s="4">
         <v>39907</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" s="2" customFormat="1">
-      <c r="B87" s="8"/>
-      <c r="C87" s="2" t="s">
-        <v>97</v>
+      <c r="C87" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:7" s="2" customFormat="1">
       <c r="B88" s="8"/>
       <c r="C88" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" s="2" customFormat="1">
-      <c r="B89" s="8"/>
-      <c r="D89" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" s="3" customFormat="1">
-      <c r="A90" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B90" s="4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" s="3" customFormat="1">
+      <c r="A89" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B89" s="4">
         <v>39907</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>99</v>
+      <c r="C89" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" s="2" customFormat="1">
+      <c r="B90" s="8"/>
+      <c r="C90" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="2" customFormat="1">
       <c r="B91" s="8"/>
       <c r="C91" s="2" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
     </row>
     <row r="92" spans="1:7" s="2" customFormat="1">
       <c r="B92" s="8"/>
-      <c r="C92" s="2" t="s">
+      <c r="D92" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" s="3" customFormat="1">
+      <c r="A93" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B93" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" s="2" customFormat="1">
+      <c r="B94" s="8"/>
+      <c r="C94" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" s="2" customFormat="1">
+      <c r="B95" s="8"/>
+      <c r="C95" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="2" customFormat="1">
-      <c r="B93" s="8"/>
-      <c r="D93" s="2" t="s">
+    <row r="96" spans="1:7" s="2" customFormat="1">
+      <c r="B96" s="8"/>
+      <c r="D96" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
-      <c r="C95" s="5" t="s">
+    <row r="98" spans="1:4">
+      <c r="C98" s="5" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7">
-      <c r="C96" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="C97" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="C98" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="C99" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="C100" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="C101" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="C102" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="C103" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="C102" s="5" t="s">
+    <row r="105" spans="1:4">
+      <c r="C105" s="5" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" s="3" customFormat="1">
-      <c r="A103" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B103" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" s="3" customFormat="1">
-      <c r="A104" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B104" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" s="3" customFormat="1">
-      <c r="A105" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B105" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="106" spans="1:4" s="3" customFormat="1">
@@ -1800,265 +1797,303 @@
         <v>39902</v>
       </c>
       <c r="C106" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" s="3" customFormat="1">
+      <c r="A107" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B107" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" s="3" customFormat="1">
+      <c r="A108" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B108" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" s="3" customFormat="1">
+      <c r="A109" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B109" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="C107" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="D108" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
-      <c r="C109" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="C110" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="D111" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="C112" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="C113" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
-      <c r="C111" s="1" t="s">
+    <row r="114" spans="1:10">
+      <c r="C114" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
-      <c r="C115" s="1" t="s">
+    <row r="118" spans="1:10">
+      <c r="C118" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="E118" s="1" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10">
-      <c r="A117" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B117" s="1">
-        <v>1</v>
-      </c>
-      <c r="C117" s="1">
-        <v>56</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10">
-      <c r="A118" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B118" s="1">
-        <v>7</v>
-      </c>
-      <c r="C118" s="1">
-        <v>64</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10">
-      <c r="A119" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B119" s="1">
-        <v>6</v>
-      </c>
-      <c r="C119" s="1">
-        <v>78</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="120" spans="1:10">
       <c r="A120" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B120" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C120" s="1">
-        <v>110</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:10">
       <c r="A121" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B121" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C121" s="1">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="122" spans="1:10">
       <c r="A122" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B122" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C122" s="1">
-        <v>154</v>
+        <v>64</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="123" spans="1:10">
       <c r="A123" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B123" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C123" s="1">
-        <v>156</v>
+        <v>110</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I123" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="J123" s="1" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
     </row>
     <row r="124" spans="1:10">
       <c r="A124" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B124" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C124" s="1">
-        <v>182</v>
+        <v>128</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="125" spans="1:10">
       <c r="A125" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B125" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C125" s="1">
-        <v>306</v>
-      </c>
-      <c r="D125" s="1">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:10">
       <c r="A126" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B126" s="1">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C126" s="1">
-        <v>318</v>
+        <v>156</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="127" spans="1:10">
       <c r="A127" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B127" s="1">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C127" s="1">
+        <v>182</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="128" spans="1:10">
       <c r="A128" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B128" s="1">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="C128" s="1">
+        <v>306</v>
+      </c>
+      <c r="D128" s="1">
+        <v>164</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="129" spans="1:12">
       <c r="A129" s="1" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B129" s="1">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C129" s="1">
-        <v>92</v>
+        <v>318</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L129" s="1" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B130" s="1">
-        <v>4</v>
-      </c>
-      <c r="C130" s="1">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L130" s="1" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="131" spans="1:12">
       <c r="A131" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B131" s="1">
+        <v>15</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
+      <c r="A132" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B132" s="1">
+        <v>5</v>
+      </c>
+      <c r="C132" s="1">
+        <v>92</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L132" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
+      <c r="A133" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B133" s="1">
+        <v>4</v>
+      </c>
+      <c r="C133" s="1">
+        <v>88</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L133" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
+      <c r="A134" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B131" s="1">
+      <c r="B134" s="1">
         <v>2</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C134" s="1">
         <v>156</v>
       </c>
-      <c r="G131" s="1" t="s">
+      <c r="G134" s="1" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
+      <c r="B137" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
massive map updates yay everybody playtest the maps and make sure they are all beatable
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="151">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -369,9 +369,6 @@
     <t>not very complex, fairly easy as well - lots of random extra stuff not related to finishing the map</t>
   </si>
   <si>
-    <t>could probably lose the reprogram square, additionally, not sure if intended, but the last two switches can be skipped entirely, may want to disable jump on this map, or make some reason for the switches</t>
-  </si>
-  <si>
     <t>very linear, interesting figuring out what does what</t>
   </si>
   <si>
@@ -466,6 +463,12 @@
   </si>
   <si>
     <t>tutorial map 7 - remove the two solid blocks</t>
+  </si>
+  <si>
+    <t>make reset button, reset zoom as well</t>
+  </si>
+  <si>
+    <t>needs rebalance</t>
   </si>
 </sst>
 </file>
@@ -848,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P137"/>
+  <dimension ref="A1:P139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1317,13 +1320,13 @@
         <v>39908</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="2" customFormat="1">
       <c r="B43" s="8"/>
       <c r="C43" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="2" customFormat="1">
@@ -1332,13 +1335,13 @@
     <row r="45" spans="1:3" s="2" customFormat="1">
       <c r="B45" s="8"/>
       <c r="C45" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="2" customFormat="1">
       <c r="B46" s="8"/>
       <c r="C46" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="2" customFormat="1">
@@ -1347,89 +1350,79 @@
     <row r="48" spans="1:3" s="2" customFormat="1">
       <c r="B48" s="8"/>
       <c r="C48" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="6" customFormat="1">
-      <c r="B49" s="7"/>
-    </row>
-    <row r="50" spans="1:3" s="5" customFormat="1">
-      <c r="C50" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="2" customFormat="1">
+      <c r="B49" s="8"/>
+      <c r="C49" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="2" customFormat="1">
+      <c r="B50" s="8"/>
+    </row>
+    <row r="51" spans="1:3" s="6" customFormat="1">
+      <c r="B51" s="7"/>
+    </row>
+    <row r="52" spans="1:3" s="5" customFormat="1">
+      <c r="C52" s="5" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" s="3" customFormat="1">
-      <c r="A51" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B51" s="4">
-        <v>39901</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" s="3" customFormat="1">
-      <c r="A52" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B52" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="3" customFormat="1">
       <c r="A53" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B53" s="4">
-        <v>39904</v>
+        <v>39901</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="3" customFormat="1">
       <c r="A54" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B54" s="4">
-        <v>39904</v>
+        <v>39902</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="3" customFormat="1">
       <c r="A55" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B55" s="4">
-        <v>39906</v>
+        <v>39904</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="3" customFormat="1">
       <c r="A56" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B56" s="4">
-        <v>39908</v>
+        <v>39904</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" s="9" customFormat="1">
-      <c r="A57" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="3" customFormat="1">
+      <c r="A57" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="4">
+        <v>39906</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="3" customFormat="1">
@@ -1440,125 +1433,122 @@
         <v>39908</v>
       </c>
       <c r="C58" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="9" customFormat="1">
+      <c r="A59" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="3" customFormat="1">
+      <c r="A60" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="9" customFormat="1">
+      <c r="C61" s="9" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" s="9" customFormat="1">
-      <c r="C59" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" s="9" customFormat="1">
-      <c r="C60" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="9" customFormat="1">
-      <c r="A61" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="9" customFormat="1">
       <c r="C62" s="9" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="9" customFormat="1">
+      <c r="A63" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="C63" s="9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="9" customFormat="1">
       <c r="C64" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" s="9" customFormat="1">
+      <c r="C65" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" s="9" customFormat="1">
+      <c r="C66" s="9" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" s="9" customFormat="1">
-      <c r="D65" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" s="9" customFormat="1">
-      <c r="D66" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:16" s="9" customFormat="1">
       <c r="D67" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" s="9" customFormat="1">
+      <c r="D68" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" s="9" customFormat="1">
+      <c r="D69" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="9" customFormat="1">
-      <c r="A68" s="9" t="s">
+    <row r="70" spans="1:16" s="9" customFormat="1">
+      <c r="A70" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C70" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="9" customFormat="1">
-      <c r="B69" s="10"/>
-      <c r="C69" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-      <c r="K70" s="2"/>
-      <c r="L70" s="2"/>
-      <c r="M70" s="2"/>
-      <c r="N70" s="2"/>
-      <c r="O70" s="2"/>
-      <c r="P70" s="2"/>
+    <row r="71" spans="1:16" s="9" customFormat="1">
+      <c r="B71" s="10"/>
+      <c r="C71" s="9" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="72" spans="1:16">
-      <c r="C72" s="5" t="s">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+      <c r="N72" s="2"/>
+      <c r="O72" s="2"/>
+      <c r="P72" s="2"/>
+    </row>
+    <row r="74" spans="1:16">
+      <c r="C74" s="5" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" s="3" customFormat="1">
-      <c r="A73" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B73" s="4">
-        <v>39888</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" s="3" customFormat="1">
-      <c r="A74" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B74" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:16" s="3" customFormat="1">
       <c r="A75" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B75" s="4">
-        <v>39882</v>
+        <v>39888</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:16" s="3" customFormat="1">
@@ -1566,10 +1556,10 @@
         <v>9</v>
       </c>
       <c r="B76" s="4">
-        <v>39887</v>
+        <v>39881</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="77" spans="1:16" s="3" customFormat="1">
@@ -1577,10 +1567,10 @@
         <v>13</v>
       </c>
       <c r="B77" s="4">
-        <v>39901</v>
+        <v>39882</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="1:16" s="3" customFormat="1">
@@ -1591,18 +1581,18 @@
         <v>39887</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:16" s="3" customFormat="1">
       <c r="A79" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B79" s="4">
-        <v>39887</v>
+        <v>39901</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="80" spans="1:16" s="3" customFormat="1">
@@ -1613,7 +1603,7 @@
         <v>39887</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:7" s="3" customFormat="1">
@@ -1624,7 +1614,7 @@
         <v>39887</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="1:7" s="3" customFormat="1">
@@ -1632,68 +1622,73 @@
         <v>9</v>
       </c>
       <c r="B82" s="4">
-        <v>39902</v>
+        <v>39887</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" s="9" customFormat="1">
-      <c r="C83" s="9" t="s">
-        <v>101</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" s="3" customFormat="1">
+      <c r="A83" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="3" customFormat="1">
       <c r="A84" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B84" s="4">
-        <v>39905</v>
+        <v>39902</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="3" customFormat="1">
-      <c r="A85" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B85" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>76</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="9" customFormat="1">
+      <c r="C85" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:7" s="3" customFormat="1">
       <c r="A86" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B86" s="4">
-        <v>39902</v>
+        <v>39905</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="87" spans="1:7" s="3" customFormat="1">
       <c r="A87" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B87" s="4">
-        <v>39907</v>
+        <v>39902</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" s="2" customFormat="1">
-      <c r="B88" s="8"/>
-      <c r="C88" s="2" t="s">
-        <v>94</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" s="3" customFormat="1">
+      <c r="A88" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B88" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:7" s="3" customFormat="1">
@@ -1704,111 +1699,106 @@
         <v>39907</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:7" s="2" customFormat="1">
       <c r="B90" s="8"/>
       <c r="C90" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" s="2" customFormat="1">
-      <c r="B91" s="8"/>
-      <c r="C91" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="3" customFormat="1">
+      <c r="A91" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:7" s="2" customFormat="1">
       <c r="B92" s="8"/>
-      <c r="D92" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" s="3" customFormat="1">
-      <c r="A93" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B93" s="4">
-        <v>39907</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>99</v>
+      <c r="C92" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" s="2" customFormat="1">
+      <c r="B93" s="8"/>
+      <c r="C93" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="94" spans="1:7" s="2" customFormat="1">
       <c r="B94" s="8"/>
-      <c r="C94" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" s="2" customFormat="1">
-      <c r="B95" s="8"/>
-      <c r="C95" s="2" t="s">
-        <v>141</v>
+      <c r="D94" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" s="3" customFormat="1">
+      <c r="A95" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B95" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:7" s="2" customFormat="1">
       <c r="B96" s="8"/>
-      <c r="D96" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="C98" s="5" t="s">
+      <c r="C96" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" s="2" customFormat="1">
+      <c r="B97" s="8"/>
+      <c r="C97" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="2" customFormat="1">
+      <c r="B98" s="8"/>
+      <c r="D98" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="C100" s="5" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="C99" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="C100" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="C101" s="1" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="C102" s="1" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="C103" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="C104" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="C105" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
-      <c r="C105" s="5" t="s">
+    <row r="107" spans="1:4">
+      <c r="C107" s="5" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" s="3" customFormat="1">
-      <c r="A106" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B106" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" s="3" customFormat="1">
-      <c r="A107" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B107" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="108" spans="1:4" s="3" customFormat="1">
@@ -1819,7 +1809,7 @@
         <v>39902</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="109" spans="1:4" s="3" customFormat="1">
@@ -1830,270 +1820,292 @@
         <v>39902</v>
       </c>
       <c r="C109" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" s="3" customFormat="1">
+      <c r="A110" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B110" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" s="3" customFormat="1">
+      <c r="A111" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C111" s="3" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
-      <c r="C110" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="D111" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="C112" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="113" spans="1:10">
-      <c r="C113" s="1" t="s">
-        <v>55</v>
+      <c r="D113" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="114" spans="1:10">
       <c r="C114" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="C115" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="C116" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
-      <c r="C118" s="1" t="s">
+    <row r="120" spans="1:10">
+      <c r="C120" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="E120" s="1" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10">
-      <c r="A120" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B120" s="1">
-        <v>1</v>
-      </c>
-      <c r="C120" s="1">
-        <v>56</v>
-      </c>
-      <c r="G120" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10">
-      <c r="A121" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B121" s="1">
-        <v>6</v>
-      </c>
-      <c r="C121" s="1">
-        <v>78</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="122" spans="1:10">
       <c r="A122" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B122" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C122" s="1">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
     </row>
     <row r="123" spans="1:10">
       <c r="A123" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B123" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C123" s="1">
-        <v>110</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
     </row>
     <row r="124" spans="1:10">
       <c r="A124" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B124" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C124" s="1">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="125" spans="1:10">
       <c r="A125" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B125" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C125" s="1">
-        <v>154</v>
+        <v>110</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="126" spans="1:10">
       <c r="A126" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B126" s="1">
+        <v>11</v>
+      </c>
+      <c r="C126" s="1">
         <v>128</v>
       </c>
-      <c r="B126" s="1">
-        <v>8</v>
-      </c>
-      <c r="C126" s="1">
-        <v>156</v>
-      </c>
       <c r="G126" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I126" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="J126" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="127" spans="1:10">
       <c r="A127" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B127" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C127" s="1">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="128" spans="1:10">
       <c r="A128" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B128" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C128" s="1">
-        <v>306</v>
-      </c>
-      <c r="D128" s="1">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J128" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="129" spans="1:12">
       <c r="A129" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B129" s="1">
-        <v>14</v>
-      </c>
-      <c r="C129" s="1">
-        <v>318</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>118</v>
+        <v>13</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B130" s="1">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="C130" s="1">
+        <v>306</v>
+      </c>
+      <c r="D130" s="1">
+        <v>164</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="131" spans="1:12">
       <c r="A131" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B131" s="1">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C131" s="1">
+        <v>318</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="132" spans="1:12">
       <c r="A132" s="1" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B132" s="1">
-        <v>5</v>
-      </c>
-      <c r="C132" s="1">
-        <v>92</v>
+        <v>12</v>
+      </c>
+      <c r="E132" s="1">
+        <v>250</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L132" s="1" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="133" spans="1:12">
       <c r="A133" s="1" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="B133" s="1">
-        <v>4</v>
-      </c>
-      <c r="C133" s="1">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L133" s="1" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B134" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C134" s="1">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="137" spans="1:12">
-      <c r="B137" s="1" t="s">
-        <v>149</v>
+      <c r="L134" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
+      <c r="A135" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B135" s="1">
+        <v>4</v>
+      </c>
+      <c r="C135" s="1">
+        <v>88</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L135" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
+      <c r="A136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B136" s="1">
+        <v>2</v>
+      </c>
+      <c r="C136" s="1">
+        <v>156</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
+      <c r="B139" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3 maps removed, one change of map order delete your savegames
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="153">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -456,9 +456,6 @@
     <t>when you hit save game in pause menu, it needs to fire a click ok state</t>
   </si>
   <si>
-    <t>nuke save game button from options menu</t>
-  </si>
-  <si>
     <t>update all map mini images to match the current maps, AFTER all the maps have been cleaned up/tweaked</t>
   </si>
   <si>
@@ -475,6 +472,9 @@
   </si>
   <si>
     <t>help screen needs to load on create new profile</t>
+  </si>
+  <si>
+    <t>speed up/down images draw behind dragged command</t>
   </si>
 </sst>
 </file>
@@ -859,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1338,59 +1338,69 @@
     <row r="44" spans="1:3" s="2" customFormat="1">
       <c r="B44" s="8"/>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1">
-      <c r="B45" s="8"/>
-      <c r="C45" s="2" t="s">
+    <row r="45" spans="1:3" s="3" customFormat="1">
+      <c r="A45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="2" customFormat="1">
       <c r="B46" s="8"/>
-      <c r="C46" s="2" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="47" spans="1:3" s="2" customFormat="1">
       <c r="B47" s="8"/>
+      <c r="C47" s="2" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="48" spans="1:3" s="2" customFormat="1">
       <c r="B48" s="8"/>
       <c r="C48" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="2" customFormat="1">
-      <c r="B49" s="8"/>
-      <c r="C49" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" s="3" customFormat="1">
-      <c r="A50" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="3" customFormat="1">
+      <c r="A49" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B49" s="4">
         <v>39908</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C49" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="2" customFormat="1">
+      <c r="B50" s="8"/>
+      <c r="C50" s="2" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="2" customFormat="1">
       <c r="B51" s="8"/>
-      <c r="C51" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" s="2" customFormat="1">
-      <c r="B52" s="8"/>
-    </row>
-    <row r="53" spans="1:3" s="6" customFormat="1">
-      <c r="B53" s="7"/>
-    </row>
-    <row r="54" spans="1:3" s="5" customFormat="1">
-      <c r="C54" s="5" t="s">
+    </row>
+    <row r="52" spans="1:3" s="6" customFormat="1">
+      <c r="B52" s="7"/>
+    </row>
+    <row r="53" spans="1:3" s="5" customFormat="1">
+      <c r="C53" s="5" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="3" customFormat="1">
+      <c r="A54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="4">
+        <v>39901</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="3" customFormat="1">
@@ -1398,21 +1408,21 @@
         <v>9</v>
       </c>
       <c r="B55" s="4">
-        <v>39901</v>
+        <v>39902</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="3" customFormat="1">
       <c r="A56" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B56" s="4">
-        <v>39902</v>
+        <v>39904</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="3" customFormat="1">
@@ -1423,18 +1433,18 @@
         <v>39904</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="3" customFormat="1">
       <c r="A58" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B58" s="4">
-        <v>39904</v>
+        <v>39906</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="3" customFormat="1">
@@ -1442,125 +1452,125 @@
         <v>9</v>
       </c>
       <c r="B59" s="4">
-        <v>39906</v>
+        <v>39908</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" s="3" customFormat="1">
-      <c r="A60" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B60" s="4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="9" customFormat="1">
+      <c r="A60" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="3" customFormat="1">
+      <c r="A61" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61" s="4">
         <v>39908</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="9" customFormat="1">
-      <c r="A61" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" s="3" customFormat="1">
-      <c r="A62" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B62" s="4">
-        <v>39908</v>
-      </c>
-      <c r="C62" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="9" customFormat="1">
+      <c r="C62" s="9" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="9" customFormat="1">
       <c r="C63" s="9" t="s">
-        <v>144</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="9" customFormat="1">
+      <c r="A64" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="C64" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:16" s="9" customFormat="1">
-      <c r="A65" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="C65" s="9" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:16" s="9" customFormat="1">
       <c r="C66" s="9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:16" s="9" customFormat="1">
       <c r="C67" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:16" s="9" customFormat="1">
-      <c r="C68" s="9" t="s">
-        <v>16</v>
+      <c r="D68" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:16" s="9" customFormat="1">
       <c r="D69" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:16" s="9" customFormat="1">
       <c r="D70" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:16" s="9" customFormat="1">
-      <c r="D71" s="9" t="s">
-        <v>19</v>
+      <c r="A71" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:16" s="9" customFormat="1">
-      <c r="A72" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="B72" s="10"/>
       <c r="C72" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" s="9" customFormat="1">
-      <c r="B73" s="10"/>
-      <c r="C73" s="9" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-      <c r="K74" s="2"/>
-      <c r="L74" s="2"/>
-      <c r="M74" s="2"/>
-      <c r="N74" s="2"/>
-      <c r="O74" s="2"/>
-      <c r="P74" s="2"/>
-    </row>
-    <row r="76" spans="1:16">
-      <c r="C76" s="5" t="s">
+    <row r="73" spans="1:16">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+      <c r="O73" s="2"/>
+      <c r="P73" s="2"/>
+    </row>
+    <row r="75" spans="1:16">
+      <c r="C75" s="5" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" s="3" customFormat="1">
+      <c r="A76" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76" s="4">
+        <v>39888</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="77" spans="1:16" s="3" customFormat="1">
@@ -1568,54 +1578,54 @@
         <v>9</v>
       </c>
       <c r="B77" s="4">
-        <v>39888</v>
+        <v>39881</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:16" s="3" customFormat="1">
       <c r="A78" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B78" s="4">
-        <v>39881</v>
+        <v>39882</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="1:16" s="3" customFormat="1">
       <c r="A79" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B79" s="4">
-        <v>39882</v>
+        <v>39887</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="80" spans="1:16" s="3" customFormat="1">
       <c r="A80" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B80" s="4">
-        <v>39887</v>
+        <v>39901</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:7" s="3" customFormat="1">
       <c r="A81" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B81" s="4">
-        <v>39901</v>
+        <v>39887</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:7" s="3" customFormat="1">
@@ -1626,7 +1636,7 @@
         <v>39887</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:7" s="3" customFormat="1">
@@ -1637,7 +1647,7 @@
         <v>39887</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="3" customFormat="1">
@@ -1648,7 +1658,7 @@
         <v>39887</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:7" s="3" customFormat="1">
@@ -1656,26 +1666,29 @@
         <v>9</v>
       </c>
       <c r="B85" s="4">
-        <v>39887</v>
+        <v>39902</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" s="3" customFormat="1">
-      <c r="A86" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B86" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C86" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="9" customFormat="1">
-      <c r="C87" s="9" t="s">
+    <row r="86" spans="1:7" s="9" customFormat="1">
+      <c r="C86" s="9" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="3" customFormat="1">
+      <c r="A87" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="4">
+        <v>39905</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:7" s="3" customFormat="1">
@@ -1683,24 +1696,21 @@
         <v>6</v>
       </c>
       <c r="B88" s="4">
-        <v>39905</v>
+        <v>39902</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="89" spans="1:7" s="3" customFormat="1">
       <c r="A89" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B89" s="4">
         <v>39902</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:7" s="3" customFormat="1">
@@ -1708,85 +1718,80 @@
         <v>9</v>
       </c>
       <c r="B90" s="4">
-        <v>39902</v>
+        <v>39907</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" s="3" customFormat="1">
-      <c r="A91" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B91" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="2" customFormat="1">
+      <c r="B91" s="8"/>
+      <c r="C91" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" s="3" customFormat="1">
+      <c r="A92" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B92" s="4">
         <v>39907</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" s="2" customFormat="1">
-      <c r="B92" s="8"/>
-      <c r="C92" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" s="3" customFormat="1">
-      <c r="A93" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B93" s="4">
-        <v>39907</v>
-      </c>
-      <c r="C93" s="3" t="s">
+      <c r="C92" s="3" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" s="2" customFormat="1">
+      <c r="B93" s="8"/>
+      <c r="C93" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:7" s="2" customFormat="1">
       <c r="B94" s="8"/>
       <c r="C94" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" spans="1:7" s="2" customFormat="1">
       <c r="B95" s="8"/>
-      <c r="C95" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" s="2" customFormat="1">
-      <c r="B96" s="8"/>
-      <c r="D96" s="2" t="s">
+      <c r="D95" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:4" s="3" customFormat="1">
-      <c r="A97" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B97" s="4">
+    <row r="96" spans="1:7" s="3" customFormat="1">
+      <c r="A96" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96" s="4">
         <v>39907</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" s="2" customFormat="1">
+      <c r="B97" s="8"/>
+      <c r="C97" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="98" spans="1:4" s="2" customFormat="1">
       <c r="B98" s="8"/>
       <c r="C98" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="2" customFormat="1">
       <c r="B99" s="8"/>
-      <c r="C99" s="2" t="s">
-        <v>140</v>
+      <c r="D99" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="100" spans="1:4" s="2" customFormat="1">
       <c r="B100" s="8"/>
-      <c r="D100" s="2" t="s">
-        <v>141</v>
+      <c r="C100" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2021,8 +2026,11 @@
       <c r="C131" s="1">
         <v>296</v>
       </c>
+      <c r="D131" s="1">
+        <v>438</v>
+      </c>
       <c r="E131" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="132" spans="1:12">
@@ -2050,7 +2058,7 @@
         <v>14</v>
       </c>
       <c r="C133" s="1">
-        <v>318</v>
+        <v>792</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>117</v>
@@ -2131,7 +2139,7 @@
     </row>
     <row r="141" spans="1:12">
       <c r="B141" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
map reordering again, proper memory amounts available on all maps now maps c2, c4 and c5 totally removed from the gamevars
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="158">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -475,6 +475,21 @@
   </si>
   <si>
     <t>speed up/down images draw behind dragged command</t>
+  </si>
+  <si>
+    <t>map c2 - try with no electric walls</t>
+  </si>
+  <si>
+    <t>memory given</t>
+  </si>
+  <si>
+    <t>flip the location of reset and clear buttons</t>
+  </si>
+  <si>
+    <t>when robot hits a reprogram square, it should do a little dance</t>
+  </si>
+  <si>
+    <t>go ahead, delete your save game, then go click load profile, then go try making a new profile, try it I dare you</t>
   </si>
 </sst>
 </file>
@@ -857,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P141"/>
+  <dimension ref="A1:P146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1351,6 +1366,9 @@
     </row>
     <row r="46" spans="1:3" s="2" customFormat="1">
       <c r="B46" s="8"/>
+      <c r="C46" s="2" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="47" spans="1:3" s="2" customFormat="1">
       <c r="B47" s="8"/>
@@ -1358,9 +1376,14 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="2" customFormat="1">
-      <c r="B48" s="8"/>
-      <c r="C48" s="2" t="s">
+    <row r="48" spans="1:3" s="3" customFormat="1">
+      <c r="A48" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1375,95 +1398,103 @@
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="2" customFormat="1">
-      <c r="B50" s="8"/>
-      <c r="C50" s="2" t="s">
+    <row r="50" spans="1:3" s="3" customFormat="1">
+      <c r="A50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="2" customFormat="1">
-      <c r="B51" s="8"/>
-    </row>
-    <row r="52" spans="1:3" s="6" customFormat="1">
-      <c r="B52" s="7"/>
-    </row>
-    <row r="53" spans="1:3" s="5" customFormat="1">
-      <c r="C53" s="5" t="s">
+    <row r="51" spans="1:3" s="3" customFormat="1">
+      <c r="A51" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="3" customFormat="1">
+      <c r="A52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="2" customFormat="1">
+      <c r="B53" s="8"/>
+    </row>
+    <row r="54" spans="1:3" s="6" customFormat="1">
+      <c r="B54" s="7"/>
+    </row>
+    <row r="55" spans="1:3" s="5" customFormat="1">
+      <c r="C55" s="5" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" s="3" customFormat="1">
-      <c r="A54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B54" s="4">
-        <v>39901</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" s="3" customFormat="1">
-      <c r="A55" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B55" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="3" customFormat="1">
       <c r="A56" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B56" s="4">
-        <v>39904</v>
+        <v>39901</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="3" customFormat="1">
       <c r="A57" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B57" s="4">
-        <v>39904</v>
+        <v>39902</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="3" customFormat="1">
       <c r="A58" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B58" s="4">
-        <v>39906</v>
+        <v>39904</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="3" customFormat="1">
       <c r="A59" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B59" s="4">
-        <v>39908</v>
+        <v>39904</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" s="9" customFormat="1">
-      <c r="A60" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="3" customFormat="1">
+      <c r="A60" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" s="4">
+        <v>39906</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="3" customFormat="1">
@@ -1474,125 +1505,122 @@
         <v>39908</v>
       </c>
       <c r="C61" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="9" customFormat="1">
+      <c r="A62" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="3" customFormat="1">
+      <c r="A63" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="9" customFormat="1">
-      <c r="C62" s="9" t="s">
+    <row r="64" spans="1:3" s="9" customFormat="1">
+      <c r="C64" s="9" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" s="9" customFormat="1">
-      <c r="C63" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" s="9" customFormat="1">
-      <c r="A64" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:16" s="9" customFormat="1">
       <c r="C65" s="9" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:16" s="9" customFormat="1">
+      <c r="A66" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="C66" s="9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:16" s="9" customFormat="1">
       <c r="C67" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" s="9" customFormat="1">
+      <c r="C68" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" s="9" customFormat="1">
+      <c r="C69" s="9" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" s="9" customFormat="1">
-      <c r="D68" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" s="9" customFormat="1">
-      <c r="D69" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:16" s="9" customFormat="1">
       <c r="D70" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" s="9" customFormat="1">
+      <c r="D71" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" s="9" customFormat="1">
+      <c r="D72" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:16" s="9" customFormat="1">
-      <c r="A71" s="9" t="s">
+    <row r="73" spans="1:16" s="9" customFormat="1">
+      <c r="A73" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C71" s="9" t="s">
+      <c r="C73" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="9" customFormat="1">
-      <c r="B72" s="10"/>
-      <c r="C72" s="9" t="s">
+    <row r="74" spans="1:16" s="9" customFormat="1">
+      <c r="B74" s="10"/>
+      <c r="C74" s="9" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="L73" s="2"/>
-      <c r="M73" s="2"/>
-      <c r="N73" s="2"/>
-      <c r="O73" s="2"/>
-      <c r="P73" s="2"/>
-    </row>
     <row r="75" spans="1:16">
-      <c r="C75" s="5" t="s">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
+      <c r="O75" s="2"/>
+      <c r="P75" s="2"/>
+    </row>
+    <row r="77" spans="1:16">
+      <c r="C77" s="5" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" s="3" customFormat="1">
-      <c r="A76" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B76" s="4">
-        <v>39888</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" s="3" customFormat="1">
-      <c r="A77" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B77" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:16" s="3" customFormat="1">
       <c r="A78" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B78" s="4">
-        <v>39882</v>
+        <v>39888</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:16" s="3" customFormat="1">
@@ -1600,10 +1628,10 @@
         <v>9</v>
       </c>
       <c r="B79" s="4">
-        <v>39887</v>
+        <v>39881</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="80" spans="1:16" s="3" customFormat="1">
@@ -1611,10 +1639,10 @@
         <v>13</v>
       </c>
       <c r="B80" s="4">
-        <v>39901</v>
+        <v>39882</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:7" s="3" customFormat="1">
@@ -1625,18 +1653,18 @@
         <v>39887</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:7" s="3" customFormat="1">
       <c r="A82" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B82" s="4">
-        <v>39887</v>
+        <v>39901</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:7" s="3" customFormat="1">
@@ -1647,7 +1675,7 @@
         <v>39887</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="3" customFormat="1">
@@ -1658,7 +1686,7 @@
         <v>39887</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85" spans="1:7" s="3" customFormat="1">
@@ -1666,68 +1694,73 @@
         <v>9</v>
       </c>
       <c r="B85" s="4">
-        <v>39902</v>
+        <v>39887</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" s="9" customFormat="1">
-      <c r="C86" s="9" t="s">
-        <v>101</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" s="3" customFormat="1">
+      <c r="A86" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B86" s="4">
+        <v>39887</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:7" s="3" customFormat="1">
       <c r="A87" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B87" s="4">
-        <v>39905</v>
+        <v>39902</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" s="3" customFormat="1">
-      <c r="A88" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B88" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>76</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" s="9" customFormat="1">
+      <c r="C88" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:7" s="3" customFormat="1">
       <c r="A89" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B89" s="4">
-        <v>39902</v>
+        <v>39905</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:7" s="3" customFormat="1">
       <c r="A90" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B90" s="4">
-        <v>39907</v>
+        <v>39902</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" s="2" customFormat="1">
-      <c r="B91" s="8"/>
-      <c r="C91" s="2" t="s">
-        <v>94</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="3" customFormat="1">
+      <c r="A91" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="1:7" s="3" customFormat="1">
@@ -1738,117 +1771,117 @@
         <v>39907</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:7" s="2" customFormat="1">
       <c r="B93" s="8"/>
       <c r="C93" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" s="3" customFormat="1">
+      <c r="A94" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B94" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" s="3" customFormat="1">
+      <c r="A95" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B95" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="2" customFormat="1">
-      <c r="B94" s="8"/>
-      <c r="C94" s="2" t="s">
+    <row r="96" spans="1:7" s="2" customFormat="1">
+      <c r="B96" s="8"/>
+      <c r="C96" s="2" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" s="2" customFormat="1">
-      <c r="B95" s="8"/>
-      <c r="D95" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" s="3" customFormat="1">
-      <c r="A96" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B96" s="4">
-        <v>39907</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="2" customFormat="1">
       <c r="B97" s="8"/>
-      <c r="C97" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" s="2" customFormat="1">
-      <c r="B98" s="8"/>
-      <c r="C98" s="2" t="s">
-        <v>140</v>
+      <c r="D97" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="3" customFormat="1">
+      <c r="A98" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B98" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="2" customFormat="1">
       <c r="B99" s="8"/>
-      <c r="D99" s="2" t="s">
-        <v>141</v>
+      <c r="C99" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:4" s="2" customFormat="1">
       <c r="B100" s="8"/>
       <c r="C100" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" s="2" customFormat="1">
+      <c r="B101" s="8"/>
+      <c r="D101" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" s="2" customFormat="1">
+      <c r="B102" s="8"/>
+      <c r="C102" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="C102" s="5" t="s">
+    <row r="104" spans="1:4">
+      <c r="C104" s="5" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="C103" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="C104" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="C105" s="1" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="C106" s="1" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="C107" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="C108" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="C109" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
-      <c r="C109" s="5" t="s">
+    <row r="111" spans="1:4">
+      <c r="C111" s="5" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" s="3" customFormat="1">
-      <c r="A110" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B110" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" s="3" customFormat="1">
-      <c r="A111" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B111" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="112" spans="1:4" s="3" customFormat="1">
@@ -1859,10 +1892,10 @@
         <v>39902</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" s="3" customFormat="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" s="3" customFormat="1">
       <c r="A113" s="3" t="s">
         <v>9</v>
       </c>
@@ -1870,280 +1903,356 @@
         <v>39902</v>
       </c>
       <c r="C113" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" s="3" customFormat="1">
+      <c r="A114" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B114" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" s="3" customFormat="1">
+      <c r="A115" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B115" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
-      <c r="C114" s="1" t="s">
+    <row r="116" spans="1:9">
+      <c r="C116" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
-      <c r="D115" s="1" t="s">
+    <row r="117" spans="1:9">
+      <c r="D117" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
-      <c r="C116" s="1" t="s">
+    <row r="118" spans="1:9">
+      <c r="C118" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
-      <c r="C117" s="1" t="s">
+    <row r="119" spans="1:9">
+      <c r="C119" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
-      <c r="C118" s="1" t="s">
+    <row r="120" spans="1:9">
+      <c r="C120" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
-      <c r="C122" s="1" t="s">
+    <row r="124" spans="1:9">
+      <c r="C124" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D124" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E122" s="1" t="s">
+      <c r="E124" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G124" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
-      <c r="A124" s="1" t="s">
+    <row r="126" spans="1:9">
+      <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B126" s="1">
         <v>1</v>
       </c>
-      <c r="C124" s="1">
+      <c r="C126" s="1">
         <v>56</v>
       </c>
-      <c r="G124" s="1" t="s">
+      <c r="E126" s="3">
+        <v>64</v>
+      </c>
+      <c r="I126" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
-      <c r="A125" s="1" t="s">
+    <row r="127" spans="1:9">
+      <c r="A127" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B125" s="1">
+      <c r="B127" s="1">
         <v>6</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C127" s="1">
         <v>78</v>
       </c>
-      <c r="G125" s="1" t="s">
+      <c r="E127" s="3">
+        <v>90</v>
+      </c>
+      <c r="I127" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
-      <c r="A126" s="1" t="s">
+    <row r="128" spans="1:9">
+      <c r="A128" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B126" s="1">
+      <c r="B128" s="1">
         <v>7</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C128" s="1">
         <v>64</v>
       </c>
-      <c r="G126" s="1" t="s">
+      <c r="E128" s="3">
+        <v>82</v>
+      </c>
+      <c r="I128" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
-      <c r="A127" s="1" t="s">
+    <row r="129" spans="1:14">
+      <c r="A129" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B127" s="1">
+      <c r="B129" s="1">
         <v>3</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C129" s="1">
         <v>110</v>
       </c>
-      <c r="E127" s="1" t="s">
+      <c r="E129" s="3">
+        <v>128</v>
+      </c>
+      <c r="G129" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G127" s="1" t="s">
+      <c r="I129" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
-      <c r="A128" s="1" t="s">
+    <row r="130" spans="1:14">
+      <c r="A130" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B128" s="1">
+      <c r="B130" s="1">
         <v>11</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C130" s="1">
         <v>128</v>
       </c>
-      <c r="G128" s="1" t="s">
+      <c r="E130" s="3">
+        <v>140</v>
+      </c>
+      <c r="I130" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="129" spans="1:12">
-      <c r="A129" s="1" t="s">
+    <row r="131" spans="1:14">
+      <c r="A131" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B129" s="1">
+      <c r="B131" s="1">
         <v>10</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C131" s="1">
         <v>154</v>
       </c>
-      <c r="G129" s="1" t="s">
+      <c r="E131" s="3">
+        <v>164</v>
+      </c>
+      <c r="I131" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="130" spans="1:12">
-      <c r="A130" s="1" t="s">
+    <row r="132" spans="1:14">
+      <c r="A132" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B130" s="1">
+      <c r="B132" s="1">
         <v>8</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C132" s="1">
         <v>156</v>
       </c>
-      <c r="G130" s="1" t="s">
+      <c r="E132" s="3">
+        <v>164</v>
+      </c>
+      <c r="I132" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I130" s="1" t="s">
+      <c r="K132" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J130" s="1" t="s">
+      <c r="L132" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="131" spans="1:12">
-      <c r="A131" s="1" t="s">
+    <row r="133" spans="1:14">
+      <c r="A133" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B133" s="1">
+        <v>9</v>
+      </c>
+      <c r="C133" s="1">
+        <v>306</v>
+      </c>
+      <c r="D133" s="1">
+        <v>164</v>
+      </c>
+      <c r="E133" s="3">
+        <v>364</v>
+      </c>
+      <c r="I133" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14">
+      <c r="A134" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B131" s="1">
+      <c r="B134" s="1">
         <v>13</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C134" s="1">
         <v>296</v>
       </c>
-      <c r="D131" s="1">
+      <c r="D134" s="1">
         <v>438</v>
       </c>
-      <c r="E131" s="1" t="s">
+      <c r="E134" s="3">
+        <v>512</v>
+      </c>
+      <c r="G134" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="132" spans="1:12">
-      <c r="A132" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B132" s="1">
-        <v>9</v>
-      </c>
-      <c r="C132" s="1">
-        <v>306</v>
-      </c>
-      <c r="D132" s="1">
-        <v>164</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12">
-      <c r="A133" s="1" t="s">
+    <row r="135" spans="1:14">
+      <c r="A135" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B133" s="1">
+      <c r="B135" s="1">
         <v>14</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C135" s="1">
         <v>792</v>
       </c>
-      <c r="G133" s="1" t="s">
+      <c r="E135" s="3">
+        <v>812</v>
+      </c>
+      <c r="I135" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="134" spans="1:12">
-      <c r="A134" s="1" t="s">
+    <row r="136" spans="1:14">
+      <c r="A136" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B134" s="1">
+      <c r="B136" s="1">
         <v>12</v>
       </c>
-      <c r="E134" s="1">
+      <c r="C136" s="1">
+        <v>242</v>
+      </c>
+      <c r="E136" s="3">
+        <v>256</v>
+      </c>
+      <c r="G136" s="1">
         <v>250</v>
       </c>
-      <c r="G134" s="1" t="s">
+      <c r="I136" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="135" spans="1:12">
-      <c r="A135" s="1" t="s">
+    <row r="137" spans="1:14">
+      <c r="A137" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B135" s="1">
+      <c r="B137" s="1">
         <v>15</v>
       </c>
-      <c r="G135" s="1" t="s">
+      <c r="E137" s="3"/>
+      <c r="I137" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="136" spans="1:12">
-      <c r="A136" s="1" t="s">
+    <row r="138" spans="1:14">
+      <c r="A138" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B136" s="1">
+      <c r="B138" s="1">
         <v>5</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C138" s="1">
         <v>92</v>
       </c>
-      <c r="G136" s="1" t="s">
+      <c r="E138" s="3">
+        <v>1024</v>
+      </c>
+      <c r="I138" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="L136" s="1" t="s">
+      <c r="N138" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="137" spans="1:12">
-      <c r="A137" s="1" t="s">
+    <row r="139" spans="1:14">
+      <c r="A139" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B139" s="1">
         <v>4</v>
       </c>
-      <c r="C137" s="1">
+      <c r="C139" s="1">
         <v>88</v>
       </c>
-      <c r="G137" s="1" t="s">
+      <c r="E139" s="3">
+        <v>1024</v>
+      </c>
+      <c r="I139" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="L137" s="1" t="s">
+      <c r="N139" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="138" spans="1:12">
-      <c r="A138" s="1" t="s">
+    <row r="140" spans="1:14">
+      <c r="A140" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B140" s="1">
         <v>2</v>
       </c>
-      <c r="C138" s="1">
+      <c r="C140" s="1">
         <v>156</v>
       </c>
-      <c r="G138" s="1" t="s">
+      <c r="E140" s="3">
+        <v>150</v>
+      </c>
+      <c r="I140" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="141" spans="1:12">
-      <c r="B141" s="1" t="s">
+    <row r="143" spans="1:14">
+      <c r="B143" s="1" t="s">
         <v>147</v>
       </c>
     </row>
+    <row r="146" spans="2:2">
+      <c r="B146" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A126:L140">
+  <sortState ref="A125:N139">
     <sortCondition ref="C126:C140"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated history document wish list is now sorted by date instead of by randomness
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="157">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -457,9 +457,6 @@
   </si>
   <si>
     <t>update all map mini images to match the current maps, AFTER all the maps have been cleaned up/tweaked</t>
-  </si>
-  <si>
-    <t>tutorial map 7 - remove the two solid blocks</t>
   </si>
   <si>
     <t>make reset button, reset zoom as well</t>
@@ -874,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -906,13 +903,13 @@
     </row>
     <row r="3" spans="1:3" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4">
-        <v>39892</v>
+        <v>39881</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1">
@@ -920,32 +917,32 @@
         <v>9</v>
       </c>
       <c r="B4" s="4">
-        <v>39883</v>
+        <v>39881</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4">
         <v>39881</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B6" s="4">
-        <v>39883</v>
+        <v>39881</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="3" customFormat="1">
@@ -956,7 +953,7 @@
         <v>39881</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="3" customFormat="1">
@@ -964,54 +961,54 @@
         <v>9</v>
       </c>
       <c r="B8" s="4">
-        <v>39881</v>
+        <v>39883</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" s="4">
         <v>39883</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
-        <v>39881</v>
+        <v>39883</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="3" customFormat="1">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B11" s="4">
-        <v>39881</v>
+        <v>39883</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="3" customFormat="1" ht="16.5" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4">
         <v>39883</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="3" customFormat="1">
@@ -1022,7 +1019,7 @@
         <v>39883</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="3" customFormat="1">
@@ -1033,7 +1030,7 @@
         <v>39883</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="3" customFormat="1">
@@ -1044,7 +1041,7 @@
         <v>39883</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="3" customFormat="1">
@@ -1055,7 +1052,7 @@
         <v>39883</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="3" customFormat="1">
@@ -1066,7 +1063,7 @@
         <v>39883</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="3" customFormat="1">
@@ -1074,10 +1071,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="4">
-        <v>39883</v>
+        <v>39888</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="3" customFormat="1">
@@ -1088,29 +1085,29 @@
         <v>39888</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="3" customFormat="1">
       <c r="A20" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B20" s="4">
-        <v>39901</v>
+        <v>39888</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="3" customFormat="1">
       <c r="A21" s="3" t="s">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="B21" s="4">
-        <v>39901</v>
+        <v>39888</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="3" customFormat="1">
@@ -1118,43 +1115,43 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>39888</v>
+        <v>39889</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="3" customFormat="1">
       <c r="A23" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B23" s="4">
-        <v>39888</v>
+        <v>39892</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="3" customFormat="1">
       <c r="A24" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B24" s="4">
-        <v>39888</v>
+        <v>39901</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="3" customFormat="1">
       <c r="A25" s="3" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="B25" s="4">
-        <v>39889</v>
+        <v>39901</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="3" customFormat="1">
@@ -1170,13 +1167,13 @@
     </row>
     <row r="27" spans="1:3" s="3" customFormat="1">
       <c r="A27" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B27" s="4">
-        <v>39902</v>
+        <v>39901</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="3" customFormat="1">
@@ -1187,7 +1184,7 @@
         <v>39901</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="3" customFormat="1">
@@ -1198,40 +1195,40 @@
         <v>39901</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="3" customFormat="1">
       <c r="A30" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B30" s="4">
-        <v>39901</v>
+        <v>39902</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="3" customFormat="1">
       <c r="A31" s="3" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B31" s="4">
-        <v>39907</v>
+        <v>39902</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="3" customFormat="1">
       <c r="A32" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B32" s="4">
-        <v>39904</v>
+        <v>39902</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="3" customFormat="1">
@@ -1242,18 +1239,18 @@
         <v>39902</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="3" customFormat="1">
       <c r="A34" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B34" s="4">
-        <v>39902</v>
+        <v>39904</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="3" customFormat="1">
@@ -1261,10 +1258,10 @@
         <v>13</v>
       </c>
       <c r="B35" s="4">
-        <v>39902</v>
+        <v>39904</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="3" customFormat="1">
@@ -1280,13 +1277,13 @@
     </row>
     <row r="37" spans="1:3" s="3" customFormat="1">
       <c r="A37" s="3" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B37" s="4">
-        <v>39904</v>
+        <v>39907</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="3" customFormat="1">
@@ -1344,36 +1341,59 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="2" customFormat="1">
-      <c r="B43" s="8"/>
-      <c r="C43" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" s="2" customFormat="1">
-      <c r="B44" s="8"/>
+    <row r="43" spans="1:3" s="3" customFormat="1">
+      <c r="A43" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="3" customFormat="1">
+      <c r="A44" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="45" spans="1:3" s="3" customFormat="1">
       <c r="A45" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B45" s="4">
         <v>39908</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" s="2" customFormat="1">
-      <c r="B46" s="8"/>
-      <c r="C46" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" s="2" customFormat="1">
-      <c r="B47" s="8"/>
-      <c r="C47" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="3" customFormat="1">
+      <c r="A46" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="3" customFormat="1">
+      <c r="A47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="3" customFormat="1">
@@ -1384,51 +1404,28 @@
         <v>39908</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="3" customFormat="1">
-      <c r="A49" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="4">
-        <v>39908</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" s="3" customFormat="1">
-      <c r="A50" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50" s="4">
-        <v>39908</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" s="3" customFormat="1">
-      <c r="A51" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="4">
-        <v>39908</v>
-      </c>
-      <c r="C51" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="2" customFormat="1">
+      <c r="B49" s="8"/>
+      <c r="C49" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="2" customFormat="1">
+      <c r="B50" s="8"/>
+    </row>
+    <row r="51" spans="1:3" s="2" customFormat="1">
+      <c r="B51" s="8"/>
+      <c r="C51" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="3" customFormat="1">
-      <c r="A52" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B52" s="4">
-        <v>39908</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>157</v>
+    <row r="52" spans="1:3" s="2" customFormat="1">
+      <c r="B52" s="8"/>
+      <c r="C52" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="2" customFormat="1">
@@ -1508,23 +1505,23 @@
         <v>138</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="9" customFormat="1">
-      <c r="A62" s="9" t="s">
+    <row r="62" spans="1:3" s="3" customFormat="1">
+      <c r="A62" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="9" customFormat="1">
+      <c r="A63" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C63" s="9" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" s="3" customFormat="1">
-      <c r="A63" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B63" s="4">
-        <v>39908</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="9" customFormat="1">
@@ -1617,32 +1614,32 @@
         <v>9</v>
       </c>
       <c r="B78" s="4">
-        <v>39888</v>
+        <v>39881</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="79" spans="1:16" s="3" customFormat="1">
       <c r="A79" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B79" s="4">
-        <v>39881</v>
+        <v>39882</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="80" spans="1:16" s="3" customFormat="1">
       <c r="A80" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B80" s="4">
-        <v>39882</v>
+        <v>39887</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="81" spans="1:7" s="3" customFormat="1">
@@ -1653,18 +1650,18 @@
         <v>39887</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:7" s="3" customFormat="1">
       <c r="A82" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B82" s="4">
-        <v>39901</v>
+        <v>39887</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:7" s="3" customFormat="1">
@@ -1675,7 +1672,7 @@
         <v>39887</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="3" customFormat="1">
@@ -1686,7 +1683,7 @@
         <v>39887</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:7" s="3" customFormat="1">
@@ -1694,21 +1691,21 @@
         <v>9</v>
       </c>
       <c r="B85" s="4">
-        <v>39887</v>
+        <v>39888</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:7" s="3" customFormat="1">
       <c r="A86" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B86" s="4">
-        <v>39887</v>
+        <v>39901</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="87" spans="1:7" s="3" customFormat="1">
@@ -1722,23 +1719,29 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:7" s="9" customFormat="1">
-      <c r="C88" s="9" t="s">
-        <v>101</v>
+    <row r="88" spans="1:7" s="3" customFormat="1">
+      <c r="A88" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:7" s="3" customFormat="1">
       <c r="A89" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B89" s="4">
-        <v>39905</v>
+        <v>39902</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:7" s="3" customFormat="1">
@@ -1746,10 +1749,10 @@
         <v>6</v>
       </c>
       <c r="B90" s="4">
-        <v>39902</v>
+        <v>39905</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="3" customFormat="1">
@@ -1757,10 +1760,10 @@
         <v>9</v>
       </c>
       <c r="B91" s="4">
-        <v>39902</v>
+        <v>39907</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="92" spans="1:7" s="3" customFormat="1">
@@ -1771,58 +1774,52 @@
         <v>39907</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" s="2" customFormat="1">
-      <c r="B93" s="8"/>
-      <c r="C93" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" s="3" customFormat="1">
+      <c r="A93" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B93" s="4">
+        <v>39907</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="1:7" s="3" customFormat="1">
       <c r="A94" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B94" s="4">
-        <v>39907</v>
+        <v>39908</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" s="3" customFormat="1">
-      <c r="A95" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B95" s="4">
-        <v>39908</v>
-      </c>
-      <c r="C95" s="3" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" s="9" customFormat="1">
+      <c r="C95" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:7" s="2" customFormat="1">
       <c r="B96" s="8"/>
       <c r="C96" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="2" customFormat="1">
       <c r="B97" s="8"/>
-      <c r="D97" s="2" t="s">
+      <c r="C97" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="2" customFormat="1">
+      <c r="B98" s="8"/>
+      <c r="D98" s="2" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" s="3" customFormat="1">
-      <c r="A98" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B98" s="4">
-        <v>39907</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="2" customFormat="1">
@@ -1846,7 +1843,7 @@
     <row r="102" spans="1:4" s="2" customFormat="1">
       <c r="B102" s="8"/>
       <c r="C102" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1961,7 +1958,7 @@
         <v>112</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>113</v>
@@ -2117,56 +2114,56 @@
     </row>
     <row r="134" spans="1:14">
       <c r="A134" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C134" s="1">
-        <v>296</v>
-      </c>
-      <c r="D134" s="1">
-        <v>438</v>
+        <v>242</v>
       </c>
       <c r="E134" s="3">
-        <v>512</v>
-      </c>
-      <c r="G134" s="1" t="s">
-        <v>149</v>
+        <v>256</v>
+      </c>
+      <c r="G134" s="1">
+        <v>250</v>
+      </c>
+      <c r="I134" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B135" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C135" s="1">
-        <v>792</v>
+        <v>296</v>
+      </c>
+      <c r="D135" s="1">
+        <v>438</v>
       </c>
       <c r="E135" s="3">
-        <v>812</v>
-      </c>
-      <c r="I135" s="1" t="s">
-        <v>117</v>
+        <v>512</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="136" spans="1:14">
       <c r="A136" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B136" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C136" s="1">
-        <v>242</v>
+        <v>442</v>
       </c>
       <c r="E136" s="3">
-        <v>256</v>
-      </c>
-      <c r="G136" s="1">
-        <v>250</v>
+        <v>512</v>
       </c>
       <c r="I136" s="1" t="s">
         <v>118</v>
@@ -2174,14 +2171,19 @@
     </row>
     <row r="137" spans="1:14">
       <c r="A137" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B137" s="1">
-        <v>15</v>
-      </c>
-      <c r="E137" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C137" s="1">
+        <v>792</v>
+      </c>
+      <c r="E137" s="3">
+        <v>812</v>
+      </c>
       <c r="I137" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="138" spans="1:14">
@@ -2241,19 +2243,14 @@
         <v>114</v>
       </c>
     </row>
-    <row r="143" spans="1:14">
-      <c r="B143" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
     <row r="146" spans="2:2">
       <c r="B146" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A125:N139">
-    <sortCondition ref="C126:C140"/>
+  <sortState ref="A78:C94">
+    <sortCondition ref="B78:B94"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed auto-scrolling issues with the instruction list, and highlighting. Yay.
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="11040" windowHeight="6930" tabRatio="499"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="163">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -889,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1872,43 +1872,64 @@
         <v>101</v>
       </c>
     </row>
-    <row r="101" spans="1:4" s="2" customFormat="1">
-      <c r="B101" s="8"/>
-      <c r="C101" s="2" t="s">
+    <row r="101" spans="1:4" s="3" customFormat="1">
+      <c r="A101" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" s="4">
+        <v>39909</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="102" spans="1:4" s="2" customFormat="1">
-      <c r="B102" s="8"/>
-      <c r="C102" s="2" t="s">
+    <row r="102" spans="1:4" s="3" customFormat="1">
+      <c r="A102" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102" s="4">
+        <v>39910</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="103" spans="1:4" s="2" customFormat="1">
-      <c r="B103" s="8"/>
-      <c r="D103" s="2" t="s">
+    <row r="103" spans="1:4" s="3" customFormat="1">
+      <c r="B103" s="4"/>
+      <c r="D103" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:4" s="2" customFormat="1">
+      <c r="A104" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B104" s="8"/>
       <c r="C104" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="105" spans="1:4" s="2" customFormat="1">
-      <c r="B105" s="8"/>
-      <c r="C105" s="2" t="s">
+    <row r="105" spans="1:4" s="3" customFormat="1">
+      <c r="A105" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" s="4">
+        <v>39910</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="106" spans="1:4" s="2" customFormat="1">
-      <c r="B106" s="8"/>
-      <c r="D106" s="2" t="s">
+    <row r="106" spans="1:4" s="3" customFormat="1">
+      <c r="B106" s="4"/>
+      <c r="D106" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="107" spans="1:4" s="2" customFormat="1">
+      <c r="A107" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B107" s="8"/>
       <c r="C107" s="2" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
I think this might be my last commit on the project! Bug Fixes: Sub1 & Sub2 Instructions now display proper messages in tooltips (not enough memory / you can't place sub routines here).
Speed up / Slow Down / Help buttons transfered to LogicInterface so they'll draw correctly and all that jazz.

Later y'all!
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -889,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1926,12 +1926,14 @@
         <v>141</v>
       </c>
     </row>
-    <row r="107" spans="1:4" s="2" customFormat="1">
-      <c r="A107" s="2" t="s">
+    <row r="107" spans="1:4" s="3" customFormat="1">
+      <c r="A107" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B107" s="8"/>
-      <c r="C107" s="2" t="s">
+      <c r="B107" s="4">
+        <v>39910</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed climb from tutorialmap5
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="163">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -502,6 +502,9 @@
   </si>
   <si>
     <t>when robot hits a reprogram square, it should do a popup</t>
+  </si>
+  <si>
+    <t>update help for interface to have new positions for buttons and speed and stuff</t>
   </si>
 </sst>
 </file>
@@ -884,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P150"/>
+  <dimension ref="A1:P151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:XFD66"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1501,24 +1504,19 @@
     </row>
     <row r="56" spans="1:3" s="2" customFormat="1">
       <c r="B56" s="8"/>
-    </row>
-    <row r="57" spans="1:3" s="6" customFormat="1">
-      <c r="B57" s="7"/>
-    </row>
-    <row r="58" spans="1:3" s="5" customFormat="1">
-      <c r="C58" s="5" t="s">
+      <c r="C56" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="2" customFormat="1">
+      <c r="B57" s="8"/>
+    </row>
+    <row r="58" spans="1:3" s="6" customFormat="1">
+      <c r="B58" s="7"/>
+    </row>
+    <row r="59" spans="1:3" s="5" customFormat="1">
+      <c r="C59" s="5" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" s="3" customFormat="1">
-      <c r="A59" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B59" s="4">
-        <v>39901</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="3" customFormat="1">
@@ -1526,21 +1524,21 @@
         <v>9</v>
       </c>
       <c r="B60" s="4">
-        <v>39902</v>
+        <v>39901</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="3" customFormat="1">
       <c r="A61" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B61" s="4">
-        <v>39904</v>
+        <v>39902</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="3" customFormat="1">
@@ -1551,18 +1549,18 @@
         <v>39904</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="3" customFormat="1">
       <c r="A63" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B63" s="4">
-        <v>39906</v>
+        <v>39904</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="3" customFormat="1">
@@ -1570,10 +1568,10 @@
         <v>9</v>
       </c>
       <c r="B64" s="4">
-        <v>39908</v>
+        <v>39906</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:16" s="3" customFormat="1">
@@ -1584,7 +1582,7 @@
         <v>39908</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:16" s="3" customFormat="1">
@@ -1592,136 +1590,136 @@
         <v>9</v>
       </c>
       <c r="B66" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" s="3" customFormat="1">
+      <c r="A67" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" s="4">
         <v>39909</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="9" customFormat="1">
-      <c r="A67" s="9" t="s">
+    <row r="68" spans="1:16" s="9" customFormat="1">
+      <c r="A68" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C68" s="9" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" s="9" customFormat="1">
-      <c r="C68" s="9" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:16" s="9" customFormat="1">
       <c r="C69" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" s="9" customFormat="1">
+      <c r="C70" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:16" s="9" customFormat="1">
-      <c r="A70" s="9" t="s">
+    <row r="71" spans="1:16" s="9" customFormat="1">
+      <c r="A71" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="C71" s="9" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" s="9" customFormat="1">
-      <c r="C71" s="9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:16" s="9" customFormat="1">
       <c r="C72" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:16" s="9" customFormat="1">
       <c r="C73" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" s="9" customFormat="1">
+      <c r="C74" s="9" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" s="9" customFormat="1">
-      <c r="D74" s="9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:16" s="9" customFormat="1">
       <c r="D75" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:16" s="9" customFormat="1">
       <c r="D76" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" s="9" customFormat="1">
+      <c r="D77" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="9" customFormat="1">
-      <c r="A77" s="9" t="s">
+    <row r="78" spans="1:16" s="9" customFormat="1">
+      <c r="A78" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C78" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="9" customFormat="1">
-      <c r="B78" s="10"/>
-      <c r="C78" s="9" t="s">
+    <row r="79" spans="1:16" s="9" customFormat="1">
+      <c r="B79" s="10"/>
+      <c r="C79" s="9" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
-      <c r="L79" s="2"/>
-      <c r="M79" s="2"/>
-      <c r="N79" s="2"/>
-      <c r="O79" s="2"/>
-      <c r="P79" s="2"/>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="C81" s="5" t="s">
+    <row r="80" spans="1:16">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+      <c r="O80" s="2"/>
+      <c r="P80" s="2"/>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="C82" s="5" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" s="3" customFormat="1">
-      <c r="A82" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B82" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:7" s="3" customFormat="1">
       <c r="A83" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B83" s="4">
-        <v>39882</v>
+        <v>39881</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="3" customFormat="1">
       <c r="A84" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B84" s="4">
-        <v>39887</v>
+        <v>39882</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="85" spans="1:7" s="3" customFormat="1">
@@ -1732,7 +1730,7 @@
         <v>39887</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="86" spans="1:7" s="3" customFormat="1">
@@ -1743,7 +1741,7 @@
         <v>39887</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="87" spans="1:7" s="3" customFormat="1">
@@ -1754,7 +1752,7 @@
         <v>39887</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="88" spans="1:7" s="3" customFormat="1">
@@ -1765,7 +1763,7 @@
         <v>39887</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="89" spans="1:7" s="3" customFormat="1">
@@ -1773,79 +1771,79 @@
         <v>9</v>
       </c>
       <c r="B89" s="4">
-        <v>39888</v>
+        <v>39887</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
     </row>
     <row r="90" spans="1:7" s="3" customFormat="1">
       <c r="A90" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B90" s="4">
-        <v>39901</v>
+        <v>39888</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="3" customFormat="1">
       <c r="A91" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B91" s="4">
-        <v>39902</v>
+        <v>39901</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" spans="1:7" s="3" customFormat="1">
       <c r="A92" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B92" s="4">
         <v>39902</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="93" spans="1:7" s="3" customFormat="1">
       <c r="A93" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B93" s="4">
         <v>39902</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="1:7" s="3" customFormat="1">
       <c r="A94" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B94" s="4">
-        <v>39905</v>
+        <v>39902</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="95" spans="1:7" s="3" customFormat="1">
       <c r="A95" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B95" s="4">
-        <v>39907</v>
+        <v>39905</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="96" spans="1:7" s="3" customFormat="1">
@@ -1856,7 +1854,7 @@
         <v>39907</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="3" customFormat="1">
@@ -1867,29 +1865,29 @@
         <v>39907</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:4" s="3" customFormat="1">
       <c r="A98" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B98" s="4">
-        <v>39908</v>
+        <v>39907</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="3" customFormat="1">
       <c r="A99" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B99" s="4">
-        <v>39909</v>
+        <v>39908</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:4" s="3" customFormat="1">
@@ -1897,10 +1895,10 @@
         <v>6</v>
       </c>
       <c r="B100" s="4">
-        <v>39910</v>
+        <v>39909</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:4" s="3" customFormat="1">
@@ -1911,7 +1909,7 @@
         <v>39910</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
     </row>
     <row r="102" spans="1:4" s="3" customFormat="1">
@@ -1922,89 +1920,89 @@
         <v>39910</v>
       </c>
       <c r="C102" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" s="3" customFormat="1">
+      <c r="A103" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B103" s="4">
+        <v>39910</v>
+      </c>
+      <c r="C103" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="103" spans="1:4" s="3" customFormat="1">
-      <c r="B103" s="4"/>
-      <c r="D103" s="3" t="s">
+    <row r="104" spans="1:4" s="3" customFormat="1">
+      <c r="B104" s="4"/>
+      <c r="D104" s="3" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" s="3" customFormat="1">
-      <c r="A104" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B104" s="4">
-        <v>39910</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="105" spans="1:4" s="3" customFormat="1">
       <c r="A105" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B105" s="4">
         <v>39910</v>
       </c>
       <c r="C105" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" s="3" customFormat="1">
+      <c r="A106" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B106" s="4">
+        <v>39910</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="106" spans="1:4" s="9" customFormat="1">
-      <c r="C106" s="9" t="s">
+    <row r="107" spans="1:4" s="9" customFormat="1">
+      <c r="C107" s="9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
-      <c r="C108" s="5" t="s">
+    <row r="109" spans="1:4">
+      <c r="C109" s="5" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
-      <c r="C109" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="C110" s="1" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="C111" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="C112" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="C113" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
-      <c r="C113" s="1" t="s">
+    <row r="114" spans="1:4">
+      <c r="C114" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
-      <c r="C115" s="5" t="s">
+    <row r="116" spans="1:4">
+      <c r="C116" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="116" spans="1:7" s="3" customFormat="1">
-      <c r="A116" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B116" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" s="3" customFormat="1">
+    <row r="117" spans="1:4" s="3" customFormat="1">
       <c r="A117" s="3" t="s">
         <v>9</v>
       </c>
@@ -2012,10 +2010,10 @@
         <v>39902</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" s="3" customFormat="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" s="3" customFormat="1">
       <c r="A118" s="3" t="s">
         <v>9</v>
       </c>
@@ -2023,10 +2021,10 @@
         <v>39902</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" s="3" customFormat="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" s="3" customFormat="1">
       <c r="A119" s="3" t="s">
         <v>9</v>
       </c>
@@ -2034,94 +2032,88 @@
         <v>39902</v>
       </c>
       <c r="C119" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" s="3" customFormat="1">
+      <c r="A120" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B120" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C120" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
-      <c r="C120" s="1" t="s">
+    <row r="121" spans="1:4">
+      <c r="C121" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
-      <c r="D121" s="1" t="s">
+    <row r="122" spans="1:4">
+      <c r="D122" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
-      <c r="C122" s="1" t="s">
+    <row r="123" spans="1:4">
+      <c r="C123" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
-      <c r="C123" s="1" t="s">
+    <row r="124" spans="1:4">
+      <c r="C124" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
-      <c r="C124" s="1" t="s">
+    <row r="125" spans="1:4">
+      <c r="C125" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
-      <c r="C128" s="1" t="s">
+    <row r="129" spans="1:14">
+      <c r="C129" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="D129" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E128" s="1" t="s">
+      <c r="E129" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G128" s="1" t="s">
+      <c r="G129" s="1" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="130" spans="1:14">
-      <c r="A130" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B130" s="1">
-        <v>1</v>
-      </c>
-      <c r="C130" s="1">
-        <v>56</v>
-      </c>
-      <c r="E130" s="3">
-        <v>64</v>
-      </c>
-      <c r="I130" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="131" spans="1:14">
       <c r="A131" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B131" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C131" s="1">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E131" s="3">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="132" spans="1:14">
       <c r="A132" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B132" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C132" s="1">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="E132" s="3">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>105</v>
@@ -2129,204 +2121,201 @@
     </row>
     <row r="133" spans="1:14">
       <c r="A133" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B133" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C133" s="1">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="E133" s="3">
-        <v>128</v>
-      </c>
-      <c r="G133" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
     </row>
     <row r="134" spans="1:14">
       <c r="A134" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B134" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C134" s="1">
+        <v>110</v>
+      </c>
+      <c r="E134" s="3">
         <v>128</v>
       </c>
-      <c r="E134" s="3">
-        <v>140</v>
+      <c r="G134" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B135" s="1">
+        <v>11</v>
+      </c>
+      <c r="C135" s="1">
         <v>128</v>
       </c>
-      <c r="B135" s="1">
-        <v>10</v>
-      </c>
-      <c r="C135" s="1">
-        <v>154</v>
-      </c>
       <c r="E135" s="3">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="136" spans="1:14">
       <c r="A136" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B136" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C136" s="1">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E136" s="3">
         <v>164</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K136" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="L136" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="137" spans="1:14">
       <c r="A137" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B137" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C137" s="1">
-        <v>306</v>
-      </c>
-      <c r="D137" s="1">
+        <v>156</v>
+      </c>
+      <c r="E137" s="3">
         <v>164</v>
       </c>
-      <c r="E137" s="3">
-        <v>364</v>
-      </c>
       <c r="I137" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="138" spans="1:14">
       <c r="A138" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B138" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C138" s="1">
-        <v>242</v>
+        <v>306</v>
+      </c>
+      <c r="D138" s="1">
+        <v>164</v>
       </c>
       <c r="E138" s="3">
-        <v>256</v>
-      </c>
-      <c r="G138" s="1">
-        <v>250</v>
+        <v>364</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="139" spans="1:14">
       <c r="A139" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B139" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C139" s="1">
-        <v>296</v>
-      </c>
-      <c r="D139" s="1">
-        <v>438</v>
+        <v>242</v>
       </c>
       <c r="E139" s="3">
-        <v>512</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>147</v>
+        <v>256</v>
+      </c>
+      <c r="G139" s="1">
+        <v>250</v>
+      </c>
+      <c r="I139" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="140" spans="1:14">
       <c r="A140" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B140" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C140" s="1">
-        <v>442</v>
+        <v>296</v>
+      </c>
+      <c r="D140" s="1">
+        <v>438</v>
       </c>
       <c r="E140" s="3">
         <v>512</v>
       </c>
-      <c r="I140" s="1" t="s">
-        <v>117</v>
+      <c r="G140" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="141" spans="1:14">
       <c r="A141" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B141" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C141" s="1">
-        <v>792</v>
+        <v>442</v>
       </c>
       <c r="E141" s="3">
-        <v>812</v>
+        <v>512</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="142" spans="1:14">
       <c r="A142" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B142" s="1">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C142" s="1">
-        <v>92</v>
+        <v>792</v>
       </c>
       <c r="E142" s="3">
-        <v>1024</v>
+        <v>812</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N142" s="1" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="143" spans="1:14">
       <c r="A143" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B143" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C143" s="1">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E143" s="3">
         <v>1024</v>
@@ -2335,28 +2324,48 @@
         <v>113</v>
       </c>
       <c r="N143" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="144" spans="1:14">
       <c r="A144" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B144" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C144" s="1">
-        <v>156</v>
+        <v>88</v>
       </c>
       <c r="E144" s="3">
-        <v>150</v>
+        <v>1024</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="150" spans="2:2">
-      <c r="B150" s="1" t="s">
+      <c r="N144" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9">
+      <c r="A145" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B145" s="1">
+        <v>2</v>
+      </c>
+      <c r="C145" s="1">
+        <v>156</v>
+      </c>
+      <c r="E145" s="3">
+        <v>150</v>
+      </c>
+      <c r="I145" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9">
+      <c r="B151" s="1" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2 more bugs added to wish list grr
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="168">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -513,31 +513,13 @@
     <t>Dave/Corwin</t>
   </si>
   <si>
-    <t>Fix every spot in the game that uses fonts</t>
-  </si>
-  <si>
-    <t>in-game UI</t>
-  </si>
-  <si>
-    <t>Help Screen</t>
-  </si>
-  <si>
-    <t>Start New Game</t>
-  </si>
-  <si>
-    <t>Select Profile State</t>
-  </si>
-  <si>
-    <t>Delete Profile State</t>
-  </si>
-  <si>
-    <t>Click ok state</t>
-  </si>
-  <si>
-    <t>create profile state</t>
-  </si>
-  <si>
-    <t>engame text</t>
+    <t>replay level breaks the instruction list highlighting for current level</t>
+  </si>
+  <si>
+    <t>total score needs to be calculated on the fly based off of all your level scores</t>
+  </si>
+  <si>
+    <t>replaying a level over and over keeps increasing total score</t>
   </si>
 </sst>
 </file>
@@ -620,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -633,7 +615,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P171"/>
+  <dimension ref="A1:P162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2025,494 +2006,419 @@
       </c>
     </row>
     <row r="110" spans="1:4" s="11" customFormat="1">
-      <c r="A110" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B110" s="12">
-        <v>39912</v>
-      </c>
       <c r="C110" s="11" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="111" spans="1:4" s="11" customFormat="1">
-      <c r="C111" s="11" t="s">
+      <c r="D111" s="11" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="112" spans="1:4" s="11" customFormat="1">
-      <c r="A112" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B112" s="12">
-        <v>39912</v>
-      </c>
-      <c r="C112" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" s="11" customFormat="1">
-      <c r="A113" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B113" s="12">
-        <v>39912</v>
-      </c>
-      <c r="C113" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" s="11" customFormat="1">
-      <c r="A114" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B114" s="12">
-        <v>39912</v>
-      </c>
-      <c r="C114" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" s="11" customFormat="1">
-      <c r="A115" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B115" s="12">
-        <v>39912</v>
-      </c>
-      <c r="C115" s="11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" s="11" customFormat="1">
-      <c r="A116" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B116" s="12">
-        <v>39912</v>
-      </c>
-      <c r="C116" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" s="11" customFormat="1">
-      <c r="A117" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B117" s="12">
-        <v>39912</v>
-      </c>
-      <c r="C117" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" s="11" customFormat="1"/>
-    <row r="119" spans="1:3" s="11" customFormat="1"/>
-    <row r="120" spans="1:3" s="11" customFormat="1"/>
-    <row r="121" spans="1:3" s="11" customFormat="1"/>
-    <row r="122" spans="1:3" s="11" customFormat="1"/>
-    <row r="123" spans="1:3" s="11" customFormat="1"/>
-    <row r="124" spans="1:3" s="11" customFormat="1"/>
-    <row r="125" spans="1:3" s="11" customFormat="1"/>
-    <row r="129" spans="1:4">
-      <c r="C129" s="5" t="s">
+    <row r="112" spans="1:4" s="11" customFormat="1"/>
+    <row r="113" spans="1:3" s="11" customFormat="1"/>
+    <row r="114" spans="1:3" s="11" customFormat="1"/>
+    <row r="115" spans="1:3" s="11" customFormat="1"/>
+    <row r="116" spans="1:3" s="11" customFormat="1"/>
+    <row r="120" spans="1:3">
+      <c r="C120" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
-      <c r="C130" s="1" t="s">
+    <row r="121" spans="1:3">
+      <c r="C121" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
-      <c r="C131" s="1" t="s">
+    <row r="122" spans="1:3">
+      <c r="C122" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="123" spans="1:3">
+      <c r="C123" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="C124" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="C125" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="C127" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" s="3" customFormat="1">
+      <c r="A128" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B128" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" s="3" customFormat="1">
+      <c r="A129" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B129" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" s="3" customFormat="1">
+      <c r="A130" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B130" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" s="3" customFormat="1">
+      <c r="A131" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B131" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
       <c r="C132" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4">
-      <c r="C133" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="D133" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
       <c r="C134" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4">
-      <c r="C136" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" s="3" customFormat="1">
-      <c r="A137" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B137" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" s="3" customFormat="1">
-      <c r="A138" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B138" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" s="3" customFormat="1">
-      <c r="A139" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B139" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" s="3" customFormat="1">
-      <c r="A140" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B140" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
-      <c r="C141" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
-      <c r="D142" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4">
-      <c r="C143" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
-      <c r="C144" s="1" t="s">
+    <row r="135" spans="1:9">
+      <c r="C135" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="145" spans="1:12">
-      <c r="C145" s="1" t="s">
+    <row r="136" spans="1:9">
+      <c r="C136" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="149" spans="1:12">
-      <c r="C149" s="1" t="s">
+    <row r="140" spans="1:9">
+      <c r="C140" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D149" s="1" t="s">
+      <c r="D140" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E149" s="1" t="s">
+      <c r="E140" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G149" s="1" t="s">
+      <c r="G140" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="151" spans="1:12">
+    <row r="142" spans="1:9">
+      <c r="A142" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B142" s="1">
+        <v>1</v>
+      </c>
+      <c r="C142" s="1">
+        <v>56</v>
+      </c>
+      <c r="E142" s="3">
+        <v>64</v>
+      </c>
+      <c r="I142" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
+      <c r="A143" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B143" s="1">
+        <v>6</v>
+      </c>
+      <c r="C143" s="1">
+        <v>78</v>
+      </c>
+      <c r="E143" s="3">
+        <v>90</v>
+      </c>
+      <c r="I143" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
+      <c r="A144" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B144" s="1">
+        <v>7</v>
+      </c>
+      <c r="C144" s="1">
+        <v>64</v>
+      </c>
+      <c r="E144" s="3">
+        <v>82</v>
+      </c>
+      <c r="I144" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14">
+      <c r="A145" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B145" s="1">
+        <v>3</v>
+      </c>
+      <c r="C145" s="1">
+        <v>110</v>
+      </c>
+      <c r="E145" s="3">
+        <v>128</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I145" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14">
+      <c r="A146" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B146" s="1">
+        <v>11</v>
+      </c>
+      <c r="C146" s="1">
+        <v>128</v>
+      </c>
+      <c r="E146" s="3">
+        <v>140</v>
+      </c>
+      <c r="I146" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14">
+      <c r="A147" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B147" s="1">
+        <v>10</v>
+      </c>
+      <c r="C147" s="1">
+        <v>154</v>
+      </c>
+      <c r="E147" s="3">
+        <v>164</v>
+      </c>
+      <c r="I147" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14">
+      <c r="A148" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B148" s="1">
+        <v>8</v>
+      </c>
+      <c r="C148" s="1">
+        <v>156</v>
+      </c>
+      <c r="E148" s="3">
+        <v>164</v>
+      </c>
+      <c r="I148" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K148" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L148" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14">
+      <c r="A149" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B149" s="1">
+        <v>9</v>
+      </c>
+      <c r="C149" s="1">
+        <v>306</v>
+      </c>
+      <c r="D149" s="1">
+        <v>164</v>
+      </c>
+      <c r="E149" s="3">
+        <v>364</v>
+      </c>
+      <c r="I149" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14">
+      <c r="A150" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B150" s="1">
+        <v>12</v>
+      </c>
+      <c r="C150" s="1">
+        <v>242</v>
+      </c>
+      <c r="E150" s="3">
+        <v>256</v>
+      </c>
+      <c r="G150" s="1">
+        <v>250</v>
+      </c>
+      <c r="I150" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14">
       <c r="A151" s="1" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B151" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C151" s="1">
-        <v>56</v>
+        <v>296</v>
+      </c>
+      <c r="D151" s="1">
+        <v>438</v>
       </c>
       <c r="E151" s="3">
-        <v>64</v>
-      </c>
-      <c r="I151" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="152" spans="1:12">
+        <v>512</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14">
       <c r="A152" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="B152" s="1">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C152" s="1">
-        <v>78</v>
+        <v>442</v>
       </c>
       <c r="E152" s="3">
-        <v>90</v>
+        <v>512</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="153" spans="1:12">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14">
       <c r="A153" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B153" s="1">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C153" s="1">
-        <v>64</v>
+        <v>792</v>
       </c>
       <c r="E153" s="3">
-        <v>82</v>
+        <v>812</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="154" spans="1:12">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14">
       <c r="A154" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B154" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C154" s="1">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="E154" s="3">
-        <v>128</v>
-      </c>
-      <c r="G154" s="1" t="s">
-        <v>96</v>
+        <v>1024</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="155" spans="1:12">
+        <v>113</v>
+      </c>
+      <c r="N154" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14">
       <c r="A155" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B155" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C155" s="1">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="E155" s="3">
-        <v>140</v>
+        <v>1024</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="156" spans="1:12">
+        <v>113</v>
+      </c>
+      <c r="N155" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14">
       <c r="A156" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B156" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C156" s="1">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E156" s="3">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="157" spans="1:12">
-      <c r="A157" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B157" s="1">
-        <v>8</v>
-      </c>
-      <c r="C157" s="1">
-        <v>156</v>
-      </c>
-      <c r="E157" s="3">
-        <v>164</v>
-      </c>
-      <c r="I157" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K157" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="L157" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="158" spans="1:12">
-      <c r="A158" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B158" s="1">
-        <v>9</v>
-      </c>
-      <c r="C158" s="1">
-        <v>306</v>
-      </c>
-      <c r="D158" s="1">
-        <v>164</v>
-      </c>
-      <c r="E158" s="3">
-        <v>364</v>
-      </c>
-      <c r="I158" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="159" spans="1:12">
-      <c r="A159" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B159" s="1">
-        <v>12</v>
-      </c>
-      <c r="C159" s="1">
-        <v>242</v>
-      </c>
-      <c r="E159" s="3">
-        <v>256</v>
-      </c>
-      <c r="G159" s="1">
-        <v>250</v>
-      </c>
-      <c r="I159" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="160" spans="1:12">
-      <c r="A160" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B160" s="1">
-        <v>13</v>
-      </c>
-      <c r="C160" s="1">
-        <v>296</v>
-      </c>
-      <c r="D160" s="1">
-        <v>438</v>
-      </c>
-      <c r="E160" s="3">
-        <v>512</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="161" spans="1:14">
-      <c r="A161" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B161" s="1">
-        <v>15</v>
-      </c>
-      <c r="C161" s="1">
-        <v>442</v>
-      </c>
-      <c r="E161" s="3">
-        <v>512</v>
-      </c>
-      <c r="I161" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="162" spans="1:14">
-      <c r="A162" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B162" s="1">
-        <v>14</v>
-      </c>
-      <c r="C162" s="1">
-        <v>792</v>
-      </c>
-      <c r="E162" s="3">
-        <v>812</v>
-      </c>
-      <c r="I162" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="163" spans="1:14">
-      <c r="A163" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B163" s="1">
-        <v>5</v>
-      </c>
-      <c r="C163" s="1">
-        <v>92</v>
-      </c>
-      <c r="E163" s="3">
-        <v>1024</v>
-      </c>
-      <c r="I163" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N163" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="164" spans="1:14">
-      <c r="A164" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B164" s="1">
-        <v>4</v>
-      </c>
-      <c r="C164" s="1">
-        <v>88</v>
-      </c>
-      <c r="E164" s="3">
-        <v>1024</v>
-      </c>
-      <c r="I164" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N164" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="165" spans="1:14">
-      <c r="A165" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B165" s="1">
-        <v>2</v>
-      </c>
-      <c r="C165" s="1">
-        <v>156</v>
-      </c>
-      <c r="E165" s="3">
-        <v>150</v>
-      </c>
-      <c r="I165" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="171" spans="1:14">
-      <c r="B171" s="1" t="s">
+    </row>
+    <row r="162" spans="2:2">
+      <c r="B162" s="1" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
levels added and removed, reposisitioned, and new level mini arts
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -609,10 +609,10 @@
     <t>switch map files to use the enum names instead of ints</t>
   </si>
   <si>
-    <t>click ok state</t>
-  </si>
-  <si>
     <t>maybe - change help interface png</t>
+  </si>
+  <si>
+    <t>update new map pngs</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1019,7 @@
   <dimension ref="A1:P198"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1199,7 +1199,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="3" customFormat="1">
+    <row r="17" spans="1:3" s="3" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="3" customFormat="1">
+    <row r="18" spans="1:3" s="3" customFormat="1">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="3" customFormat="1">
+    <row r="19" spans="1:3" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="3" customFormat="1">
+    <row r="20" spans="1:3" s="3" customFormat="1">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="3" customFormat="1">
+    <row r="21" spans="1:3" s="3" customFormat="1">
       <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="3" customFormat="1">
+    <row r="22" spans="1:3" s="3" customFormat="1">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -1265,57 +1265,60 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="11" customFormat="1">
-      <c r="A23" s="11" t="s">
+    <row r="23" spans="1:3" s="3" customFormat="1">
+      <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="B23" s="4">
+        <v>39913</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="11" customFormat="1">
-      <c r="D24" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="11" customFormat="1">
+    <row r="24" spans="1:3" s="11" customFormat="1">
+      <c r="A24" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="11" customFormat="1">
       <c r="A25" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="11" customFormat="1">
-      <c r="A26" s="11" t="s">
-        <v>6</v>
-      </c>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="11" customFormat="1">
       <c r="C26" s="11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="11" customFormat="1">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="11" customFormat="1">
       <c r="C27" s="11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="11" customFormat="1">
+    <row r="28" spans="1:3" s="11" customFormat="1">
       <c r="C28" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="11" customFormat="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="11" customFormat="1">
       <c r="C29" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="11" customFormat="1"/>
-    <row r="31" spans="1:4" s="13" customFormat="1">
+    <row r="30" spans="1:3" s="11" customFormat="1"/>
+    <row r="31" spans="1:3" s="13" customFormat="1">
       <c r="C31" s="13" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="13" customFormat="1">
+    <row r="32" spans="1:3" s="13" customFormat="1">
       <c r="C32" s="13" t="s">
         <v>190</v>
       </c>

</xml_diff>

<commit_message>
interface help update save file for release tom has 1 bug to fix DO NOT TOUCH ANYTHING IN THE WISH LIST UNTIL YOU ARE DONE WITH YOUR KGA'S
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="195">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -327,12 +327,6 @@
     <t>level select should show the score for the current level</t>
   </si>
   <si>
-    <t>used left switch</t>
-  </si>
-  <si>
-    <t>fixed bad switch</t>
-  </si>
-  <si>
     <t>very easy, should be an earlier level</t>
   </si>
   <si>
@@ -357,9 +351,6 @@
     <t>reprogram</t>
   </si>
   <si>
-    <t>annoying as hell</t>
-  </si>
-  <si>
     <t>easy - very straightforward</t>
   </si>
   <si>
@@ -369,24 +360,12 @@
     <t>very linear, interesting figuring out what does what</t>
   </si>
   <si>
-    <t>can't be beaten</t>
-  </si>
-  <si>
     <t>short and sweet</t>
   </si>
   <si>
-    <t>c2</t>
-  </si>
-  <si>
     <t>c3</t>
   </si>
   <si>
-    <t>c4</t>
-  </si>
-  <si>
-    <t>c5</t>
-  </si>
-  <si>
     <t>c1</t>
   </si>
   <si>
@@ -613,6 +592,15 @@
   </si>
   <si>
     <t>update new map pngs</t>
+  </si>
+  <si>
+    <t>switch crouching/climbing/jumping - make it a dropoff</t>
+  </si>
+  <si>
+    <t>tutorials - add a button for skipping level</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH THESE UNTIL ALL YOUR KGA'S ARE DONE, DOESN'T MATTER WHICH CLASS, DO THEM FIRST</t>
   </si>
 </sst>
 </file>
@@ -707,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -722,6 +710,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P198"/>
+  <dimension ref="A1:P200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1031,7 +1020,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1">
       <c r="C1" s="5" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1">
@@ -1042,7 +1031,7 @@
         <v>39913</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="3" customFormat="1">
@@ -1053,7 +1042,7 @@
         <v>39913</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1">
@@ -1064,7 +1053,7 @@
         <v>39913</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1">
@@ -1075,7 +1064,7 @@
         <v>39913</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="3" customFormat="1">
@@ -1086,7 +1075,7 @@
         <v>39913</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="3" customFormat="1">
@@ -1097,7 +1086,7 @@
         <v>39913</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="3" customFormat="1">
@@ -1108,7 +1097,7 @@
         <v>39913</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="3" customFormat="1">
@@ -1119,7 +1108,7 @@
         <v>39913</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="3" customFormat="1">
@@ -1130,7 +1119,7 @@
         <v>39913</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="3" customFormat="1">
@@ -1141,7 +1130,7 @@
         <v>39913</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="3" customFormat="1">
@@ -1152,7 +1141,7 @@
         <v>39913</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="3" customFormat="1">
@@ -1163,7 +1152,7 @@
         <v>39913</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="3" customFormat="1">
@@ -1174,7 +1163,7 @@
         <v>39913</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="3" customFormat="1">
@@ -1185,7 +1174,7 @@
         <v>39913</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="3" customFormat="1">
@@ -1196,7 +1185,7 @@
         <v>39913</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="3" customFormat="1">
@@ -1207,7 +1196,7 @@
         <v>39913</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="3" customFormat="1">
@@ -1218,7 +1207,7 @@
         <v>39913</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="3" customFormat="1">
@@ -1229,7 +1218,7 @@
         <v>39913</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="3" customFormat="1">
@@ -1240,7 +1229,7 @@
         <v>39913</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="3" customFormat="1">
@@ -1251,7 +1240,7 @@
         <v>39913</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="3" customFormat="1">
@@ -1262,7 +1251,7 @@
         <v>39913</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="3" customFormat="1">
@@ -1273,120 +1262,139 @@
         <v>39913</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="11" customFormat="1">
-      <c r="A24" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="3" customFormat="1">
+      <c r="A24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="4">
+        <v>39913</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="3" customFormat="1">
+      <c r="A25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" s="11" customFormat="1">
-      <c r="A25" s="11" t="s">
+      <c r="B25" s="4">
+        <v>39913</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="3" customFormat="1">
+      <c r="A26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="4">
+        <v>39913</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="3" customFormat="1">
+      <c r="A27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="11" customFormat="1">
-      <c r="C26" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="11" customFormat="1">
-      <c r="C27" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="11" customFormat="1">
-      <c r="C28" s="11" t="s">
-        <v>197</v>
+      <c r="B27" s="4">
+        <v>39913</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="3" customFormat="1">
+      <c r="A28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="4">
+        <v>39913</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="11" customFormat="1">
+      <c r="A29" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="C29" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="11" customFormat="1"/>
-    <row r="31" spans="1:3" s="13" customFormat="1">
-      <c r="C31" s="13" t="s">
-        <v>184</v>
+    <row r="31" spans="1:3" s="14" customFormat="1">
+      <c r="A31" s="14" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="13" customFormat="1">
       <c r="C32" s="13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="11" customFormat="1"/>
-    <row r="34" spans="1:3" s="11" customFormat="1"/>
-    <row r="35" spans="1:3" s="12" customFormat="1"/>
-    <row r="36" spans="1:3" s="5" customFormat="1">
-      <c r="B36" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="13" customFormat="1">
+      <c r="C33" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="13" customFormat="1">
+      <c r="C34" s="13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="13" customFormat="1">
+      <c r="C35" s="13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="11" customFormat="1"/>
+    <row r="37" spans="1:3" s="12" customFormat="1"/>
+    <row r="38" spans="1:3" s="5" customFormat="1">
+      <c r="B38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="3" customFormat="1">
-      <c r="A37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="3" customFormat="1">
-      <c r="A38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="3" customFormat="1">
       <c r="A39" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B39" s="4">
         <v>39881</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="3" customFormat="1">
       <c r="A40" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B40" s="4">
         <v>39881</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="3" customFormat="1">
       <c r="A41" s="3" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="B41" s="4">
         <v>39881</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="3" customFormat="1">
@@ -1397,29 +1405,29 @@
         <v>39881</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="3" customFormat="1">
       <c r="A43" s="3" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B43" s="4">
-        <v>39883</v>
+        <v>39881</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="3" customFormat="1">
       <c r="A44" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B44" s="4">
-        <v>39883</v>
+        <v>39881</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="3" customFormat="1">
@@ -1430,21 +1438,21 @@
         <v>39883</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="3" customFormat="1">
       <c r="A46" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B46" s="4">
         <v>39883</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" s="3" customFormat="1" ht="16.5" customHeight="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="3" customFormat="1">
       <c r="A47" s="3" t="s">
         <v>9</v>
       </c>
@@ -1452,21 +1460,21 @@
         <v>39883</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="3" customFormat="1">
       <c r="A48" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B48" s="4">
         <v>39883</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="3" customFormat="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="3" customFormat="1" ht="16.5" customHeight="1">
       <c r="A49" s="3" t="s">
         <v>9</v>
       </c>
@@ -1474,7 +1482,7 @@
         <v>39883</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="3" customFormat="1">
@@ -1485,7 +1493,7 @@
         <v>39883</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="3" customFormat="1">
@@ -1496,7 +1504,7 @@
         <v>39883</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="3" customFormat="1">
@@ -1507,7 +1515,7 @@
         <v>39883</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="3" customFormat="1">
@@ -1515,10 +1523,10 @@
         <v>9</v>
       </c>
       <c r="B53" s="4">
-        <v>39888</v>
+        <v>39883</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="3" customFormat="1">
@@ -1526,10 +1534,10 @@
         <v>9</v>
       </c>
       <c r="B54" s="4">
-        <v>39888</v>
+        <v>39883</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="3" customFormat="1">
@@ -1540,7 +1548,7 @@
         <v>39888</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="3" customFormat="1">
@@ -1551,7 +1559,7 @@
         <v>39888</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="3" customFormat="1">
@@ -1559,76 +1567,76 @@
         <v>9</v>
       </c>
       <c r="B57" s="4">
-        <v>39889</v>
+        <v>39888</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="3" customFormat="1">
       <c r="A58" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B58" s="4">
-        <v>39892</v>
+        <v>39888</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="3" customFormat="1">
       <c r="A59" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B59" s="4">
-        <v>39901</v>
+        <v>39889</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="3" customFormat="1">
       <c r="A60" s="3" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="B60" s="4">
-        <v>39901</v>
+        <v>39892</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="3" customFormat="1">
       <c r="A61" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B61" s="4">
         <v>39901</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="3" customFormat="1">
       <c r="A62" s="3" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="B62" s="4">
         <v>39901</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="3" customFormat="1">
       <c r="A63" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B63" s="4">
         <v>39901</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="3" customFormat="1">
@@ -1639,40 +1647,40 @@
         <v>39901</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="3" customFormat="1">
       <c r="A65" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B65" s="4">
-        <v>39902</v>
+        <v>39901</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="3" customFormat="1">
       <c r="A66" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B66" s="4">
-        <v>39902</v>
+        <v>39901</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="3" customFormat="1">
       <c r="A67" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B67" s="4">
         <v>39902</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="3" customFormat="1">
@@ -1683,18 +1691,18 @@
         <v>39902</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="3" customFormat="1">
       <c r="A69" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B69" s="4">
-        <v>39904</v>
+        <v>39902</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="3" customFormat="1">
@@ -1702,54 +1710,54 @@
         <v>13</v>
       </c>
       <c r="B70" s="4">
-        <v>39904</v>
+        <v>39902</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:3" s="3" customFormat="1">
       <c r="A71" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B71" s="4">
-        <v>39905</v>
+        <v>39904</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="3" customFormat="1">
       <c r="A72" s="3" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B72" s="4">
-        <v>39907</v>
+        <v>39904</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="3" customFormat="1">
       <c r="A73" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B73" s="4">
-        <v>39907</v>
+        <v>39905</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:3" s="3" customFormat="1">
       <c r="A74" s="3" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B74" s="4">
         <v>39907</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
     </row>
     <row r="75" spans="1:3" s="3" customFormat="1">
@@ -1760,10 +1768,10 @@
         <v>39907</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" s="3" customFormat="1" ht="15.75" customHeight="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" s="3" customFormat="1">
       <c r="A76" s="3" t="s">
         <v>9</v>
       </c>
@@ -1771,7 +1779,7 @@
         <v>39907</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="3" customFormat="1">
@@ -1779,43 +1787,43 @@
         <v>9</v>
       </c>
       <c r="B77" s="4">
-        <v>39908</v>
+        <v>39907</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" s="3" customFormat="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" s="3" customFormat="1" ht="15.75" customHeight="1">
       <c r="A78" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B78" s="4">
-        <v>39908</v>
+        <v>39907</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="3" customFormat="1">
       <c r="A79" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B79" s="4">
         <v>39908</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="3" customFormat="1">
       <c r="A80" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B80" s="4">
         <v>39908</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="3" customFormat="1">
@@ -1826,7 +1834,7 @@
         <v>39908</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="1:3" s="3" customFormat="1">
@@ -1837,7 +1845,7 @@
         <v>39908</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="3" customFormat="1">
@@ -1848,18 +1856,18 @@
         <v>39908</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="84" spans="1:3" s="3" customFormat="1">
       <c r="A84" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B84" s="4">
-        <v>39910</v>
+        <v>39908</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:3" s="3" customFormat="1">
@@ -1867,32 +1875,32 @@
         <v>13</v>
       </c>
       <c r="B85" s="4">
-        <v>39910</v>
+        <v>39908</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" spans="1:3" s="3" customFormat="1">
       <c r="A86" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B86" s="4">
         <v>39910</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="3" customFormat="1">
       <c r="A87" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B87" s="4">
         <v>39910</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="88" spans="1:3" s="3" customFormat="1">
@@ -1903,7 +1911,7 @@
         <v>39910</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:3" s="3" customFormat="1">
@@ -1914,101 +1922,101 @@
         <v>39910</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="90" spans="1:3" s="3" customFormat="1">
       <c r="A90" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B90" s="4">
         <v>39910</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" s="2" customFormat="1">
-      <c r="B91" s="8"/>
-      <c r="C91" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" s="2" customFormat="1">
-      <c r="B92" s="8"/>
-    </row>
-    <row r="93" spans="1:3" s="6" customFormat="1">
-      <c r="B93" s="7"/>
-    </row>
-    <row r="94" spans="1:3" s="5" customFormat="1">
-      <c r="C94" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" s="3" customFormat="1">
+      <c r="A91" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91" s="4">
+        <v>39910</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" s="3" customFormat="1">
+      <c r="A92" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B92" s="4">
+        <v>39910</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" s="2" customFormat="1">
+      <c r="B93" s="8"/>
+      <c r="C93" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" s="2" customFormat="1">
+      <c r="B94" s="8"/>
+    </row>
+    <row r="95" spans="1:3" s="6" customFormat="1">
+      <c r="B95" s="7"/>
+    </row>
+    <row r="96" spans="1:3" s="5" customFormat="1">
+      <c r="C96" s="5" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" s="3" customFormat="1">
-      <c r="A95" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B95" s="4">
-        <v>39901</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" s="3" customFormat="1">
-      <c r="A96" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B96" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="3" customFormat="1">
       <c r="A97" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B97" s="4">
-        <v>39904</v>
+        <v>39901</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98" spans="1:4" s="3" customFormat="1">
       <c r="A98" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B98" s="4">
-        <v>39904</v>
+        <v>39902</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="3" customFormat="1">
       <c r="A99" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B99" s="4">
-        <v>39906</v>
+        <v>39904</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100" spans="1:4" s="3" customFormat="1">
       <c r="A100" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B100" s="4">
-        <v>39908</v>
+        <v>39904</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>137</v>
+        <v>22</v>
       </c>
     </row>
     <row r="101" spans="1:4" s="3" customFormat="1">
@@ -2016,10 +2024,10 @@
         <v>9</v>
       </c>
       <c r="B101" s="4">
-        <v>39908</v>
+        <v>39906</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>142</v>
+        <v>63</v>
       </c>
     </row>
     <row r="102" spans="1:4" s="3" customFormat="1">
@@ -2027,145 +2035,145 @@
         <v>9</v>
       </c>
       <c r="B102" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" s="3" customFormat="1">
+      <c r="A103" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B103" s="4">
+        <v>39908</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" s="3" customFormat="1">
+      <c r="A104" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B104" s="4">
         <v>39909</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" s="9" customFormat="1">
-      <c r="A103" s="9" t="s">
+      <c r="C104" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" s="9" customFormat="1">
+      <c r="A105" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C103" s="9" t="s">
+      <c r="C105" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:4" s="9" customFormat="1">
-      <c r="C104" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" s="9" customFormat="1">
-      <c r="C105" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="106" spans="1:4" s="9" customFormat="1">
-      <c r="A106" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="C106" s="9" t="s">
-        <v>5</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" spans="1:4" s="9" customFormat="1">
       <c r="C107" s="9" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:4" s="9" customFormat="1">
       <c r="A108" s="9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:4" s="9" customFormat="1">
       <c r="C109" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" s="9" customFormat="1">
+      <c r="A110" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" s="9" customFormat="1">
+      <c r="C111" s="9" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" s="9" customFormat="1">
-      <c r="D110" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" s="9" customFormat="1">
-      <c r="D111" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="112" spans="1:4" s="9" customFormat="1">
       <c r="D112" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" s="9" customFormat="1">
+      <c r="D113" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" s="9" customFormat="1">
+      <c r="D114" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:16" s="9" customFormat="1">
-      <c r="A113" s="9" t="s">
+    <row r="115" spans="1:16" s="9" customFormat="1">
+      <c r="A115" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C113" s="9" t="s">
+      <c r="C115" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="114" spans="1:16" s="9" customFormat="1">
-      <c r="B114" s="10"/>
-      <c r="C114" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="115" spans="1:16" s="9" customFormat="1">
-      <c r="B115" s="10"/>
-      <c r="C115" s="9" t="s">
-        <v>193</v>
-      </c>
-    </row>
     <row r="116" spans="1:16" s="9" customFormat="1">
+      <c r="B116" s="10"/>
       <c r="C116" s="9" t="s">
-        <v>176</v>
+        <v>134</v>
       </c>
     </row>
     <row r="117" spans="1:16" s="9" customFormat="1">
+      <c r="B117" s="10"/>
       <c r="C117" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="118" spans="1:16" s="9" customFormat="1"/>
-    <row r="119" spans="1:16">
-      <c r="A119" s="2"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="2"/>
-      <c r="F119" s="2"/>
-      <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
-      <c r="I119" s="2"/>
-      <c r="J119" s="2"/>
-      <c r="K119" s="2"/>
-      <c r="L119" s="2"/>
-      <c r="M119" s="2"/>
-      <c r="N119" s="2"/>
-      <c r="O119" s="2"/>
-      <c r="P119" s="2"/>
-    </row>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" s="9" customFormat="1">
+      <c r="C118" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" s="9" customFormat="1">
+      <c r="C119" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" s="9" customFormat="1"/>
     <row r="121" spans="1:16">
-      <c r="C121" s="5" t="s">
+      <c r="A121" s="2"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+      <c r="J121" s="2"/>
+      <c r="K121" s="2"/>
+      <c r="L121" s="2"/>
+      <c r="M121" s="2"/>
+      <c r="N121" s="2"/>
+      <c r="O121" s="2"/>
+      <c r="P121" s="2"/>
+    </row>
+    <row r="123" spans="1:16">
+      <c r="C123" s="5" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="122" spans="1:16" s="3" customFormat="1">
-      <c r="A122" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B122" s="4">
-        <v>39881</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="123" spans="1:16" s="3" customFormat="1">
-      <c r="A123" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B123" s="4">
-        <v>39882</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="124" spans="1:16" s="3" customFormat="1">
@@ -2173,21 +2181,21 @@
         <v>9</v>
       </c>
       <c r="B124" s="4">
-        <v>39887</v>
+        <v>39881</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="125" spans="1:16" s="3" customFormat="1">
       <c r="A125" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B125" s="4">
-        <v>39887</v>
+        <v>39882</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="126" spans="1:16" s="3" customFormat="1">
@@ -2198,7 +2206,7 @@
         <v>39887</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="127" spans="1:16" s="3" customFormat="1">
@@ -2209,7 +2217,7 @@
         <v>39887</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="128" spans="1:16" s="3" customFormat="1">
@@ -2220,7 +2228,7 @@
         <v>39887</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="129" spans="1:7" s="3" customFormat="1">
@@ -2228,21 +2236,21 @@
         <v>9</v>
       </c>
       <c r="B129" s="4">
-        <v>39888</v>
+        <v>39887</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
     </row>
     <row r="130" spans="1:7" s="3" customFormat="1">
       <c r="A130" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B130" s="4">
-        <v>39901</v>
+        <v>39887</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="131" spans="1:7" s="3" customFormat="1">
@@ -2250,24 +2258,21 @@
         <v>9</v>
       </c>
       <c r="B131" s="4">
-        <v>39902</v>
+        <v>39888</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
     </row>
     <row r="132" spans="1:7" s="3" customFormat="1">
       <c r="A132" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B132" s="4">
-        <v>39902</v>
+        <v>39901</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G132" s="3" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
     </row>
     <row r="133" spans="1:7" s="3" customFormat="1">
@@ -2278,7 +2283,7 @@
         <v>39902</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="134" spans="1:7" s="3" customFormat="1">
@@ -2286,10 +2291,13 @@
         <v>6</v>
       </c>
       <c r="B134" s="4">
-        <v>39905</v>
+        <v>39902</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="135" spans="1:7" s="3" customFormat="1">
@@ -2297,21 +2305,21 @@
         <v>9</v>
       </c>
       <c r="B135" s="4">
-        <v>39907</v>
+        <v>39902</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="136" spans="1:7" s="3" customFormat="1">
       <c r="A136" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B136" s="4">
-        <v>39907</v>
+        <v>39905</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="137" spans="1:7" s="3" customFormat="1">
@@ -2322,40 +2330,40 @@
         <v>39907</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="138" spans="1:7" s="3" customFormat="1">
       <c r="A138" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B138" s="4">
-        <v>39908</v>
+        <v>39907</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="139" spans="1:7" s="3" customFormat="1">
       <c r="A139" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B139" s="4">
-        <v>39909</v>
+        <v>39907</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="140" spans="1:7" s="3" customFormat="1">
       <c r="A140" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B140" s="4">
-        <v>39910</v>
+        <v>39908</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="141" spans="1:7" s="3" customFormat="1">
@@ -2363,10 +2371,10 @@
         <v>6</v>
       </c>
       <c r="B141" s="4">
-        <v>39910</v>
+        <v>39909</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>136</v>
+        <v>94</v>
       </c>
     </row>
     <row r="142" spans="1:7" s="3" customFormat="1">
@@ -2377,13 +2385,18 @@
         <v>39910</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
     </row>
     <row r="143" spans="1:7" s="3" customFormat="1">
-      <c r="B143" s="4"/>
-      <c r="D143" s="3" t="s">
-        <v>140</v>
+      <c r="A143" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B143" s="4">
+        <v>39910</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="144" spans="1:7" s="3" customFormat="1">
@@ -2394,99 +2407,94 @@
         <v>39910</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" s="3" customFormat="1">
-      <c r="A145" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B145" s="4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" s="3" customFormat="1">
+      <c r="B145" s="4"/>
+      <c r="D145" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" s="3" customFormat="1">
+      <c r="A146" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B146" s="4">
         <v>39910</v>
       </c>
-      <c r="C145" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" s="9" customFormat="1">
-      <c r="C146" s="9" t="s">
+      <c r="C146" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" s="3" customFormat="1">
+      <c r="A147" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B147" s="4">
+        <v>39910</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" s="9" customFormat="1">
+      <c r="C148" s="9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="147" spans="1:3" s="3" customFormat="1">
-      <c r="A147" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B147" s="4">
+    <row r="149" spans="1:4" s="3" customFormat="1">
+      <c r="A149" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B149" s="4">
         <v>39912</v>
       </c>
-      <c r="C147" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" s="11" customFormat="1"/>
-    <row r="149" spans="1:3" s="11" customFormat="1"/>
-    <row r="150" spans="1:3" s="11" customFormat="1"/>
-    <row r="151" spans="1:3" s="11" customFormat="1"/>
-    <row r="152" spans="1:3" s="11" customFormat="1"/>
-    <row r="156" spans="1:3">
-      <c r="C156" s="5" t="s">
+      <c r="C149" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" s="11" customFormat="1"/>
+    <row r="151" spans="1:4" s="11" customFormat="1"/>
+    <row r="152" spans="1:4" s="11" customFormat="1"/>
+    <row r="153" spans="1:4" s="11" customFormat="1"/>
+    <row r="154" spans="1:4" s="11" customFormat="1"/>
+    <row r="158" spans="1:4">
+      <c r="C158" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
-      <c r="C157" s="1" t="s">
+    <row r="159" spans="1:4">
+      <c r="C159" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
-      <c r="C158" s="1" t="s">
+    <row r="160" spans="1:4">
+      <c r="C160" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
-      <c r="C159" s="1" t="s">
+    <row r="161" spans="1:4">
+      <c r="C161" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
-      <c r="C160" s="1" t="s">
+    <row r="162" spans="1:4">
+      <c r="C162" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
-      <c r="C161" s="1" t="s">
+    <row r="163" spans="1:4">
+      <c r="C163" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
-      <c r="C163" s="5" t="s">
+    <row r="165" spans="1:4">
+      <c r="C165" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="164" spans="1:7" s="3" customFormat="1">
-      <c r="A164" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B164" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" s="3" customFormat="1">
-      <c r="A165" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B165" s="4">
-        <v>39902</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" s="3" customFormat="1">
+    <row r="166" spans="1:4" s="3" customFormat="1">
       <c r="A166" s="3" t="s">
         <v>9</v>
       </c>
@@ -2494,10 +2502,10 @@
         <v>39902</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" s="3" customFormat="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" s="3" customFormat="1">
       <c r="A167" s="3" t="s">
         <v>9</v>
       </c>
@@ -2505,330 +2513,307 @@
         <v>39902</v>
       </c>
       <c r="C167" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" s="3" customFormat="1">
+      <c r="A168" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B168" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" s="3" customFormat="1">
+      <c r="A169" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B169" s="4">
+        <v>39902</v>
+      </c>
+      <c r="C169" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="168" spans="1:7">
-      <c r="C168" s="1" t="s">
+    <row r="170" spans="1:4">
+      <c r="C170" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
-      <c r="D169" s="1" t="s">
+    <row r="171" spans="1:4">
+      <c r="D171" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="170" spans="1:7">
-      <c r="C170" s="1" t="s">
+    <row r="172" spans="1:4">
+      <c r="C172" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
-      <c r="C171" s="1" t="s">
+    <row r="173" spans="1:4">
+      <c r="C173" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
-      <c r="C172" s="1" t="s">
+    <row r="174" spans="1:4">
+      <c r="C174" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
-      <c r="C176" s="1" t="s">
+    <row r="178" spans="1:12">
+      <c r="C178" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G178" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D176" s="1" t="s">
+    </row>
+    <row r="180" spans="1:12">
+      <c r="A180" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B180" s="1">
+        <v>1</v>
+      </c>
+      <c r="C180" s="1">
+        <v>56</v>
+      </c>
+      <c r="E180" s="3">
+        <v>64</v>
+      </c>
+      <c r="I180" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12">
+      <c r="A181" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B181" s="1">
+        <v>6</v>
+      </c>
+      <c r="C181" s="1">
+        <v>78</v>
+      </c>
+      <c r="E181" s="3">
+        <v>90</v>
+      </c>
+      <c r="I181" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12">
+      <c r="A182" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B182" s="1">
+        <v>7</v>
+      </c>
+      <c r="C182" s="1">
+        <v>64</v>
+      </c>
+      <c r="E182" s="3">
+        <v>82</v>
+      </c>
+      <c r="I182" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12">
+      <c r="A183" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B183" s="1">
+        <v>3</v>
+      </c>
+      <c r="C183" s="1">
+        <v>110</v>
+      </c>
+      <c r="E183" s="3">
+        <v>128</v>
+      </c>
+      <c r="G183" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I183" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12">
+      <c r="A184" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B184" s="1">
+        <v>11</v>
+      </c>
+      <c r="C184" s="1">
+        <v>128</v>
+      </c>
+      <c r="E184" s="3">
+        <v>140</v>
+      </c>
+      <c r="I184" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12">
+      <c r="A185" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B185" s="1">
+        <v>10</v>
+      </c>
+      <c r="C185" s="1">
+        <v>154</v>
+      </c>
+      <c r="E185" s="3">
+        <v>164</v>
+      </c>
+      <c r="I185" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E176" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G176" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="178" spans="1:14">
-      <c r="A178" s="1" t="s">
+    </row>
+    <row r="186" spans="1:12">
+      <c r="A186" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B186" s="1">
+        <v>8</v>
+      </c>
+      <c r="C186" s="1">
+        <v>156</v>
+      </c>
+      <c r="E186" s="3">
+        <v>164</v>
+      </c>
+      <c r="I186" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K186" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L186" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12">
+      <c r="A187" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B187" s="1">
+        <v>9</v>
+      </c>
+      <c r="C187" s="1">
+        <v>306</v>
+      </c>
+      <c r="D187" s="1">
+        <v>164</v>
+      </c>
+      <c r="E187" s="3">
+        <v>364</v>
+      </c>
+      <c r="I187" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12">
+      <c r="A188" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B178" s="1">
-        <v>1</v>
-      </c>
-      <c r="C178" s="1">
-        <v>56</v>
-      </c>
-      <c r="E178" s="3">
-        <v>64</v>
-      </c>
-      <c r="I178" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="179" spans="1:14">
-      <c r="A179" s="1" t="s">
+      <c r="B188" s="1">
+        <v>12</v>
+      </c>
+      <c r="C188" s="1">
+        <v>242</v>
+      </c>
+      <c r="E188" s="3">
+        <v>256</v>
+      </c>
+      <c r="G188" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12">
+      <c r="A189" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B179" s="1">
-        <v>6</v>
-      </c>
-      <c r="C179" s="1">
-        <v>78</v>
-      </c>
-      <c r="E179" s="3">
-        <v>90</v>
-      </c>
-      <c r="I179" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="180" spans="1:14">
-      <c r="A180" s="1" t="s">
+      <c r="B189" s="1">
+        <v>13</v>
+      </c>
+      <c r="C189" s="1">
+        <v>296</v>
+      </c>
+      <c r="D189" s="1">
+        <v>438</v>
+      </c>
+      <c r="E189" s="3">
+        <v>512</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12">
+      <c r="A190" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B190" s="1">
+        <v>15</v>
+      </c>
+      <c r="C190" s="1">
+        <v>442</v>
+      </c>
+      <c r="E190" s="3">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12">
+      <c r="A191" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B180" s="1">
-        <v>7</v>
-      </c>
-      <c r="C180" s="1">
-        <v>64</v>
-      </c>
-      <c r="E180" s="3">
-        <v>82</v>
-      </c>
-      <c r="I180" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="181" spans="1:14">
-      <c r="A181" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B181" s="1">
-        <v>3</v>
-      </c>
-      <c r="C181" s="1">
-        <v>110</v>
-      </c>
-      <c r="E181" s="3">
-        <v>128</v>
-      </c>
-      <c r="G181" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I181" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="182" spans="1:14">
-      <c r="A182" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B182" s="1">
-        <v>11</v>
-      </c>
-      <c r="C182" s="1">
-        <v>128</v>
-      </c>
-      <c r="E182" s="3">
-        <v>140</v>
-      </c>
-      <c r="I182" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="183" spans="1:14">
-      <c r="A183" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B183" s="1">
-        <v>10</v>
-      </c>
-      <c r="C183" s="1">
-        <v>154</v>
-      </c>
-      <c r="E183" s="3">
-        <v>164</v>
-      </c>
-      <c r="I183" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="184" spans="1:14">
-      <c r="A184" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B184" s="1">
-        <v>8</v>
-      </c>
-      <c r="C184" s="1">
-        <v>156</v>
-      </c>
-      <c r="E184" s="3">
-        <v>164</v>
-      </c>
-      <c r="I184" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K184" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="L184" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="185" spans="1:14">
-      <c r="A185" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B185" s="1">
-        <v>9</v>
-      </c>
-      <c r="C185" s="1">
-        <v>306</v>
-      </c>
-      <c r="D185" s="1">
-        <v>164</v>
-      </c>
-      <c r="E185" s="3">
-        <v>364</v>
-      </c>
-      <c r="I185" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="186" spans="1:14">
-      <c r="A186" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B186" s="1">
-        <v>12</v>
-      </c>
-      <c r="C186" s="1">
-        <v>242</v>
-      </c>
-      <c r="E186" s="3">
-        <v>256</v>
-      </c>
-      <c r="G186" s="1">
-        <v>250</v>
-      </c>
-      <c r="I186" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="187" spans="1:14">
-      <c r="A187" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B187" s="1">
-        <v>13</v>
-      </c>
-      <c r="C187" s="1">
-        <v>296</v>
-      </c>
-      <c r="D187" s="1">
-        <v>438</v>
-      </c>
-      <c r="E187" s="3">
-        <v>512</v>
-      </c>
-      <c r="G187" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="188" spans="1:14">
-      <c r="A188" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B188" s="1">
-        <v>15</v>
-      </c>
-      <c r="C188" s="1">
-        <v>442</v>
-      </c>
-      <c r="E188" s="3">
-        <v>512</v>
-      </c>
-      <c r="I188" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="189" spans="1:14">
-      <c r="A189" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B189" s="1">
+      <c r="B191" s="1">
         <v>14</v>
       </c>
-      <c r="C189" s="1">
+      <c r="C191" s="1">
         <v>792</v>
       </c>
-      <c r="E189" s="3">
+      <c r="E191" s="3">
         <v>812</v>
-      </c>
-      <c r="I189" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="190" spans="1:14">
-      <c r="A190" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B190" s="1">
-        <v>5</v>
-      </c>
-      <c r="C190" s="1">
-        <v>92</v>
-      </c>
-      <c r="E190" s="3">
-        <v>1024</v>
-      </c>
-      <c r="I190" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N190" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="191" spans="1:14">
-      <c r="A191" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B191" s="1">
-        <v>4</v>
-      </c>
-      <c r="C191" s="1">
-        <v>88</v>
-      </c>
-      <c r="E191" s="3">
-        <v>1024</v>
       </c>
       <c r="I191" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N191" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="192" spans="1:14">
-      <c r="A192" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B192" s="1">
-        <v>2</v>
-      </c>
-      <c r="C192" s="1">
-        <v>156</v>
-      </c>
-      <c r="E192" s="3">
-        <v>150</v>
-      </c>
-      <c r="I192" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="198" spans="2:2">
-      <c r="B198" s="1" t="s">
-        <v>151</v>
+    </row>
+    <row r="192" spans="1:12">
+      <c r="B192" s="12"/>
+      <c r="C192" s="12"/>
+      <c r="D192" s="12"/>
+      <c r="E192" s="12"/>
+    </row>
+    <row r="193" spans="2:5">
+      <c r="B193" s="12"/>
+      <c r="C193" s="12"/>
+      <c r="D193" s="12"/>
+      <c r="E193" s="12"/>
+    </row>
+    <row r="194" spans="2:5">
+      <c r="B194" s="12"/>
+      <c r="C194" s="12"/>
+      <c r="D194" s="12"/>
+      <c r="E194" s="12"/>
+    </row>
+    <row r="200" spans="2:5">
+      <c r="B200" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added victory dance state to gameboard... fixed the bug with aborting during victory dance
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="197">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -604,6 +604,9 @@
   </si>
   <si>
     <t>BUG - if you click abort during victory dance, you get stuck</t>
+  </si>
+  <si>
+    <t>if you execute then abort, then try to insert just after the lit item, crash</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1014,7 @@
   <dimension ref="A1:P201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1339,7 +1342,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="11" customFormat="1"/>
+    <row r="31" spans="1:3" s="11" customFormat="1">
+      <c r="C31" s="11" t="s">
+        <v>196</v>
+      </c>
+    </row>
     <row r="32" spans="1:3" s="14" customFormat="1">
       <c r="A32" s="14" t="s">
         <v>194</v>

</xml_diff>

<commit_message>
added two new button arts, yes and no added do you want to play the tutorial popup pregame
</commit_message>
<xml_diff>
--- a/seeautz/Content/Wish List.xlsx
+++ b/seeautz/Content/Wish List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="197">
   <si>
     <t>THINGS NEEDED</t>
   </si>
@@ -1013,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1337,8 +1337,14 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="11" customFormat="1">
-      <c r="C30" s="11" t="s">
+    <row r="30" spans="1:3" s="3" customFormat="1">
+      <c r="A30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="4">
+        <v>39919</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>195</v>
       </c>
     </row>
@@ -1352,8 +1358,14 @@
         <v>194</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="13" customFormat="1">
-      <c r="C33" s="13" t="s">
+    <row r="33" spans="1:3" s="3" customFormat="1">
+      <c r="A33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="4">
+        <v>39919</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>177</v>
       </c>
     </row>

</xml_diff>